<commit_message>
feat: cedula da mudança de nome, adicionado ao codigo
</commit_message>
<xml_diff>
--- a/FICHA_FUNCIONAL_TEMPLATE.xlsx
+++ b/FICHA_FUNCIONAL_TEMPLATE.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="116">
   <si>
     <t xml:space="preserve">GOVERNO DO ESTADO DO AMAZONAS</t>
   </si>
@@ -48,7 +48,7 @@
     <t xml:space="preserve">C.G.C.</t>
   </si>
   <si>
-    <t xml:space="preserve">RETRATO                                      3x4</t>
+    <t xml:space="preserve">              RETRATO                3x4</t>
   </si>
   <si>
     <t xml:space="preserve">RUA 2, N 02, CONJUNTO CELETRAMAZON, BAIRRO ADRIANOPOLIS, 69057-350</t>
@@ -178,9 +178,6 @@
     <t xml:space="preserve">ÓRGÃO EXPEDIDOR</t>
   </si>
   <si>
-    <t xml:space="preserve">RUA EBANO ORIENTAL, 400 - ALVORADA - 69043-000</t>
-  </si>
-  <si>
     <t xml:space="preserve">ENDEREÇO</t>
   </si>
   <si>
@@ -283,7 +280,7 @@
     <t xml:space="preserve">RETRATAÇÃO</t>
   </si>
   <si>
-    <t xml:space="preserve">IMPRESSÃO                           DIGITAL</t>
+    <t xml:space="preserve">                     IMPRESSÃO                      DIGITAL</t>
   </si>
   <si>
     <t xml:space="preserve">CAMPO_DESLIGAMENTO</t>
@@ -616,336 +613,320 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="79">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="justify" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -972,9 +953,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>836280</xdr:colOff>
+      <xdr:colOff>835920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>124200</xdr:rowOff>
+      <xdr:rowOff>123840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -987,13 +968,12 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="894600" y="847440"/>
-          <a:ext cx="1188360" cy="1570320"/>
+          <a:off x="894240" y="847440"/>
+          <a:ext cx="1187640" cy="1569960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
         <a:ln w="0">
           <a:noFill/>
         </a:ln>
@@ -1117,13 +1097,13 @@
   </sheetPr>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AG22" activeCellId="0" sqref="AG22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AE50" activeCellId="0" sqref="AE50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="6.12"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="3.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="7.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="18.41"/>
@@ -1132,7 +1112,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="10.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="8" style="1" width="1.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="5.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="16.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="1.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="14.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="1.7"/>
@@ -2157,9 +2137,7 @@
         <v>6</v>
       </c>
       <c r="C30" s="34"/>
-      <c r="D30" s="35" t="s">
-        <v>51</v>
-      </c>
+      <c r="D30" s="35"/>
       <c r="E30" s="35"/>
       <c r="F30" s="35"/>
       <c r="G30" s="35"/>
@@ -2170,7 +2148,7 @@
       <c r="L30" s="35"/>
       <c r="M30" s="35"/>
       <c r="O30" s="36" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P30" s="36"/>
       <c r="Q30" s="18"/>
@@ -2223,10 +2201,10 @@
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="2"/>
       <c r="B32" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="C32" s="34" t="s">
         <v>53</v>
-      </c>
-      <c r="C32" s="34" t="s">
-        <v>54</v>
       </c>
       <c r="D32" s="34"/>
       <c r="E32" s="34"/>
@@ -2236,18 +2214,18 @@
       <c r="I32" s="34"/>
       <c r="J32" s="34"/>
       <c r="K32" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="L32" s="10" t="s">
         <v>55</v>
-      </c>
-      <c r="L32" s="10" t="s">
-        <v>56</v>
       </c>
       <c r="M32" s="10"/>
       <c r="N32" s="7"/>
       <c r="O32" s="37" t="s">
+        <v>52</v>
+      </c>
+      <c r="P32" s="34" t="s">
         <v>53</v>
-      </c>
-      <c r="P32" s="34" t="s">
-        <v>54</v>
       </c>
       <c r="Q32" s="34"/>
       <c r="R32" s="34"/>
@@ -2260,10 +2238,10 @@
       <c r="Y32" s="34"/>
       <c r="Z32" s="34"/>
       <c r="AA32" s="38" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="AB32" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="AC32" s="2"/>
       <c r="AD32" s="4"/>
@@ -2281,10 +2259,10 @@
       <c r="I33" s="34"/>
       <c r="J33" s="34"/>
       <c r="K33" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="L33" s="39" t="s">
         <v>58</v>
-      </c>
-      <c r="L33" s="39" t="s">
-        <v>59</v>
       </c>
       <c r="M33" s="39"/>
       <c r="N33" s="7"/>
@@ -2301,10 +2279,10 @@
       <c r="Y33" s="34"/>
       <c r="Z33" s="34"/>
       <c r="AA33" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="AB33" s="39" t="s">
         <v>58</v>
-      </c>
-      <c r="AB33" s="39" t="s">
-        <v>59</v>
       </c>
       <c r="AC33" s="2"/>
       <c r="AD33" s="4"/>
@@ -2314,7 +2292,7 @@
       <c r="A34" s="2"/>
       <c r="B34" s="37"/>
       <c r="C34" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D34" s="41"/>
       <c r="E34" s="41"/>
@@ -2324,16 +2302,16 @@
       <c r="I34" s="41"/>
       <c r="J34" s="41"/>
       <c r="K34" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="L34" s="43" t="s">
         <v>61</v>
-      </c>
-      <c r="L34" s="43" t="s">
-        <v>62</v>
       </c>
       <c r="M34" s="43"/>
       <c r="N34" s="7"/>
       <c r="O34" s="37"/>
       <c r="P34" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q34" s="44"/>
       <c r="R34" s="44"/>
@@ -2346,10 +2324,10 @@
       <c r="Y34" s="4"/>
       <c r="Z34" s="4"/>
       <c r="AA34" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB34" s="45" t="s">
         <v>64</v>
-      </c>
-      <c r="AB34" s="45" t="s">
-        <v>65</v>
       </c>
       <c r="AC34" s="2"/>
       <c r="AD34" s="4"/>
@@ -2359,7 +2337,7 @@
       <c r="A35" s="2"/>
       <c r="B35" s="37"/>
       <c r="C35" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D35" s="41"/>
       <c r="E35" s="41"/>
@@ -2369,16 +2347,16 @@
       <c r="I35" s="41"/>
       <c r="J35" s="41"/>
       <c r="K35" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="L35" s="43" t="s">
         <v>61</v>
-      </c>
-      <c r="L35" s="43" t="s">
-        <v>62</v>
       </c>
       <c r="M35" s="43"/>
       <c r="N35" s="7"/>
       <c r="O35" s="37"/>
       <c r="P35" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q35" s="44"/>
       <c r="R35" s="44"/>
@@ -2391,10 +2369,10 @@
       <c r="Y35" s="4"/>
       <c r="Z35" s="4"/>
       <c r="AA35" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB35" s="45" t="s">
         <v>64</v>
-      </c>
-      <c r="AB35" s="45" t="s">
-        <v>65</v>
       </c>
       <c r="AC35" s="2"/>
       <c r="AD35" s="4"/>
@@ -2404,7 +2382,7 @@
       <c r="A36" s="2"/>
       <c r="B36" s="37"/>
       <c r="C36" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D36" s="41"/>
       <c r="E36" s="41"/>
@@ -2414,16 +2392,16 @@
       <c r="I36" s="41"/>
       <c r="J36" s="41"/>
       <c r="K36" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="L36" s="43" t="s">
         <v>61</v>
-      </c>
-      <c r="L36" s="43" t="s">
-        <v>62</v>
       </c>
       <c r="M36" s="43"/>
       <c r="N36" s="7"/>
       <c r="O36" s="37"/>
       <c r="P36" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q36" s="44"/>
       <c r="R36" s="44"/>
@@ -2436,10 +2414,10 @@
       <c r="Y36" s="4"/>
       <c r="Z36" s="4"/>
       <c r="AA36" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB36" s="45" t="s">
         <v>64</v>
-      </c>
-      <c r="AB36" s="45" t="s">
-        <v>65</v>
       </c>
       <c r="AC36" s="2"/>
       <c r="AD36" s="4"/>
@@ -2449,7 +2427,7 @@
       <c r="A37" s="2"/>
       <c r="B37" s="37"/>
       <c r="C37" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D37" s="41"/>
       <c r="E37" s="41"/>
@@ -2459,16 +2437,16 @@
       <c r="I37" s="41"/>
       <c r="J37" s="41"/>
       <c r="K37" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="L37" s="43" t="s">
         <v>61</v>
-      </c>
-      <c r="L37" s="43" t="s">
-        <v>62</v>
       </c>
       <c r="M37" s="43"/>
       <c r="N37" s="7"/>
       <c r="O37" s="37"/>
       <c r="P37" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q37" s="44"/>
       <c r="R37" s="44"/>
@@ -2481,10 +2459,10 @@
       <c r="Y37" s="4"/>
       <c r="Z37" s="4"/>
       <c r="AA37" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB37" s="45" t="s">
         <v>64</v>
-      </c>
-      <c r="AB37" s="45" t="s">
-        <v>65</v>
       </c>
       <c r="AC37" s="2"/>
       <c r="AD37" s="4"/>
@@ -2494,7 +2472,7 @@
       <c r="A38" s="2"/>
       <c r="B38" s="37"/>
       <c r="C38" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D38" s="41"/>
       <c r="E38" s="41"/>
@@ -2504,16 +2482,16 @@
       <c r="I38" s="41"/>
       <c r="J38" s="41"/>
       <c r="K38" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="L38" s="43" t="s">
         <v>61</v>
-      </c>
-      <c r="L38" s="43" t="s">
-        <v>62</v>
       </c>
       <c r="M38" s="43"/>
       <c r="N38" s="7"/>
       <c r="O38" s="37"/>
       <c r="P38" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q38" s="44"/>
       <c r="R38" s="44"/>
@@ -2526,10 +2504,10 @@
       <c r="Y38" s="4"/>
       <c r="Z38" s="4"/>
       <c r="AA38" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB38" s="45" t="s">
         <v>64</v>
-      </c>
-      <c r="AB38" s="45" t="s">
-        <v>65</v>
       </c>
       <c r="AC38" s="2"/>
       <c r="AD38" s="4"/>
@@ -2539,7 +2517,7 @@
       <c r="A39" s="2"/>
       <c r="B39" s="37"/>
       <c r="C39" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D39" s="41"/>
       <c r="E39" s="41"/>
@@ -2549,16 +2527,16 @@
       <c r="I39" s="41"/>
       <c r="J39" s="41"/>
       <c r="K39" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="L39" s="43" t="s">
         <v>61</v>
-      </c>
-      <c r="L39" s="43" t="s">
-        <v>62</v>
       </c>
       <c r="M39" s="43"/>
       <c r="N39" s="7"/>
       <c r="O39" s="37"/>
       <c r="P39" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q39" s="44"/>
       <c r="R39" s="44"/>
@@ -2571,10 +2549,10 @@
       <c r="Y39" s="4"/>
       <c r="Z39" s="4"/>
       <c r="AA39" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB39" s="45" t="s">
         <v>64</v>
-      </c>
-      <c r="AB39" s="45" t="s">
-        <v>65</v>
       </c>
       <c r="AC39" s="2"/>
       <c r="AD39" s="4"/>
@@ -2584,7 +2562,7 @@
       <c r="A40" s="2"/>
       <c r="B40" s="37"/>
       <c r="C40" s="41" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D40" s="41"/>
       <c r="E40" s="41"/>
@@ -2594,16 +2572,16 @@
       <c r="I40" s="41"/>
       <c r="J40" s="41"/>
       <c r="K40" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="L40" s="43" t="s">
         <v>61</v>
-      </c>
-      <c r="L40" s="43" t="s">
-        <v>62</v>
       </c>
       <c r="M40" s="43"/>
       <c r="N40" s="7"/>
       <c r="O40" s="37"/>
       <c r="P40" s="44" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q40" s="44"/>
       <c r="R40" s="44"/>
@@ -2616,10 +2594,10 @@
       <c r="Y40" s="46"/>
       <c r="Z40" s="4"/>
       <c r="AA40" s="42" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB40" s="45" t="s">
         <v>64</v>
-      </c>
-      <c r="AB40" s="45" t="s">
-        <v>65</v>
       </c>
       <c r="AC40" s="2"/>
       <c r="AD40" s="4"/>
@@ -2663,44 +2641,44 @@
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="2"/>
       <c r="B42" s="13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C42" s="13"/>
       <c r="D42" s="13"/>
       <c r="E42" s="2"/>
       <c r="F42" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G42" s="13"/>
       <c r="H42" s="3"/>
       <c r="I42" s="13" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="J42" s="13"/>
       <c r="K42" s="13"/>
       <c r="L42" s="2"/>
       <c r="M42" s="13" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="N42" s="13"/>
       <c r="O42" s="13"/>
       <c r="P42" s="13"/>
       <c r="Q42" s="2"/>
       <c r="R42" s="13" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="S42" s="13"/>
       <c r="T42" s="13"/>
       <c r="U42" s="2"/>
       <c r="V42" s="13" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="W42" s="13"/>
       <c r="X42" s="2"/>
       <c r="Y42" s="47"/>
       <c r="Z42" s="2"/>
       <c r="AA42" s="13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="AB42" s="13"/>
       <c r="AC42" s="2"/>
@@ -2712,37 +2690,37 @@
     <row r="43" s="49" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
       <c r="B43" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
       <c r="E43" s="2"/>
       <c r="F43" s="48" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G43" s="48"/>
       <c r="H43" s="3"/>
       <c r="I43" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J43" s="20"/>
       <c r="K43" s="20"/>
       <c r="L43" s="2"/>
       <c r="M43" s="20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="N43" s="20"/>
       <c r="O43" s="20"/>
       <c r="P43" s="20"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="21" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S43" s="21"/>
       <c r="T43" s="21"/>
       <c r="U43" s="2"/>
       <c r="V43" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="W43" s="21"/>
       <c r="X43" s="2"/>
@@ -2793,94 +2771,94 @@
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="2"/>
       <c r="B45" s="13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C45" s="13"/>
       <c r="D45" s="13"/>
       <c r="E45" s="2"/>
       <c r="F45" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G45" s="13"/>
       <c r="H45" s="2"/>
       <c r="I45" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J45" s="13"/>
       <c r="K45" s="13"/>
       <c r="L45" s="2"/>
       <c r="M45" s="13" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="N45" s="13"/>
       <c r="O45" s="13"/>
       <c r="P45" s="13"/>
       <c r="Q45" s="51"/>
       <c r="R45" s="36" t="s">
+        <v>82</v>
+      </c>
+      <c r="S45" s="13" t="s">
         <v>83</v>
-      </c>
-      <c r="S45" s="13" t="s">
-        <v>84</v>
       </c>
       <c r="T45" s="13"/>
       <c r="U45" s="51"/>
       <c r="V45" s="36" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="W45" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="X45" s="2"/>
       <c r="Z45" s="33"/>
       <c r="AA45" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="AB45" s="6"/>
       <c r="AC45" s="2"/>
       <c r="AD45" s="52"/>
       <c r="AE45" s="52"/>
-      <c r="AF45" s="53"/>
+      <c r="AF45" s="4"/>
     </row>
     <row r="46" s="49" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2"/>
       <c r="B46" s="20" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C46" s="20"/>
       <c r="D46" s="20"/>
       <c r="E46" s="2"/>
-      <c r="F46" s="54" t="s">
+      <c r="F46" s="53" t="s">
+        <v>87</v>
+      </c>
+      <c r="G46" s="53"/>
+      <c r="H46" s="2"/>
+      <c r="I46" s="54" t="s">
         <v>88</v>
       </c>
-      <c r="G46" s="54"/>
-      <c r="H46" s="2"/>
-      <c r="I46" s="55" t="s">
-        <v>89</v>
-      </c>
-      <c r="J46" s="55"/>
-      <c r="K46" s="55"/>
+      <c r="J46" s="54"/>
+      <c r="K46" s="54"/>
       <c r="L46" s="2"/>
       <c r="M46" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="N46" s="20"/>
       <c r="O46" s="20"/>
       <c r="P46" s="20"/>
       <c r="Q46" s="51"/>
       <c r="R46" s="36"/>
-      <c r="S46" s="56"/>
-      <c r="T46" s="56"/>
+      <c r="S46" s="55"/>
+      <c r="T46" s="55"/>
       <c r="U46" s="51"/>
       <c r="V46" s="36"/>
-      <c r="W46" s="57"/>
+      <c r="W46" s="56"/>
       <c r="X46" s="2"/>
-      <c r="Z46" s="58"/>
+      <c r="Z46" s="57"/>
       <c r="AA46" s="6"/>
       <c r="AB46" s="6"/>
       <c r="AC46" s="2"/>
-      <c r="AD46" s="59"/>
-      <c r="AE46" s="59"/>
-      <c r="AF46" s="60"/>
+      <c r="AD46" s="58"/>
+      <c r="AE46" s="58"/>
+      <c r="AF46" s="17"/>
     </row>
     <row r="47" customFormat="false" ht="6.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="2"/>
@@ -2912,7 +2890,7 @@
       <c r="AC47" s="2"/>
       <c r="AD47" s="52"/>
       <c r="AE47" s="52"/>
-      <c r="AF47" s="53"/>
+      <c r="AF47" s="4"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="2"/>
@@ -2944,7 +2922,7 @@
       <c r="AC48" s="2"/>
       <c r="AD48" s="52"/>
       <c r="AE48" s="52"/>
-      <c r="AF48" s="53"/>
+      <c r="AF48" s="4"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="2"/>
@@ -2976,7 +2954,7 @@
       <c r="AC49" s="2"/>
       <c r="AD49" s="52"/>
       <c r="AE49" s="52"/>
-      <c r="AF49" s="53"/>
+      <c r="AF49" s="4"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="2"/>
@@ -3008,7 +2986,7 @@
       <c r="AC50" s="2"/>
       <c r="AD50" s="52"/>
       <c r="AE50" s="52"/>
-      <c r="AF50" s="53"/>
+      <c r="AF50" s="4"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="2"/>
@@ -3040,7 +3018,7 @@
       <c r="AC51" s="2"/>
       <c r="AD51" s="52"/>
       <c r="AE51" s="52"/>
-      <c r="AF51" s="53"/>
+      <c r="AF51" s="4"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="2"/>
@@ -3072,20 +3050,20 @@
       <c r="AC52" s="2"/>
       <c r="AD52" s="52"/>
       <c r="AE52" s="52"/>
-      <c r="AF52" s="53"/>
+      <c r="AF52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="2"/>
-      <c r="B53" s="61" t="s">
+      <c r="B53" s="59" t="s">
+        <v>90</v>
+      </c>
+      <c r="C53" s="59"/>
+      <c r="D53" s="59"/>
+      <c r="E53" s="59"/>
+      <c r="F53" s="59"/>
+      <c r="G53" s="59"/>
+      <c r="H53" s="2" t="s">
         <v>91</v>
-      </c>
-      <c r="C53" s="61"/>
-      <c r="D53" s="61"/>
-      <c r="E53" s="61"/>
-      <c r="F53" s="61"/>
-      <c r="G53" s="61"/>
-      <c r="H53" s="2" t="s">
-        <v>92</v>
       </c>
       <c r="I53" s="2"/>
       <c r="J53" s="2"/>
@@ -3097,7 +3075,7 @@
       <c r="P53" s="2"/>
       <c r="Q53" s="2"/>
       <c r="R53" s="2" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="S53" s="2"/>
       <c r="T53" s="2"/>
@@ -3110,7 +3088,7 @@
       <c r="AC53" s="2"/>
       <c r="AD53" s="52"/>
       <c r="AE53" s="52"/>
-      <c r="AF53" s="53"/>
+      <c r="AF53" s="4"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="2"/>
@@ -3131,7 +3109,7 @@
       <c r="P54" s="2"/>
       <c r="Q54" s="2"/>
       <c r="R54" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="S54" s="2"/>
       <c r="T54" s="2"/>
@@ -3144,7 +3122,7 @@
       <c r="AC54" s="2"/>
       <c r="AD54" s="52"/>
       <c r="AE54" s="52"/>
-      <c r="AF54" s="53"/>
+      <c r="AF54" s="4"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="2"/>
@@ -3178,37 +3156,9 @@
       <c r="AC55" s="2"/>
       <c r="AD55" s="52"/>
       <c r="AE55" s="52"/>
-      <c r="AF55" s="53"/>
+      <c r="AF55" s="4"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="62"/>
-      <c r="B56" s="62"/>
-      <c r="C56" s="62"/>
-      <c r="D56" s="62"/>
-      <c r="E56" s="62"/>
-      <c r="F56" s="62"/>
-      <c r="G56" s="62"/>
-      <c r="H56" s="62"/>
-      <c r="I56" s="62"/>
-      <c r="J56" s="62"/>
-      <c r="K56" s="62"/>
-      <c r="L56" s="62"/>
-      <c r="M56" s="62"/>
-      <c r="N56" s="62"/>
-      <c r="O56" s="62"/>
-      <c r="P56" s="62"/>
-      <c r="Q56" s="62"/>
-      <c r="R56" s="62"/>
-      <c r="S56" s="62"/>
-      <c r="T56" s="62"/>
-      <c r="U56" s="62"/>
-      <c r="V56" s="62"/>
-      <c r="W56" s="62"/>
-      <c r="X56" s="62"/>
-      <c r="Y56" s="62"/>
-      <c r="Z56" s="62"/>
-      <c r="AA56" s="62"/>
-      <c r="AB56" s="62"/>
       <c r="AC56" s="2"/>
       <c r="AD56" s="52"/>
     </row>
@@ -3410,28 +3360,28 @@
   </sheetPr>
   <dimension ref="B1:Z47"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C34" activeCellId="0" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="0" width="3.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="3" style="0" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="2.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="6.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="3.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="6.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="3.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="1.56"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="60" width="3.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="60" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="3" style="60" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="60" width="2.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="60" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="60" width="3.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="60" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="60" width="3.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="60" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="60" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="60" width="1.56"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
@@ -3445,7 +3395,7 @@
       <c r="L1" s="12"/>
       <c r="M1" s="12"/>
       <c r="O1" s="12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="P1" s="12"/>
       <c r="Q1" s="12"/>
@@ -3461,33 +3411,33 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G2" s="13"/>
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
       <c r="J2" s="13" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="K2" s="13"/>
       <c r="L2" s="13"/>
       <c r="M2" s="13"/>
       <c r="O2" s="13" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="P2" s="13"/>
       <c r="Q2" s="13" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="R2" s="13"/>
       <c r="S2" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="T2" s="13"/>
       <c r="U2" s="13"/>
@@ -3498,516 +3448,516 @@
       <c r="Z2" s="13"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="63"/>
-      <c r="C3" s="64"/>
-      <c r="D3" s="64"/>
-      <c r="E3" s="65"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="64"/>
-      <c r="H3" s="64"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="64"/>
-      <c r="L3" s="64"/>
-      <c r="M3" s="65"/>
-      <c r="O3" s="63"/>
-      <c r="P3" s="65"/>
-      <c r="Q3" s="63"/>
-      <c r="R3" s="65"/>
-      <c r="S3" s="66"/>
-      <c r="T3" s="67"/>
-      <c r="U3" s="67"/>
-      <c r="V3" s="67"/>
-      <c r="W3" s="67"/>
-      <c r="X3" s="67"/>
-      <c r="Y3" s="67"/>
-      <c r="Z3" s="68"/>
+      <c r="B3" s="61"/>
+      <c r="C3" s="62"/>
+      <c r="D3" s="62"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="61"/>
+      <c r="G3" s="62"/>
+      <c r="H3" s="62"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="61"/>
+      <c r="K3" s="62"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="63"/>
+      <c r="O3" s="61"/>
+      <c r="P3" s="63"/>
+      <c r="Q3" s="61"/>
+      <c r="R3" s="63"/>
+      <c r="S3" s="64"/>
+      <c r="T3" s="65"/>
+      <c r="U3" s="65"/>
+      <c r="V3" s="65"/>
+      <c r="W3" s="65"/>
+      <c r="X3" s="65"/>
+      <c r="Y3" s="65"/>
+      <c r="Z3" s="66"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="63"/>
-      <c r="C4" s="64"/>
-      <c r="D4" s="64"/>
-      <c r="E4" s="65"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="64"/>
-      <c r="H4" s="64"/>
-      <c r="I4" s="65"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="64"/>
-      <c r="L4" s="64"/>
-      <c r="M4" s="65"/>
-      <c r="O4" s="63"/>
-      <c r="P4" s="65"/>
-      <c r="Q4" s="63"/>
-      <c r="R4" s="65"/>
-      <c r="S4" s="63"/>
-      <c r="T4" s="64"/>
-      <c r="U4" s="64"/>
-      <c r="V4" s="64"/>
-      <c r="W4" s="64"/>
-      <c r="X4" s="64"/>
-      <c r="Y4" s="64"/>
-      <c r="Z4" s="65"/>
+      <c r="B4" s="61"/>
+      <c r="C4" s="62"/>
+      <c r="D4" s="62"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="62"/>
+      <c r="H4" s="62"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="62"/>
+      <c r="L4" s="62"/>
+      <c r="M4" s="63"/>
+      <c r="O4" s="61"/>
+      <c r="P4" s="63"/>
+      <c r="Q4" s="61"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="61"/>
+      <c r="T4" s="62"/>
+      <c r="U4" s="62"/>
+      <c r="V4" s="62"/>
+      <c r="W4" s="62"/>
+      <c r="X4" s="62"/>
+      <c r="Y4" s="62"/>
+      <c r="Z4" s="63"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="63"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64"/>
-      <c r="E5" s="65"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="64"/>
-      <c r="H5" s="64"/>
-      <c r="I5" s="65"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="64"/>
-      <c r="L5" s="64"/>
-      <c r="M5" s="65"/>
-      <c r="O5" s="63"/>
-      <c r="P5" s="65"/>
-      <c r="Q5" s="63"/>
-      <c r="R5" s="65"/>
-      <c r="S5" s="63"/>
-      <c r="T5" s="64"/>
-      <c r="U5" s="64"/>
-      <c r="V5" s="64"/>
-      <c r="W5" s="64"/>
-      <c r="X5" s="64"/>
-      <c r="Y5" s="64"/>
-      <c r="Z5" s="65"/>
+      <c r="B5" s="61"/>
+      <c r="C5" s="62"/>
+      <c r="D5" s="62"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="61"/>
+      <c r="G5" s="62"/>
+      <c r="H5" s="62"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="61"/>
+      <c r="K5" s="62"/>
+      <c r="L5" s="62"/>
+      <c r="M5" s="63"/>
+      <c r="O5" s="61"/>
+      <c r="P5" s="63"/>
+      <c r="Q5" s="61"/>
+      <c r="R5" s="63"/>
+      <c r="S5" s="61"/>
+      <c r="T5" s="62"/>
+      <c r="U5" s="62"/>
+      <c r="V5" s="62"/>
+      <c r="W5" s="62"/>
+      <c r="X5" s="62"/>
+      <c r="Y5" s="62"/>
+      <c r="Z5" s="63"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="63"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="65"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="64"/>
-      <c r="H6" s="64"/>
-      <c r="I6" s="65"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="64"/>
-      <c r="L6" s="64"/>
-      <c r="M6" s="65"/>
-      <c r="O6" s="63"/>
-      <c r="P6" s="65"/>
-      <c r="Q6" s="63"/>
-      <c r="R6" s="65"/>
-      <c r="S6" s="63"/>
-      <c r="T6" s="64"/>
-      <c r="U6" s="64"/>
-      <c r="V6" s="64"/>
-      <c r="W6" s="64"/>
-      <c r="X6" s="64"/>
-      <c r="Y6" s="64"/>
-      <c r="Z6" s="65"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="61"/>
+      <c r="G6" s="62"/>
+      <c r="H6" s="62"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="61"/>
+      <c r="K6" s="62"/>
+      <c r="L6" s="62"/>
+      <c r="M6" s="63"/>
+      <c r="O6" s="61"/>
+      <c r="P6" s="63"/>
+      <c r="Q6" s="61"/>
+      <c r="R6" s="63"/>
+      <c r="S6" s="61"/>
+      <c r="T6" s="62"/>
+      <c r="U6" s="62"/>
+      <c r="V6" s="62"/>
+      <c r="W6" s="62"/>
+      <c r="X6" s="62"/>
+      <c r="Y6" s="62"/>
+      <c r="Z6" s="63"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="63"/>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="65"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="64"/>
-      <c r="H7" s="64"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="63"/>
-      <c r="K7" s="64"/>
-      <c r="L7" s="64"/>
-      <c r="M7" s="65"/>
-      <c r="O7" s="63"/>
-      <c r="P7" s="65"/>
-      <c r="Q7" s="63"/>
-      <c r="R7" s="65"/>
-      <c r="S7" s="63"/>
-      <c r="T7" s="64"/>
-      <c r="U7" s="64"/>
-      <c r="V7" s="64"/>
-      <c r="W7" s="64"/>
-      <c r="X7" s="64"/>
-      <c r="Y7" s="64"/>
-      <c r="Z7" s="65"/>
+      <c r="B7" s="61"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="63"/>
+      <c r="F7" s="61"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="63"/>
+      <c r="J7" s="61"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="63"/>
+      <c r="O7" s="61"/>
+      <c r="P7" s="63"/>
+      <c r="Q7" s="61"/>
+      <c r="R7" s="63"/>
+      <c r="S7" s="61"/>
+      <c r="T7" s="62"/>
+      <c r="U7" s="62"/>
+      <c r="V7" s="62"/>
+      <c r="W7" s="62"/>
+      <c r="X7" s="62"/>
+      <c r="Y7" s="62"/>
+      <c r="Z7" s="63"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="63"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="65"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="64"/>
-      <c r="H8" s="64"/>
-      <c r="I8" s="65"/>
-      <c r="J8" s="63"/>
-      <c r="K8" s="64"/>
-      <c r="L8" s="64"/>
-      <c r="M8" s="65"/>
-      <c r="O8" s="63"/>
-      <c r="P8" s="65"/>
-      <c r="Q8" s="63"/>
-      <c r="R8" s="65"/>
-      <c r="S8" s="63"/>
-      <c r="T8" s="64"/>
-      <c r="U8" s="64"/>
-      <c r="V8" s="64"/>
-      <c r="W8" s="64"/>
-      <c r="X8" s="64"/>
-      <c r="Y8" s="64"/>
-      <c r="Z8" s="65"/>
+      <c r="B8" s="61"/>
+      <c r="C8" s="62"/>
+      <c r="D8" s="62"/>
+      <c r="E8" s="63"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="62"/>
+      <c r="H8" s="62"/>
+      <c r="I8" s="63"/>
+      <c r="J8" s="61"/>
+      <c r="K8" s="62"/>
+      <c r="L8" s="62"/>
+      <c r="M8" s="63"/>
+      <c r="O8" s="61"/>
+      <c r="P8" s="63"/>
+      <c r="Q8" s="61"/>
+      <c r="R8" s="63"/>
+      <c r="S8" s="61"/>
+      <c r="T8" s="62"/>
+      <c r="U8" s="62"/>
+      <c r="V8" s="62"/>
+      <c r="W8" s="62"/>
+      <c r="X8" s="62"/>
+      <c r="Y8" s="62"/>
+      <c r="Z8" s="63"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="63"/>
-      <c r="C9" s="64"/>
-      <c r="D9" s="64"/>
-      <c r="E9" s="65"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="64"/>
-      <c r="H9" s="64"/>
-      <c r="I9" s="65"/>
-      <c r="J9" s="63"/>
-      <c r="K9" s="64"/>
-      <c r="L9" s="64"/>
-      <c r="M9" s="65"/>
-      <c r="O9" s="63"/>
-      <c r="P9" s="65"/>
-      <c r="Q9" s="63"/>
-      <c r="R9" s="65"/>
-      <c r="S9" s="63"/>
-      <c r="T9" s="64"/>
-      <c r="U9" s="64"/>
-      <c r="V9" s="64"/>
-      <c r="W9" s="64"/>
-      <c r="X9" s="64"/>
-      <c r="Y9" s="64"/>
-      <c r="Z9" s="65"/>
+      <c r="B9" s="61"/>
+      <c r="C9" s="62"/>
+      <c r="D9" s="62"/>
+      <c r="E9" s="63"/>
+      <c r="F9" s="61"/>
+      <c r="G9" s="62"/>
+      <c r="H9" s="62"/>
+      <c r="I9" s="63"/>
+      <c r="J9" s="61"/>
+      <c r="K9" s="62"/>
+      <c r="L9" s="62"/>
+      <c r="M9" s="63"/>
+      <c r="O9" s="61"/>
+      <c r="P9" s="63"/>
+      <c r="Q9" s="61"/>
+      <c r="R9" s="63"/>
+      <c r="S9" s="61"/>
+      <c r="T9" s="62"/>
+      <c r="U9" s="62"/>
+      <c r="V9" s="62"/>
+      <c r="W9" s="62"/>
+      <c r="X9" s="62"/>
+      <c r="Y9" s="62"/>
+      <c r="Z9" s="63"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="63"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="65"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="64"/>
-      <c r="H10" s="64"/>
-      <c r="I10" s="65"/>
-      <c r="J10" s="63"/>
-      <c r="K10" s="64"/>
-      <c r="L10" s="64"/>
-      <c r="M10" s="65"/>
-      <c r="O10" s="63"/>
-      <c r="P10" s="65"/>
-      <c r="Q10" s="63"/>
-      <c r="R10" s="65"/>
-      <c r="S10" s="63"/>
-      <c r="T10" s="64"/>
-      <c r="U10" s="64"/>
-      <c r="V10" s="64"/>
-      <c r="W10" s="64"/>
-      <c r="X10" s="64"/>
-      <c r="Y10" s="64"/>
-      <c r="Z10" s="65"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="63"/>
+      <c r="F10" s="61"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="63"/>
+      <c r="J10" s="61"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="63"/>
+      <c r="O10" s="61"/>
+      <c r="P10" s="63"/>
+      <c r="Q10" s="61"/>
+      <c r="R10" s="63"/>
+      <c r="S10" s="61"/>
+      <c r="T10" s="62"/>
+      <c r="U10" s="62"/>
+      <c r="V10" s="62"/>
+      <c r="W10" s="62"/>
+      <c r="X10" s="62"/>
+      <c r="Y10" s="62"/>
+      <c r="Z10" s="63"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="63"/>
-      <c r="C11" s="64"/>
-      <c r="D11" s="64"/>
-      <c r="E11" s="65"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="64"/>
-      <c r="H11" s="64"/>
-      <c r="I11" s="65"/>
-      <c r="J11" s="63"/>
-      <c r="K11" s="64"/>
-      <c r="L11" s="64"/>
-      <c r="M11" s="65"/>
-      <c r="O11" s="63"/>
-      <c r="P11" s="65"/>
-      <c r="Q11" s="63"/>
-      <c r="R11" s="65"/>
-      <c r="S11" s="63"/>
-      <c r="T11" s="64"/>
-      <c r="U11" s="64"/>
-      <c r="V11" s="64"/>
-      <c r="W11" s="64"/>
-      <c r="X11" s="64"/>
-      <c r="Y11" s="64"/>
-      <c r="Z11" s="65"/>
+      <c r="B11" s="61"/>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="63"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="62"/>
+      <c r="H11" s="62"/>
+      <c r="I11" s="63"/>
+      <c r="J11" s="61"/>
+      <c r="K11" s="62"/>
+      <c r="L11" s="62"/>
+      <c r="M11" s="63"/>
+      <c r="O11" s="61"/>
+      <c r="P11" s="63"/>
+      <c r="Q11" s="61"/>
+      <c r="R11" s="63"/>
+      <c r="S11" s="61"/>
+      <c r="T11" s="62"/>
+      <c r="U11" s="62"/>
+      <c r="V11" s="62"/>
+      <c r="W11" s="62"/>
+      <c r="X11" s="62"/>
+      <c r="Y11" s="62"/>
+      <c r="Z11" s="63"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="63"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="64"/>
-      <c r="E12" s="65"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="64"/>
-      <c r="I12" s="65"/>
-      <c r="J12" s="63"/>
-      <c r="K12" s="64"/>
-      <c r="L12" s="64"/>
-      <c r="M12" s="65"/>
-      <c r="O12" s="63"/>
-      <c r="P12" s="65"/>
-      <c r="Q12" s="63"/>
-      <c r="R12" s="65"/>
-      <c r="S12" s="63"/>
-      <c r="T12" s="64"/>
-      <c r="U12" s="64"/>
-      <c r="V12" s="64"/>
-      <c r="W12" s="64"/>
-      <c r="X12" s="64"/>
-      <c r="Y12" s="64"/>
-      <c r="Z12" s="65"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="62"/>
+      <c r="D12" s="62"/>
+      <c r="E12" s="63"/>
+      <c r="F12" s="61"/>
+      <c r="G12" s="62"/>
+      <c r="H12" s="62"/>
+      <c r="I12" s="63"/>
+      <c r="J12" s="61"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="62"/>
+      <c r="M12" s="63"/>
+      <c r="O12" s="61"/>
+      <c r="P12" s="63"/>
+      <c r="Q12" s="61"/>
+      <c r="R12" s="63"/>
+      <c r="S12" s="61"/>
+      <c r="T12" s="62"/>
+      <c r="U12" s="62"/>
+      <c r="V12" s="62"/>
+      <c r="W12" s="62"/>
+      <c r="X12" s="62"/>
+      <c r="Y12" s="62"/>
+      <c r="Z12" s="63"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="63"/>
-      <c r="C13" s="64"/>
-      <c r="D13" s="64"/>
-      <c r="E13" s="65"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="64"/>
-      <c r="I13" s="65"/>
-      <c r="J13" s="63"/>
-      <c r="K13" s="64"/>
-      <c r="L13" s="64"/>
-      <c r="M13" s="65"/>
-      <c r="O13" s="63"/>
-      <c r="P13" s="65"/>
-      <c r="Q13" s="63"/>
-      <c r="R13" s="65"/>
-      <c r="S13" s="63"/>
-      <c r="T13" s="64"/>
-      <c r="U13" s="64"/>
-      <c r="V13" s="64"/>
-      <c r="W13" s="64"/>
-      <c r="X13" s="64"/>
-      <c r="Y13" s="64"/>
-      <c r="Z13" s="65"/>
+      <c r="B13" s="61"/>
+      <c r="C13" s="62"/>
+      <c r="D13" s="62"/>
+      <c r="E13" s="63"/>
+      <c r="F13" s="61"/>
+      <c r="G13" s="62"/>
+      <c r="H13" s="62"/>
+      <c r="I13" s="63"/>
+      <c r="J13" s="61"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="62"/>
+      <c r="M13" s="63"/>
+      <c r="O13" s="61"/>
+      <c r="P13" s="63"/>
+      <c r="Q13" s="61"/>
+      <c r="R13" s="63"/>
+      <c r="S13" s="61"/>
+      <c r="T13" s="62"/>
+      <c r="U13" s="62"/>
+      <c r="V13" s="62"/>
+      <c r="W13" s="62"/>
+      <c r="X13" s="62"/>
+      <c r="Y13" s="62"/>
+      <c r="Z13" s="63"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="63"/>
-      <c r="C14" s="64"/>
-      <c r="D14" s="64"/>
-      <c r="E14" s="65"/>
-      <c r="F14" s="63"/>
-      <c r="G14" s="64"/>
-      <c r="H14" s="64"/>
-      <c r="I14" s="65"/>
-      <c r="J14" s="63"/>
-      <c r="K14" s="64"/>
-      <c r="L14" s="64"/>
-      <c r="M14" s="65"/>
-      <c r="O14" s="63"/>
-      <c r="P14" s="65"/>
-      <c r="Q14" s="63"/>
-      <c r="R14" s="65"/>
-      <c r="S14" s="63"/>
-      <c r="T14" s="64"/>
-      <c r="U14" s="64"/>
-      <c r="V14" s="64"/>
-      <c r="W14" s="64"/>
-      <c r="X14" s="64"/>
-      <c r="Y14" s="64"/>
-      <c r="Z14" s="65"/>
+      <c r="B14" s="61"/>
+      <c r="C14" s="62"/>
+      <c r="D14" s="62"/>
+      <c r="E14" s="63"/>
+      <c r="F14" s="61"/>
+      <c r="G14" s="62"/>
+      <c r="H14" s="62"/>
+      <c r="I14" s="63"/>
+      <c r="J14" s="61"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="62"/>
+      <c r="M14" s="63"/>
+      <c r="O14" s="61"/>
+      <c r="P14" s="63"/>
+      <c r="Q14" s="61"/>
+      <c r="R14" s="63"/>
+      <c r="S14" s="61"/>
+      <c r="T14" s="62"/>
+      <c r="U14" s="62"/>
+      <c r="V14" s="62"/>
+      <c r="W14" s="62"/>
+      <c r="X14" s="62"/>
+      <c r="Y14" s="62"/>
+      <c r="Z14" s="63"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="63"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="64"/>
-      <c r="E15" s="65"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="64"/>
-      <c r="H15" s="64"/>
-      <c r="I15" s="65"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="64"/>
-      <c r="L15" s="64"/>
-      <c r="M15" s="65"/>
-      <c r="O15" s="63"/>
-      <c r="P15" s="65"/>
-      <c r="Q15" s="63"/>
-      <c r="R15" s="65"/>
-      <c r="S15" s="63"/>
-      <c r="T15" s="64"/>
-      <c r="U15" s="64"/>
-      <c r="V15" s="64"/>
-      <c r="W15" s="64"/>
-      <c r="X15" s="64"/>
-      <c r="Y15" s="64"/>
-      <c r="Z15" s="65"/>
+      <c r="B15" s="61"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="61"/>
+      <c r="G15" s="62"/>
+      <c r="H15" s="62"/>
+      <c r="I15" s="63"/>
+      <c r="J15" s="61"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="62"/>
+      <c r="M15" s="63"/>
+      <c r="O15" s="61"/>
+      <c r="P15" s="63"/>
+      <c r="Q15" s="61"/>
+      <c r="R15" s="63"/>
+      <c r="S15" s="61"/>
+      <c r="T15" s="62"/>
+      <c r="U15" s="62"/>
+      <c r="V15" s="62"/>
+      <c r="W15" s="62"/>
+      <c r="X15" s="62"/>
+      <c r="Y15" s="62"/>
+      <c r="Z15" s="63"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="63"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="64"/>
-      <c r="H16" s="64"/>
-      <c r="I16" s="65"/>
-      <c r="J16" s="63"/>
-      <c r="K16" s="64"/>
-      <c r="L16" s="64"/>
-      <c r="M16" s="65"/>
-      <c r="O16" s="63"/>
-      <c r="P16" s="65"/>
-      <c r="Q16" s="63"/>
-      <c r="R16" s="65"/>
-      <c r="S16" s="63"/>
-      <c r="T16" s="64"/>
-      <c r="U16" s="64"/>
-      <c r="V16" s="64"/>
-      <c r="W16" s="64"/>
-      <c r="X16" s="64"/>
-      <c r="Y16" s="64"/>
-      <c r="Z16" s="65"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="62"/>
+      <c r="D16" s="62"/>
+      <c r="E16" s="63"/>
+      <c r="F16" s="61"/>
+      <c r="G16" s="62"/>
+      <c r="H16" s="62"/>
+      <c r="I16" s="63"/>
+      <c r="J16" s="61"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="62"/>
+      <c r="M16" s="63"/>
+      <c r="O16" s="61"/>
+      <c r="P16" s="63"/>
+      <c r="Q16" s="61"/>
+      <c r="R16" s="63"/>
+      <c r="S16" s="61"/>
+      <c r="T16" s="62"/>
+      <c r="U16" s="62"/>
+      <c r="V16" s="62"/>
+      <c r="W16" s="62"/>
+      <c r="X16" s="62"/>
+      <c r="Y16" s="62"/>
+      <c r="Z16" s="63"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="63"/>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="65"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="64"/>
-      <c r="H17" s="64"/>
-      <c r="I17" s="65"/>
-      <c r="J17" s="63"/>
-      <c r="K17" s="64"/>
-      <c r="L17" s="64"/>
-      <c r="M17" s="65"/>
-      <c r="O17" s="63"/>
-      <c r="P17" s="65"/>
-      <c r="Q17" s="63"/>
-      <c r="R17" s="65"/>
-      <c r="S17" s="63"/>
-      <c r="T17" s="64"/>
-      <c r="U17" s="64"/>
-      <c r="V17" s="64"/>
-      <c r="W17" s="64"/>
-      <c r="X17" s="64"/>
-      <c r="Y17" s="64"/>
-      <c r="Z17" s="65"/>
+      <c r="B17" s="61"/>
+      <c r="C17" s="62"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="63"/>
+      <c r="F17" s="61"/>
+      <c r="G17" s="62"/>
+      <c r="H17" s="62"/>
+      <c r="I17" s="63"/>
+      <c r="J17" s="61"/>
+      <c r="K17" s="62"/>
+      <c r="L17" s="62"/>
+      <c r="M17" s="63"/>
+      <c r="O17" s="61"/>
+      <c r="P17" s="63"/>
+      <c r="Q17" s="61"/>
+      <c r="R17" s="63"/>
+      <c r="S17" s="61"/>
+      <c r="T17" s="62"/>
+      <c r="U17" s="62"/>
+      <c r="V17" s="62"/>
+      <c r="W17" s="62"/>
+      <c r="X17" s="62"/>
+      <c r="Y17" s="62"/>
+      <c r="Z17" s="63"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="63"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="64"/>
-      <c r="H18" s="64"/>
-      <c r="I18" s="65"/>
-      <c r="J18" s="63"/>
-      <c r="K18" s="64"/>
-      <c r="L18" s="64"/>
-      <c r="M18" s="65"/>
-      <c r="O18" s="63"/>
-      <c r="P18" s="65"/>
-      <c r="Q18" s="63"/>
-      <c r="R18" s="65"/>
-      <c r="S18" s="63"/>
-      <c r="T18" s="64"/>
-      <c r="U18" s="64"/>
-      <c r="V18" s="64"/>
-      <c r="W18" s="64"/>
-      <c r="X18" s="64"/>
-      <c r="Y18" s="64"/>
-      <c r="Z18" s="65"/>
+      <c r="B18" s="61"/>
+      <c r="C18" s="62"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="61"/>
+      <c r="G18" s="62"/>
+      <c r="H18" s="62"/>
+      <c r="I18" s="63"/>
+      <c r="J18" s="61"/>
+      <c r="K18" s="62"/>
+      <c r="L18" s="62"/>
+      <c r="M18" s="63"/>
+      <c r="O18" s="61"/>
+      <c r="P18" s="63"/>
+      <c r="Q18" s="61"/>
+      <c r="R18" s="63"/>
+      <c r="S18" s="61"/>
+      <c r="T18" s="62"/>
+      <c r="U18" s="62"/>
+      <c r="V18" s="62"/>
+      <c r="W18" s="62"/>
+      <c r="X18" s="62"/>
+      <c r="Y18" s="62"/>
+      <c r="Z18" s="63"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="63"/>
-      <c r="C19" s="64"/>
-      <c r="D19" s="64"/>
-      <c r="E19" s="65"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="64"/>
-      <c r="H19" s="64"/>
-      <c r="I19" s="65"/>
-      <c r="J19" s="63"/>
-      <c r="K19" s="64"/>
-      <c r="L19" s="64"/>
-      <c r="M19" s="65"/>
-      <c r="O19" s="63"/>
-      <c r="P19" s="65"/>
-      <c r="Q19" s="63"/>
-      <c r="R19" s="65"/>
-      <c r="S19" s="63"/>
-      <c r="T19" s="64"/>
-      <c r="U19" s="64"/>
-      <c r="V19" s="64"/>
-      <c r="W19" s="64"/>
-      <c r="X19" s="64"/>
-      <c r="Y19" s="64"/>
-      <c r="Z19" s="65"/>
+      <c r="B19" s="61"/>
+      <c r="C19" s="62"/>
+      <c r="D19" s="62"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="61"/>
+      <c r="G19" s="62"/>
+      <c r="H19" s="62"/>
+      <c r="I19" s="63"/>
+      <c r="J19" s="61"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="62"/>
+      <c r="M19" s="63"/>
+      <c r="O19" s="61"/>
+      <c r="P19" s="63"/>
+      <c r="Q19" s="61"/>
+      <c r="R19" s="63"/>
+      <c r="S19" s="61"/>
+      <c r="T19" s="62"/>
+      <c r="U19" s="62"/>
+      <c r="V19" s="62"/>
+      <c r="W19" s="62"/>
+      <c r="X19" s="62"/>
+      <c r="Y19" s="62"/>
+      <c r="Z19" s="63"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="63"/>
-      <c r="C20" s="64"/>
-      <c r="D20" s="64"/>
-      <c r="E20" s="65"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="64"/>
-      <c r="H20" s="64"/>
-      <c r="I20" s="65"/>
-      <c r="J20" s="63"/>
-      <c r="K20" s="64"/>
-      <c r="L20" s="64"/>
-      <c r="M20" s="65"/>
-      <c r="O20" s="63"/>
-      <c r="P20" s="65"/>
-      <c r="Q20" s="63"/>
-      <c r="R20" s="65"/>
-      <c r="S20" s="63"/>
-      <c r="T20" s="64"/>
-      <c r="U20" s="64"/>
-      <c r="V20" s="64"/>
-      <c r="W20" s="64"/>
-      <c r="X20" s="64"/>
-      <c r="Y20" s="64"/>
-      <c r="Z20" s="65"/>
+      <c r="B20" s="61"/>
+      <c r="C20" s="62"/>
+      <c r="D20" s="62"/>
+      <c r="E20" s="63"/>
+      <c r="F20" s="61"/>
+      <c r="G20" s="62"/>
+      <c r="H20" s="62"/>
+      <c r="I20" s="63"/>
+      <c r="J20" s="61"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="62"/>
+      <c r="M20" s="63"/>
+      <c r="O20" s="61"/>
+      <c r="P20" s="63"/>
+      <c r="Q20" s="61"/>
+      <c r="R20" s="63"/>
+      <c r="S20" s="61"/>
+      <c r="T20" s="62"/>
+      <c r="U20" s="62"/>
+      <c r="V20" s="62"/>
+      <c r="W20" s="62"/>
+      <c r="X20" s="62"/>
+      <c r="Y20" s="62"/>
+      <c r="Z20" s="63"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="69"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="70"/>
-      <c r="E21" s="71"/>
-      <c r="F21" s="69"/>
-      <c r="G21" s="70"/>
-      <c r="H21" s="70"/>
-      <c r="I21" s="71"/>
-      <c r="J21" s="69"/>
-      <c r="K21" s="70"/>
-      <c r="L21" s="70"/>
-      <c r="M21" s="71"/>
-      <c r="O21" s="63"/>
-      <c r="P21" s="65"/>
-      <c r="Q21" s="63"/>
-      <c r="R21" s="65"/>
-      <c r="S21" s="63"/>
-      <c r="T21" s="64"/>
-      <c r="U21" s="64"/>
-      <c r="V21" s="64"/>
-      <c r="W21" s="64"/>
-      <c r="X21" s="64"/>
-      <c r="Y21" s="64"/>
-      <c r="Z21" s="65"/>
+      <c r="B21" s="67"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="69"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="69"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="68"/>
+      <c r="L21" s="68"/>
+      <c r="M21" s="69"/>
+      <c r="O21" s="61"/>
+      <c r="P21" s="63"/>
+      <c r="Q21" s="61"/>
+      <c r="R21" s="63"/>
+      <c r="S21" s="61"/>
+      <c r="T21" s="62"/>
+      <c r="U21" s="62"/>
+      <c r="V21" s="62"/>
+      <c r="W21" s="62"/>
+      <c r="X21" s="62"/>
+      <c r="Y21" s="62"/>
+      <c r="Z21" s="63"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O22" s="63"/>
-      <c r="P22" s="65"/>
-      <c r="Q22" s="63"/>
-      <c r="R22" s="65"/>
-      <c r="S22" s="63"/>
-      <c r="T22" s="64"/>
-      <c r="U22" s="64"/>
-      <c r="V22" s="64"/>
-      <c r="W22" s="64"/>
-      <c r="X22" s="64"/>
-      <c r="Y22" s="64"/>
-      <c r="Z22" s="65"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="O22" s="61"/>
+      <c r="P22" s="63"/>
+      <c r="Q22" s="61"/>
+      <c r="R22" s="63"/>
+      <c r="S22" s="61"/>
+      <c r="T22" s="62"/>
+      <c r="U22" s="62"/>
+      <c r="V22" s="62"/>
+      <c r="W22" s="62"/>
+      <c r="X22" s="62"/>
+      <c r="Y22" s="62"/>
+      <c r="Z22" s="63"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C23" s="12"/>
       <c r="D23" s="12"/>
@@ -4020,340 +3970,340 @@
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
-      <c r="O23" s="63"/>
-      <c r="P23" s="65"/>
-      <c r="Q23" s="63"/>
-      <c r="R23" s="65"/>
-      <c r="S23" s="63"/>
-      <c r="T23" s="64"/>
-      <c r="U23" s="64"/>
-      <c r="V23" s="64"/>
-      <c r="W23" s="64"/>
-      <c r="X23" s="64"/>
-      <c r="Y23" s="64"/>
-      <c r="Z23" s="65"/>
+      <c r="O23" s="61"/>
+      <c r="P23" s="63"/>
+      <c r="Q23" s="61"/>
+      <c r="R23" s="63"/>
+      <c r="S23" s="61"/>
+      <c r="T23" s="62"/>
+      <c r="U23" s="62"/>
+      <c r="V23" s="62"/>
+      <c r="W23" s="62"/>
+      <c r="X23" s="62"/>
+      <c r="Y23" s="62"/>
+      <c r="Z23" s="63"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="13" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G24" s="13"/>
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
       <c r="J24" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
-      <c r="O24" s="63"/>
-      <c r="P24" s="65"/>
-      <c r="Q24" s="63"/>
-      <c r="R24" s="65"/>
-      <c r="S24" s="63"/>
-      <c r="T24" s="64"/>
-      <c r="U24" s="64"/>
-      <c r="V24" s="64"/>
-      <c r="W24" s="64"/>
-      <c r="X24" s="64"/>
-      <c r="Y24" s="64"/>
-      <c r="Z24" s="65"/>
+      <c r="O24" s="61"/>
+      <c r="P24" s="63"/>
+      <c r="Q24" s="61"/>
+      <c r="R24" s="63"/>
+      <c r="S24" s="61"/>
+      <c r="T24" s="62"/>
+      <c r="U24" s="62"/>
+      <c r="V24" s="62"/>
+      <c r="W24" s="62"/>
+      <c r="X24" s="62"/>
+      <c r="Y24" s="62"/>
+      <c r="Z24" s="63"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="72"/>
-      <c r="C25" s="64"/>
-      <c r="D25" s="64"/>
-      <c r="E25" s="65"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="64"/>
-      <c r="H25" s="64"/>
-      <c r="I25" s="65"/>
-      <c r="J25" s="63"/>
-      <c r="K25" s="67"/>
-      <c r="L25" s="67"/>
-      <c r="M25" s="68"/>
-      <c r="O25" s="63"/>
-      <c r="P25" s="65"/>
-      <c r="Q25" s="63"/>
-      <c r="R25" s="65"/>
-      <c r="S25" s="63"/>
-      <c r="T25" s="64"/>
-      <c r="U25" s="64"/>
-      <c r="V25" s="64"/>
-      <c r="W25" s="64"/>
-      <c r="X25" s="64"/>
-      <c r="Y25" s="64"/>
-      <c r="Z25" s="65"/>
+      <c r="B25" s="61"/>
+      <c r="C25" s="62"/>
+      <c r="D25" s="62"/>
+      <c r="E25" s="63"/>
+      <c r="F25" s="61"/>
+      <c r="G25" s="62"/>
+      <c r="H25" s="62"/>
+      <c r="I25" s="63"/>
+      <c r="J25" s="61"/>
+      <c r="K25" s="65"/>
+      <c r="L25" s="65"/>
+      <c r="M25" s="66"/>
+      <c r="O25" s="61"/>
+      <c r="P25" s="63"/>
+      <c r="Q25" s="61"/>
+      <c r="R25" s="63"/>
+      <c r="S25" s="61"/>
+      <c r="T25" s="62"/>
+      <c r="U25" s="62"/>
+      <c r="V25" s="62"/>
+      <c r="W25" s="62"/>
+      <c r="X25" s="62"/>
+      <c r="Y25" s="62"/>
+      <c r="Z25" s="63"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="63"/>
-      <c r="C26" s="64"/>
-      <c r="D26" s="64"/>
-      <c r="E26" s="65"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="64"/>
-      <c r="H26" s="64"/>
-      <c r="I26" s="65"/>
-      <c r="J26" s="63"/>
-      <c r="K26" s="64"/>
-      <c r="L26" s="64"/>
-      <c r="M26" s="65"/>
-      <c r="O26" s="63"/>
-      <c r="P26" s="65"/>
-      <c r="Q26" s="63"/>
-      <c r="R26" s="65"/>
-      <c r="S26" s="63"/>
-      <c r="T26" s="64"/>
-      <c r="U26" s="64"/>
-      <c r="V26" s="64"/>
-      <c r="W26" s="64"/>
-      <c r="X26" s="64"/>
-      <c r="Y26" s="64"/>
-      <c r="Z26" s="65"/>
+      <c r="B26" s="61"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="63"/>
+      <c r="F26" s="61"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="63"/>
+      <c r="J26" s="61"/>
+      <c r="K26" s="62"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="63"/>
+      <c r="O26" s="61"/>
+      <c r="P26" s="63"/>
+      <c r="Q26" s="61"/>
+      <c r="R26" s="63"/>
+      <c r="S26" s="61"/>
+      <c r="T26" s="62"/>
+      <c r="U26" s="62"/>
+      <c r="V26" s="62"/>
+      <c r="W26" s="62"/>
+      <c r="X26" s="62"/>
+      <c r="Y26" s="62"/>
+      <c r="Z26" s="63"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="63"/>
-      <c r="C27" s="64"/>
-      <c r="D27" s="64"/>
-      <c r="E27" s="65"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="64"/>
-      <c r="H27" s="64"/>
-      <c r="I27" s="65"/>
-      <c r="J27" s="63"/>
-      <c r="K27" s="64"/>
-      <c r="L27" s="64"/>
-      <c r="M27" s="65"/>
-      <c r="O27" s="63"/>
-      <c r="P27" s="65"/>
-      <c r="Q27" s="63"/>
-      <c r="R27" s="65"/>
-      <c r="S27" s="63"/>
-      <c r="T27" s="64"/>
-      <c r="U27" s="64"/>
-      <c r="V27" s="64"/>
-      <c r="W27" s="64"/>
-      <c r="X27" s="64"/>
-      <c r="Y27" s="64"/>
-      <c r="Z27" s="65"/>
+      <c r="B27" s="61"/>
+      <c r="C27" s="62"/>
+      <c r="D27" s="62"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="62"/>
+      <c r="H27" s="62"/>
+      <c r="I27" s="63"/>
+      <c r="J27" s="61"/>
+      <c r="K27" s="62"/>
+      <c r="L27" s="62"/>
+      <c r="M27" s="63"/>
+      <c r="O27" s="61"/>
+      <c r="P27" s="63"/>
+      <c r="Q27" s="61"/>
+      <c r="R27" s="63"/>
+      <c r="S27" s="61"/>
+      <c r="T27" s="62"/>
+      <c r="U27" s="62"/>
+      <c r="V27" s="62"/>
+      <c r="W27" s="62"/>
+      <c r="X27" s="62"/>
+      <c r="Y27" s="62"/>
+      <c r="Z27" s="63"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="63"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="64"/>
-      <c r="E28" s="65"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="64"/>
-      <c r="H28" s="64"/>
-      <c r="I28" s="65"/>
-      <c r="J28" s="63"/>
-      <c r="K28" s="64"/>
-      <c r="L28" s="64"/>
-      <c r="M28" s="65"/>
-      <c r="O28" s="63"/>
-      <c r="P28" s="65"/>
-      <c r="Q28" s="63"/>
-      <c r="R28" s="65"/>
-      <c r="S28" s="63"/>
-      <c r="T28" s="64"/>
-      <c r="U28" s="64"/>
-      <c r="V28" s="64"/>
-      <c r="W28" s="64"/>
-      <c r="X28" s="64"/>
-      <c r="Y28" s="64"/>
-      <c r="Z28" s="65"/>
+      <c r="B28" s="61"/>
+      <c r="C28" s="62"/>
+      <c r="D28" s="62"/>
+      <c r="E28" s="63"/>
+      <c r="F28" s="61"/>
+      <c r="G28" s="62"/>
+      <c r="H28" s="62"/>
+      <c r="I28" s="63"/>
+      <c r="J28" s="61"/>
+      <c r="K28" s="62"/>
+      <c r="L28" s="62"/>
+      <c r="M28" s="63"/>
+      <c r="O28" s="61"/>
+      <c r="P28" s="63"/>
+      <c r="Q28" s="61"/>
+      <c r="R28" s="63"/>
+      <c r="S28" s="61"/>
+      <c r="T28" s="62"/>
+      <c r="U28" s="62"/>
+      <c r="V28" s="62"/>
+      <c r="W28" s="62"/>
+      <c r="X28" s="62"/>
+      <c r="Y28" s="62"/>
+      <c r="Z28" s="63"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="63"/>
-      <c r="C29" s="64"/>
-      <c r="D29" s="64"/>
-      <c r="E29" s="65"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="64"/>
-      <c r="H29" s="64"/>
-      <c r="I29" s="65"/>
-      <c r="J29" s="63"/>
-      <c r="K29" s="64"/>
-      <c r="L29" s="64"/>
-      <c r="M29" s="65"/>
-      <c r="O29" s="63"/>
-      <c r="P29" s="65"/>
-      <c r="Q29" s="63"/>
-      <c r="R29" s="65"/>
-      <c r="S29" s="63"/>
-      <c r="T29" s="64"/>
-      <c r="U29" s="64"/>
-      <c r="V29" s="64"/>
-      <c r="W29" s="64"/>
-      <c r="X29" s="64"/>
-      <c r="Y29" s="64"/>
-      <c r="Z29" s="65"/>
+      <c r="B29" s="61"/>
+      <c r="C29" s="62"/>
+      <c r="D29" s="62"/>
+      <c r="E29" s="63"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="62"/>
+      <c r="H29" s="62"/>
+      <c r="I29" s="63"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="62"/>
+      <c r="L29" s="62"/>
+      <c r="M29" s="63"/>
+      <c r="O29" s="61"/>
+      <c r="P29" s="63"/>
+      <c r="Q29" s="61"/>
+      <c r="R29" s="63"/>
+      <c r="S29" s="61"/>
+      <c r="T29" s="62"/>
+      <c r="U29" s="62"/>
+      <c r="V29" s="62"/>
+      <c r="W29" s="62"/>
+      <c r="X29" s="62"/>
+      <c r="Y29" s="62"/>
+      <c r="Z29" s="63"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="63"/>
-      <c r="C30" s="64"/>
-      <c r="D30" s="64"/>
-      <c r="E30" s="65"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="64"/>
-      <c r="H30" s="64"/>
-      <c r="I30" s="65"/>
-      <c r="J30" s="63"/>
-      <c r="K30" s="64"/>
-      <c r="L30" s="64"/>
-      <c r="M30" s="65"/>
-      <c r="O30" s="63"/>
-      <c r="P30" s="65"/>
-      <c r="Q30" s="63"/>
-      <c r="R30" s="65"/>
-      <c r="S30" s="63"/>
-      <c r="T30" s="64"/>
-      <c r="U30" s="64"/>
-      <c r="V30" s="64"/>
-      <c r="W30" s="64"/>
-      <c r="X30" s="64"/>
-      <c r="Y30" s="64"/>
-      <c r="Z30" s="65"/>
+      <c r="B30" s="61"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="62"/>
+      <c r="E30" s="63"/>
+      <c r="F30" s="61"/>
+      <c r="G30" s="62"/>
+      <c r="H30" s="62"/>
+      <c r="I30" s="63"/>
+      <c r="J30" s="61"/>
+      <c r="K30" s="62"/>
+      <c r="L30" s="62"/>
+      <c r="M30" s="63"/>
+      <c r="O30" s="61"/>
+      <c r="P30" s="63"/>
+      <c r="Q30" s="61"/>
+      <c r="R30" s="63"/>
+      <c r="S30" s="61"/>
+      <c r="T30" s="62"/>
+      <c r="U30" s="62"/>
+      <c r="V30" s="62"/>
+      <c r="W30" s="62"/>
+      <c r="X30" s="62"/>
+      <c r="Y30" s="62"/>
+      <c r="Z30" s="63"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="63"/>
-      <c r="C31" s="64"/>
-      <c r="D31" s="64"/>
-      <c r="E31" s="65"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="64"/>
-      <c r="H31" s="64"/>
-      <c r="I31" s="65"/>
-      <c r="J31" s="63"/>
-      <c r="K31" s="64"/>
-      <c r="L31" s="64"/>
-      <c r="M31" s="65"/>
-      <c r="O31" s="63"/>
-      <c r="P31" s="65"/>
-      <c r="Q31" s="63"/>
-      <c r="R31" s="65"/>
-      <c r="S31" s="63"/>
-      <c r="T31" s="64"/>
-      <c r="U31" s="64"/>
-      <c r="V31" s="64"/>
-      <c r="W31" s="64"/>
-      <c r="X31" s="64"/>
-      <c r="Y31" s="64"/>
-      <c r="Z31" s="65"/>
+      <c r="B31" s="61"/>
+      <c r="C31" s="62"/>
+      <c r="D31" s="62"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="61"/>
+      <c r="G31" s="62"/>
+      <c r="H31" s="62"/>
+      <c r="I31" s="63"/>
+      <c r="J31" s="61"/>
+      <c r="K31" s="62"/>
+      <c r="L31" s="62"/>
+      <c r="M31" s="63"/>
+      <c r="O31" s="61"/>
+      <c r="P31" s="63"/>
+      <c r="Q31" s="61"/>
+      <c r="R31" s="63"/>
+      <c r="S31" s="61"/>
+      <c r="T31" s="62"/>
+      <c r="U31" s="62"/>
+      <c r="V31" s="62"/>
+      <c r="W31" s="62"/>
+      <c r="X31" s="62"/>
+      <c r="Y31" s="62"/>
+      <c r="Z31" s="63"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="63"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="65"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="65"/>
-      <c r="J32" s="63"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="64"/>
-      <c r="M32" s="65"/>
-      <c r="O32" s="63"/>
-      <c r="P32" s="65"/>
-      <c r="Q32" s="63"/>
-      <c r="R32" s="65"/>
-      <c r="S32" s="63"/>
-      <c r="T32" s="64"/>
-      <c r="U32" s="64"/>
-      <c r="V32" s="64"/>
-      <c r="W32" s="64"/>
-      <c r="X32" s="64"/>
-      <c r="Y32" s="64"/>
-      <c r="Z32" s="65"/>
+      <c r="B32" s="61"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="63"/>
+      <c r="F32" s="61"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="63"/>
+      <c r="J32" s="61"/>
+      <c r="K32" s="62"/>
+      <c r="L32" s="62"/>
+      <c r="M32" s="63"/>
+      <c r="O32" s="61"/>
+      <c r="P32" s="63"/>
+      <c r="Q32" s="61"/>
+      <c r="R32" s="63"/>
+      <c r="S32" s="61"/>
+      <c r="T32" s="62"/>
+      <c r="U32" s="62"/>
+      <c r="V32" s="62"/>
+      <c r="W32" s="62"/>
+      <c r="X32" s="62"/>
+      <c r="Y32" s="62"/>
+      <c r="Z32" s="63"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="63"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="65"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="65"/>
-      <c r="J33" s="63"/>
-      <c r="K33" s="64"/>
-      <c r="L33" s="64"/>
-      <c r="M33" s="65"/>
-      <c r="O33" s="63"/>
-      <c r="P33" s="65"/>
-      <c r="Q33" s="63"/>
-      <c r="R33" s="65"/>
-      <c r="S33" s="63"/>
-      <c r="T33" s="64"/>
-      <c r="U33" s="64"/>
-      <c r="V33" s="64"/>
-      <c r="W33" s="64"/>
-      <c r="X33" s="64"/>
-      <c r="Y33" s="64"/>
-      <c r="Z33" s="65"/>
+      <c r="B33" s="61"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="63"/>
+      <c r="F33" s="61"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="63"/>
+      <c r="J33" s="61"/>
+      <c r="K33" s="62"/>
+      <c r="L33" s="62"/>
+      <c r="M33" s="63"/>
+      <c r="O33" s="61"/>
+      <c r="P33" s="63"/>
+      <c r="Q33" s="61"/>
+      <c r="R33" s="63"/>
+      <c r="S33" s="61"/>
+      <c r="T33" s="62"/>
+      <c r="U33" s="62"/>
+      <c r="V33" s="62"/>
+      <c r="W33" s="62"/>
+      <c r="X33" s="62"/>
+      <c r="Y33" s="62"/>
+      <c r="Z33" s="63"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="63"/>
-      <c r="C34" s="64"/>
-      <c r="D34" s="64"/>
-      <c r="E34" s="65"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="64"/>
-      <c r="H34" s="64"/>
-      <c r="I34" s="65"/>
-      <c r="J34" s="63"/>
-      <c r="K34" s="64"/>
-      <c r="L34" s="64"/>
-      <c r="M34" s="65"/>
-      <c r="O34" s="63"/>
-      <c r="P34" s="65"/>
-      <c r="Q34" s="63"/>
-      <c r="R34" s="65"/>
-      <c r="S34" s="63"/>
-      <c r="T34" s="64"/>
-      <c r="U34" s="64"/>
-      <c r="V34" s="64"/>
-      <c r="W34" s="64"/>
-      <c r="X34" s="64"/>
-      <c r="Y34" s="64"/>
-      <c r="Z34" s="65"/>
+      <c r="B34" s="61"/>
+      <c r="C34" s="62"/>
+      <c r="D34" s="62"/>
+      <c r="E34" s="63"/>
+      <c r="F34" s="61"/>
+      <c r="G34" s="62"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="63"/>
+      <c r="J34" s="61"/>
+      <c r="K34" s="62"/>
+      <c r="L34" s="62"/>
+      <c r="M34" s="63"/>
+      <c r="O34" s="61"/>
+      <c r="P34" s="63"/>
+      <c r="Q34" s="61"/>
+      <c r="R34" s="63"/>
+      <c r="S34" s="61"/>
+      <c r="T34" s="62"/>
+      <c r="U34" s="62"/>
+      <c r="V34" s="62"/>
+      <c r="W34" s="62"/>
+      <c r="X34" s="62"/>
+      <c r="Y34" s="62"/>
+      <c r="Z34" s="63"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="69"/>
-      <c r="C35" s="70"/>
-      <c r="D35" s="70"/>
-      <c r="E35" s="71"/>
-      <c r="F35" s="69"/>
-      <c r="G35" s="70"/>
-      <c r="H35" s="70"/>
-      <c r="I35" s="71"/>
-      <c r="J35" s="69"/>
-      <c r="K35" s="70"/>
-      <c r="L35" s="70"/>
-      <c r="M35" s="71"/>
-      <c r="O35" s="69"/>
-      <c r="P35" s="71"/>
-      <c r="Q35" s="69"/>
-      <c r="R35" s="71"/>
-      <c r="S35" s="69"/>
-      <c r="T35" s="70"/>
-      <c r="U35" s="70"/>
-      <c r="V35" s="70"/>
-      <c r="W35" s="70"/>
-      <c r="X35" s="70"/>
-      <c r="Y35" s="70"/>
-      <c r="Z35" s="71"/>
+      <c r="B35" s="67"/>
+      <c r="C35" s="68"/>
+      <c r="D35" s="68"/>
+      <c r="E35" s="69"/>
+      <c r="F35" s="67"/>
+      <c r="G35" s="68"/>
+      <c r="H35" s="68"/>
+      <c r="I35" s="69"/>
+      <c r="J35" s="67"/>
+      <c r="K35" s="68"/>
+      <c r="L35" s="68"/>
+      <c r="M35" s="69"/>
+      <c r="O35" s="67"/>
+      <c r="P35" s="69"/>
+      <c r="Q35" s="67"/>
+      <c r="R35" s="69"/>
+      <c r="S35" s="67"/>
+      <c r="T35" s="68"/>
+      <c r="U35" s="68"/>
+      <c r="V35" s="68"/>
+      <c r="W35" s="68"/>
+      <c r="X35" s="68"/>
+      <c r="Y35" s="68"/>
+      <c r="Z35" s="69"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="10" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C37" s="10"/>
       <c r="D37" s="10"/>
@@ -4367,12 +4317,12 @@
       <c r="L37" s="10"/>
       <c r="M37" s="10"/>
       <c r="O37" s="44" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="P37" s="44"/>
       <c r="Q37" s="44"/>
       <c r="S37" s="44" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="T37" s="44"/>
       <c r="U37" s="44"/>
@@ -4384,267 +4334,267 @@
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C38" s="13"/>
       <c r="D38" s="13"/>
       <c r="E38" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="F38" s="13"/>
+      <c r="G38" s="70"/>
+      <c r="H38" s="13" t="s">
         <v>109</v>
-      </c>
-      <c r="F38" s="13"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="13" t="s">
-        <v>110</v>
       </c>
       <c r="I38" s="13"/>
       <c r="J38" s="13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K38" s="13"/>
       <c r="L38" s="13"/>
       <c r="M38" s="13"/>
       <c r="O38" s="13" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="P38" s="13"/>
       <c r="Q38" s="13"/>
       <c r="S38" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="T38" s="13"/>
       <c r="U38" s="13"/>
       <c r="V38" s="13"/>
       <c r="W38" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="X38" s="13"/>
       <c r="Y38" s="13"/>
       <c r="Z38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="66"/>
-      <c r="C39" s="67"/>
-      <c r="D39" s="68"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="65"/>
-      <c r="G39" s="64"/>
-      <c r="H39" s="63"/>
-      <c r="I39" s="65"/>
-      <c r="J39" s="64"/>
-      <c r="K39" s="64"/>
-      <c r="L39" s="64"/>
-      <c r="M39" s="65"/>
-      <c r="O39" s="75"/>
-      <c r="P39" s="64"/>
-      <c r="Q39" s="65"/>
-      <c r="S39" s="63"/>
-      <c r="T39" s="64"/>
-      <c r="U39" s="64"/>
-      <c r="V39" s="65"/>
-      <c r="W39" s="66"/>
-      <c r="X39" s="67"/>
-      <c r="Y39" s="67"/>
-      <c r="Z39" s="68"/>
+      <c r="B39" s="64"/>
+      <c r="C39" s="65"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="61"/>
+      <c r="F39" s="63"/>
+      <c r="G39" s="62"/>
+      <c r="H39" s="61"/>
+      <c r="I39" s="63"/>
+      <c r="J39" s="62"/>
+      <c r="K39" s="62"/>
+      <c r="L39" s="62"/>
+      <c r="M39" s="63"/>
+      <c r="O39" s="71"/>
+      <c r="P39" s="62"/>
+      <c r="Q39" s="63"/>
+      <c r="S39" s="61"/>
+      <c r="T39" s="62"/>
+      <c r="U39" s="62"/>
+      <c r="V39" s="63"/>
+      <c r="W39" s="64"/>
+      <c r="X39" s="65"/>
+      <c r="Y39" s="65"/>
+      <c r="Z39" s="66"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="63"/>
-      <c r="C40" s="64"/>
-      <c r="D40" s="65"/>
-      <c r="E40" s="63"/>
-      <c r="F40" s="65"/>
-      <c r="G40" s="64"/>
-      <c r="H40" s="63"/>
-      <c r="I40" s="65"/>
-      <c r="J40" s="64"/>
-      <c r="K40" s="64"/>
-      <c r="L40" s="64"/>
-      <c r="M40" s="65"/>
-      <c r="O40" s="63"/>
-      <c r="P40" s="64"/>
-      <c r="Q40" s="65"/>
-      <c r="S40" s="63"/>
-      <c r="T40" s="64"/>
-      <c r="U40" s="64"/>
-      <c r="V40" s="65"/>
-      <c r="W40" s="63"/>
-      <c r="X40" s="64"/>
-      <c r="Y40" s="64"/>
-      <c r="Z40" s="65"/>
+      <c r="B40" s="61"/>
+      <c r="C40" s="62"/>
+      <c r="D40" s="63"/>
+      <c r="E40" s="61"/>
+      <c r="F40" s="63"/>
+      <c r="G40" s="62"/>
+      <c r="H40" s="61"/>
+      <c r="I40" s="63"/>
+      <c r="J40" s="62"/>
+      <c r="K40" s="62"/>
+      <c r="L40" s="62"/>
+      <c r="M40" s="63"/>
+      <c r="O40" s="61"/>
+      <c r="P40" s="62"/>
+      <c r="Q40" s="63"/>
+      <c r="S40" s="61"/>
+      <c r="T40" s="62"/>
+      <c r="U40" s="62"/>
+      <c r="V40" s="63"/>
+      <c r="W40" s="61"/>
+      <c r="X40" s="62"/>
+      <c r="Y40" s="62"/>
+      <c r="Z40" s="63"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="63"/>
-      <c r="C41" s="64"/>
-      <c r="D41" s="65"/>
-      <c r="E41" s="63"/>
-      <c r="F41" s="65"/>
-      <c r="G41" s="64"/>
-      <c r="H41" s="63"/>
-      <c r="I41" s="65"/>
-      <c r="J41" s="64"/>
-      <c r="K41" s="64"/>
-      <c r="L41" s="64"/>
-      <c r="M41" s="65"/>
-      <c r="O41" s="63"/>
-      <c r="P41" s="64"/>
-      <c r="Q41" s="65"/>
-      <c r="S41" s="63"/>
-      <c r="T41" s="64"/>
-      <c r="U41" s="64"/>
-      <c r="V41" s="65"/>
-      <c r="W41" s="63"/>
-      <c r="X41" s="64"/>
-      <c r="Y41" s="64"/>
-      <c r="Z41" s="65"/>
+      <c r="B41" s="61"/>
+      <c r="C41" s="62"/>
+      <c r="D41" s="63"/>
+      <c r="E41" s="61"/>
+      <c r="F41" s="63"/>
+      <c r="G41" s="62"/>
+      <c r="H41" s="61"/>
+      <c r="I41" s="63"/>
+      <c r="J41" s="62"/>
+      <c r="K41" s="62"/>
+      <c r="L41" s="62"/>
+      <c r="M41" s="63"/>
+      <c r="O41" s="61"/>
+      <c r="P41" s="62"/>
+      <c r="Q41" s="63"/>
+      <c r="S41" s="61"/>
+      <c r="T41" s="62"/>
+      <c r="U41" s="62"/>
+      <c r="V41" s="63"/>
+      <c r="W41" s="61"/>
+      <c r="X41" s="62"/>
+      <c r="Y41" s="62"/>
+      <c r="Z41" s="63"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="63"/>
-      <c r="C42" s="64"/>
-      <c r="D42" s="65"/>
-      <c r="E42" s="63"/>
-      <c r="F42" s="65"/>
-      <c r="G42" s="64"/>
-      <c r="H42" s="63"/>
-      <c r="I42" s="65"/>
-      <c r="J42" s="64"/>
-      <c r="K42" s="64"/>
-      <c r="L42" s="64"/>
-      <c r="M42" s="65"/>
-      <c r="O42" s="63"/>
-      <c r="P42" s="64"/>
-      <c r="Q42" s="65"/>
-      <c r="S42" s="63"/>
-      <c r="T42" s="64"/>
-      <c r="U42" s="64"/>
-      <c r="V42" s="65"/>
-      <c r="W42" s="63"/>
-      <c r="X42" s="64"/>
-      <c r="Y42" s="64"/>
-      <c r="Z42" s="65"/>
+      <c r="B42" s="61"/>
+      <c r="C42" s="62"/>
+      <c r="D42" s="63"/>
+      <c r="E42" s="61"/>
+      <c r="F42" s="63"/>
+      <c r="G42" s="62"/>
+      <c r="H42" s="61"/>
+      <c r="I42" s="63"/>
+      <c r="J42" s="62"/>
+      <c r="K42" s="62"/>
+      <c r="L42" s="62"/>
+      <c r="M42" s="63"/>
+      <c r="O42" s="61"/>
+      <c r="P42" s="62"/>
+      <c r="Q42" s="63"/>
+      <c r="S42" s="61"/>
+      <c r="T42" s="62"/>
+      <c r="U42" s="62"/>
+      <c r="V42" s="63"/>
+      <c r="W42" s="61"/>
+      <c r="X42" s="62"/>
+      <c r="Y42" s="62"/>
+      <c r="Z42" s="63"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="63"/>
-      <c r="C43" s="64"/>
-      <c r="D43" s="65"/>
-      <c r="E43" s="63"/>
-      <c r="F43" s="65"/>
-      <c r="G43" s="64"/>
-      <c r="H43" s="63"/>
-      <c r="I43" s="65"/>
-      <c r="J43" s="64"/>
-      <c r="K43" s="64"/>
-      <c r="L43" s="64"/>
-      <c r="M43" s="65"/>
-      <c r="O43" s="63"/>
-      <c r="P43" s="64"/>
-      <c r="Q43" s="65"/>
-      <c r="S43" s="63"/>
-      <c r="T43" s="64"/>
-      <c r="U43" s="64"/>
-      <c r="V43" s="65"/>
-      <c r="W43" s="63"/>
-      <c r="X43" s="64"/>
-      <c r="Y43" s="64"/>
-      <c r="Z43" s="65"/>
+      <c r="B43" s="61"/>
+      <c r="C43" s="62"/>
+      <c r="D43" s="63"/>
+      <c r="E43" s="61"/>
+      <c r="F43" s="63"/>
+      <c r="G43" s="62"/>
+      <c r="H43" s="61"/>
+      <c r="I43" s="63"/>
+      <c r="J43" s="62"/>
+      <c r="K43" s="62"/>
+      <c r="L43" s="62"/>
+      <c r="M43" s="63"/>
+      <c r="O43" s="61"/>
+      <c r="P43" s="62"/>
+      <c r="Q43" s="63"/>
+      <c r="S43" s="61"/>
+      <c r="T43" s="62"/>
+      <c r="U43" s="62"/>
+      <c r="V43" s="63"/>
+      <c r="W43" s="61"/>
+      <c r="X43" s="62"/>
+      <c r="Y43" s="62"/>
+      <c r="Z43" s="63"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="63"/>
-      <c r="C44" s="64"/>
-      <c r="D44" s="65"/>
-      <c r="E44" s="63"/>
-      <c r="F44" s="65"/>
-      <c r="G44" s="64"/>
-      <c r="H44" s="63"/>
-      <c r="I44" s="65"/>
-      <c r="J44" s="64"/>
-      <c r="K44" s="64"/>
-      <c r="L44" s="64"/>
-      <c r="M44" s="65"/>
-      <c r="O44" s="63"/>
-      <c r="P44" s="64"/>
-      <c r="Q44" s="65"/>
-      <c r="S44" s="63"/>
-      <c r="T44" s="64"/>
-      <c r="U44" s="64"/>
-      <c r="V44" s="65"/>
-      <c r="W44" s="63"/>
-      <c r="X44" s="64"/>
-      <c r="Y44" s="64"/>
-      <c r="Z44" s="65"/>
+      <c r="B44" s="61"/>
+      <c r="C44" s="62"/>
+      <c r="D44" s="63"/>
+      <c r="E44" s="61"/>
+      <c r="F44" s="63"/>
+      <c r="G44" s="62"/>
+      <c r="H44" s="61"/>
+      <c r="I44" s="63"/>
+      <c r="J44" s="62"/>
+      <c r="K44" s="62"/>
+      <c r="L44" s="62"/>
+      <c r="M44" s="63"/>
+      <c r="O44" s="61"/>
+      <c r="P44" s="62"/>
+      <c r="Q44" s="63"/>
+      <c r="S44" s="61"/>
+      <c r="T44" s="62"/>
+      <c r="U44" s="62"/>
+      <c r="V44" s="63"/>
+      <c r="W44" s="61"/>
+      <c r="X44" s="62"/>
+      <c r="Y44" s="62"/>
+      <c r="Z44" s="63"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="63"/>
-      <c r="C45" s="64"/>
-      <c r="D45" s="65"/>
-      <c r="E45" s="63"/>
-      <c r="F45" s="65"/>
-      <c r="G45" s="64"/>
-      <c r="H45" s="63"/>
-      <c r="I45" s="65"/>
-      <c r="J45" s="64"/>
-      <c r="K45" s="64"/>
-      <c r="L45" s="64"/>
-      <c r="M45" s="65"/>
-      <c r="O45" s="63"/>
-      <c r="P45" s="64"/>
-      <c r="Q45" s="65"/>
-      <c r="S45" s="63"/>
-      <c r="T45" s="64"/>
-      <c r="U45" s="64"/>
-      <c r="V45" s="65"/>
-      <c r="W45" s="63"/>
-      <c r="X45" s="64"/>
-      <c r="Y45" s="64"/>
-      <c r="Z45" s="65"/>
+      <c r="B45" s="61"/>
+      <c r="C45" s="62"/>
+      <c r="D45" s="63"/>
+      <c r="E45" s="61"/>
+      <c r="F45" s="63"/>
+      <c r="G45" s="62"/>
+      <c r="H45" s="61"/>
+      <c r="I45" s="63"/>
+      <c r="J45" s="62"/>
+      <c r="K45" s="62"/>
+      <c r="L45" s="62"/>
+      <c r="M45" s="63"/>
+      <c r="O45" s="61"/>
+      <c r="P45" s="62"/>
+      <c r="Q45" s="63"/>
+      <c r="S45" s="61"/>
+      <c r="T45" s="62"/>
+      <c r="U45" s="62"/>
+      <c r="V45" s="63"/>
+      <c r="W45" s="61"/>
+      <c r="X45" s="62"/>
+      <c r="Y45" s="62"/>
+      <c r="Z45" s="63"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="63"/>
-      <c r="C46" s="64"/>
-      <c r="D46" s="65"/>
-      <c r="E46" s="63"/>
-      <c r="F46" s="65"/>
-      <c r="G46" s="64"/>
-      <c r="H46" s="63"/>
-      <c r="I46" s="65"/>
-      <c r="J46" s="64"/>
-      <c r="K46" s="64"/>
-      <c r="L46" s="64"/>
-      <c r="M46" s="65"/>
-      <c r="O46" s="63"/>
-      <c r="P46" s="64"/>
-      <c r="Q46" s="65"/>
-      <c r="S46" s="63"/>
-      <c r="T46" s="64"/>
-      <c r="U46" s="64"/>
-      <c r="V46" s="65"/>
-      <c r="W46" s="63"/>
-      <c r="X46" s="64"/>
-      <c r="Y46" s="64"/>
-      <c r="Z46" s="65"/>
+      <c r="B46" s="61"/>
+      <c r="C46" s="62"/>
+      <c r="D46" s="63"/>
+      <c r="E46" s="61"/>
+      <c r="F46" s="63"/>
+      <c r="G46" s="62"/>
+      <c r="H46" s="61"/>
+      <c r="I46" s="63"/>
+      <c r="J46" s="62"/>
+      <c r="K46" s="62"/>
+      <c r="L46" s="62"/>
+      <c r="M46" s="63"/>
+      <c r="O46" s="61"/>
+      <c r="P46" s="62"/>
+      <c r="Q46" s="63"/>
+      <c r="S46" s="61"/>
+      <c r="T46" s="62"/>
+      <c r="U46" s="62"/>
+      <c r="V46" s="63"/>
+      <c r="W46" s="61"/>
+      <c r="X46" s="62"/>
+      <c r="Y46" s="62"/>
+      <c r="Z46" s="63"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="69"/>
-      <c r="C47" s="70"/>
-      <c r="D47" s="71"/>
-      <c r="E47" s="69"/>
-      <c r="F47" s="71"/>
-      <c r="G47" s="70"/>
-      <c r="H47" s="69"/>
-      <c r="I47" s="71"/>
-      <c r="J47" s="70"/>
-      <c r="K47" s="70"/>
-      <c r="L47" s="70"/>
-      <c r="M47" s="71"/>
-      <c r="O47" s="69"/>
-      <c r="P47" s="70"/>
-      <c r="Q47" s="71"/>
-      <c r="S47" s="69"/>
-      <c r="T47" s="70"/>
-      <c r="U47" s="70"/>
-      <c r="V47" s="71"/>
-      <c r="W47" s="69"/>
-      <c r="X47" s="70"/>
-      <c r="Y47" s="70"/>
-      <c r="Z47" s="71"/>
+      <c r="B47" s="67"/>
+      <c r="C47" s="68"/>
+      <c r="D47" s="69"/>
+      <c r="E47" s="67"/>
+      <c r="F47" s="69"/>
+      <c r="G47" s="68"/>
+      <c r="H47" s="67"/>
+      <c r="I47" s="69"/>
+      <c r="J47" s="68"/>
+      <c r="K47" s="68"/>
+      <c r="L47" s="68"/>
+      <c r="M47" s="69"/>
+      <c r="O47" s="67"/>
+      <c r="P47" s="68"/>
+      <c r="Q47" s="69"/>
+      <c r="S47" s="67"/>
+      <c r="T47" s="68"/>
+      <c r="U47" s="68"/>
+      <c r="V47" s="69"/>
+      <c r="W47" s="67"/>
+      <c r="X47" s="68"/>
+      <c r="Y47" s="68"/>
+      <c r="Z47" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -4688,43 +4638,43 @@
   </sheetPr>
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="18.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="65" width="0.28"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="0" width="1.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="60" width="18.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="60" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="63" width="0.28"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="60" width="1.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="76" t="s">
+      <c r="A1" s="72" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="11" t="s">
         <v>113</v>
-      </c>
-      <c r="B1" s="76"/>
-      <c r="C1" s="76"/>
-      <c r="D1" s="76"/>
-      <c r="E1" s="76"/>
-      <c r="F1" s="76"/>
-      <c r="G1" s="76"/>
-      <c r="H1" s="76"/>
-      <c r="I1" s="76"/>
-      <c r="J1" s="76"/>
-      <c r="K1" s="76"/>
-      <c r="L1" s="76"/>
-      <c r="M1" s="76"/>
-      <c r="N1" s="76"/>
-      <c r="O1" s="76"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
-      <c r="R1" s="76"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -4738,20 +4688,20 @@
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
-      <c r="N2" s="77"/>
-      <c r="O2" s="77"/>
-      <c r="P2" s="77"/>
-      <c r="Q2" s="78"/>
-      <c r="R2" s="68"/>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="79" t="s">
-        <v>115</v>
+      <c r="N2" s="73"/>
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="74"/>
+      <c r="R2" s="66"/>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="75" t="s">
+        <v>114</v>
       </c>
       <c r="B3" s="17"/>
-      <c r="C3" s="80"/>
-      <c r="D3" s="77"/>
-      <c r="E3" s="80"/>
+      <c r="C3" s="76"/>
+      <c r="D3" s="73"/>
+      <c r="E3" s="76"/>
       <c r="F3" s="17"/>
       <c r="G3" s="17"/>
       <c r="H3" s="17"/>
@@ -4763,17 +4713,17 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
-      <c r="Q3" s="81"/>
-      <c r="R3" s="65"/>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="82" t="s">
-        <v>116</v>
+      <c r="Q3" s="77"/>
+      <c r="R3" s="63"/>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="78" t="s">
+        <v>115</v>
       </c>
       <c r="B4" s="17"/>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="76"/>
+      <c r="E4" s="76"/>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
@@ -4785,15 +4735,15 @@
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
-      <c r="Q4" s="81"/>
-      <c r="R4" s="65"/>
-      <c r="S4" s="64"/>
-    </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="82"/>
-      <c r="B5" s="80"/>
-      <c r="C5" s="80"/>
-      <c r="D5" s="80"/>
+      <c r="Q4" s="77"/>
+      <c r="R4" s="63"/>
+      <c r="S4" s="62"/>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="78"/>
+      <c r="B5" s="76"/>
+      <c r="C5" s="76"/>
+      <c r="D5" s="76"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -4806,14 +4756,14 @@
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
-      <c r="Q5" s="81"/>
-      <c r="R5" s="65"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="82"/>
-      <c r="B6" s="80"/>
-      <c r="C6" s="80"/>
-      <c r="D6" s="80"/>
+      <c r="Q5" s="77"/>
+      <c r="R5" s="63"/>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="78"/>
+      <c r="B6" s="76"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="76"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -4826,11 +4776,11 @@
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
-      <c r="Q6" s="81"/>
-      <c r="R6" s="65"/>
+      <c r="Q6" s="77"/>
+      <c r="R6" s="63"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="82"/>
+      <c r="A7" s="78"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
@@ -4846,11 +4796,11 @@
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
       <c r="P7" s="17"/>
-      <c r="Q7" s="81"/>
-      <c r="R7" s="65"/>
+      <c r="Q7" s="77"/>
+      <c r="R7" s="63"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="82"/>
+      <c r="A8" s="78"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
@@ -4866,11 +4816,11 @@
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
-      <c r="Q8" s="81"/>
-      <c r="R8" s="65"/>
+      <c r="Q8" s="77"/>
+      <c r="R8" s="63"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="82"/>
+      <c r="A9" s="78"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
@@ -4886,11 +4836,11 @@
       <c r="N9" s="17"/>
       <c r="O9" s="17"/>
       <c r="P9" s="17"/>
-      <c r="Q9" s="81"/>
-      <c r="R9" s="65"/>
+      <c r="Q9" s="77"/>
+      <c r="R9" s="63"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="82"/>
+      <c r="A10" s="78"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -4906,11 +4856,11 @@
       <c r="N10" s="17"/>
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
-      <c r="Q10" s="81"/>
-      <c r="R10" s="65"/>
+      <c r="Q10" s="77"/>
+      <c r="R10" s="63"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="82"/>
+      <c r="A11" s="78"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -4926,11 +4876,11 @@
       <c r="N11" s="17"/>
       <c r="O11" s="17"/>
       <c r="P11" s="17"/>
-      <c r="Q11" s="81"/>
-      <c r="R11" s="65"/>
+      <c r="Q11" s="77"/>
+      <c r="R11" s="63"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="82"/>
+      <c r="A12" s="78"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -4946,11 +4896,11 @@
       <c r="N12" s="17"/>
       <c r="O12" s="17"/>
       <c r="P12" s="17"/>
-      <c r="Q12" s="81"/>
-      <c r="R12" s="65"/>
+      <c r="Q12" s="77"/>
+      <c r="R12" s="63"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="82"/>
+      <c r="A13" s="78"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -4966,11 +4916,11 @@
       <c r="N13" s="17"/>
       <c r="O13" s="17"/>
       <c r="P13" s="17"/>
-      <c r="Q13" s="81"/>
-      <c r="R13" s="65"/>
+      <c r="Q13" s="77"/>
+      <c r="R13" s="63"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="82"/>
+      <c r="A14" s="78"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -4986,11 +4936,11 @@
       <c r="N14" s="17"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
-      <c r="Q14" s="81"/>
-      <c r="R14" s="65"/>
+      <c r="Q14" s="77"/>
+      <c r="R14" s="63"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="82"/>
+      <c r="A15" s="78"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -5006,11 +4956,11 @@
       <c r="N15" s="17"/>
       <c r="O15" s="17"/>
       <c r="P15" s="17"/>
-      <c r="Q15" s="81"/>
-      <c r="R15" s="65"/>
+      <c r="Q15" s="77"/>
+      <c r="R15" s="63"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="82"/>
+      <c r="A16" s="78"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -5026,11 +4976,11 @@
       <c r="N16" s="17"/>
       <c r="O16" s="17"/>
       <c r="P16" s="17"/>
-      <c r="Q16" s="81"/>
-      <c r="R16" s="65"/>
+      <c r="Q16" s="77"/>
+      <c r="R16" s="63"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="82"/>
+      <c r="A17" s="78"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -5046,11 +4996,11 @@
       <c r="N17" s="17"/>
       <c r="O17" s="17"/>
       <c r="P17" s="17"/>
-      <c r="Q17" s="81"/>
-      <c r="R17" s="65"/>
+      <c r="Q17" s="77"/>
+      <c r="R17" s="63"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="82"/>
+      <c r="A18" s="78"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -5066,11 +5016,11 @@
       <c r="N18" s="17"/>
       <c r="O18" s="17"/>
       <c r="P18" s="17"/>
-      <c r="Q18" s="81"/>
-      <c r="R18" s="65"/>
+      <c r="Q18" s="77"/>
+      <c r="R18" s="63"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="82"/>
+      <c r="A19" s="78"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -5086,11 +5036,11 @@
       <c r="N19" s="17"/>
       <c r="O19" s="17"/>
       <c r="P19" s="17"/>
-      <c r="Q19" s="81"/>
-      <c r="R19" s="65"/>
+      <c r="Q19" s="77"/>
+      <c r="R19" s="63"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="82"/>
+      <c r="A20" s="78"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -5106,11 +5056,11 @@
       <c r="N20" s="17"/>
       <c r="O20" s="17"/>
       <c r="P20" s="17"/>
-      <c r="Q20" s="81"/>
-      <c r="R20" s="65"/>
+      <c r="Q20" s="77"/>
+      <c r="R20" s="63"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="82"/>
+      <c r="A21" s="78"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -5126,11 +5076,11 @@
       <c r="N21" s="17"/>
       <c r="O21" s="17"/>
       <c r="P21" s="17"/>
-      <c r="Q21" s="81"/>
-      <c r="R21" s="65"/>
+      <c r="Q21" s="77"/>
+      <c r="R21" s="63"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="82"/>
+      <c r="A22" s="78"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -5146,11 +5096,11 @@
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
-      <c r="Q22" s="81"/>
-      <c r="R22" s="65"/>
+      <c r="Q22" s="77"/>
+      <c r="R22" s="63"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="82"/>
+      <c r="A23" s="78"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -5166,11 +5116,11 @@
       <c r="N23" s="17"/>
       <c r="O23" s="17"/>
       <c r="P23" s="17"/>
-      <c r="Q23" s="81"/>
-      <c r="R23" s="65"/>
+      <c r="Q23" s="77"/>
+      <c r="R23" s="63"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="82"/>
+      <c r="A24" s="78"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -5186,11 +5136,11 @@
       <c r="N24" s="17"/>
       <c r="O24" s="17"/>
       <c r="P24" s="17"/>
-      <c r="Q24" s="81"/>
-      <c r="R24" s="65"/>
+      <c r="Q24" s="77"/>
+      <c r="R24" s="63"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="82"/>
+      <c r="A25" s="78"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -5206,11 +5156,11 @@
       <c r="N25" s="17"/>
       <c r="O25" s="17"/>
       <c r="P25" s="17"/>
-      <c r="Q25" s="81"/>
-      <c r="R25" s="65"/>
+      <c r="Q25" s="77"/>
+      <c r="R25" s="63"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="82"/>
+      <c r="A26" s="78"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -5226,11 +5176,11 @@
       <c r="N26" s="17"/>
       <c r="O26" s="17"/>
       <c r="P26" s="17"/>
-      <c r="Q26" s="81"/>
-      <c r="R26" s="65"/>
+      <c r="Q26" s="77"/>
+      <c r="R26" s="63"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="82"/>
+      <c r="A27" s="78"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -5246,11 +5196,11 @@
       <c r="N27" s="17"/>
       <c r="O27" s="17"/>
       <c r="P27" s="17"/>
-      <c r="Q27" s="81"/>
-      <c r="R27" s="65"/>
+      <c r="Q27" s="77"/>
+      <c r="R27" s="63"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="82"/>
+      <c r="A28" s="78"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -5266,11 +5216,11 @@
       <c r="N28" s="17"/>
       <c r="O28" s="17"/>
       <c r="P28" s="17"/>
-      <c r="Q28" s="81"/>
-      <c r="R28" s="65"/>
+      <c r="Q28" s="77"/>
+      <c r="R28" s="63"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="82"/>
+      <c r="A29" s="78"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -5286,11 +5236,11 @@
       <c r="N29" s="17"/>
       <c r="O29" s="17"/>
       <c r="P29" s="17"/>
-      <c r="Q29" s="81"/>
-      <c r="R29" s="65"/>
+      <c r="Q29" s="77"/>
+      <c r="R29" s="63"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="82"/>
+      <c r="A30" s="78"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -5306,11 +5256,11 @@
       <c r="N30" s="17"/>
       <c r="O30" s="17"/>
       <c r="P30" s="17"/>
-      <c r="Q30" s="81"/>
-      <c r="R30" s="65"/>
+      <c r="Q30" s="77"/>
+      <c r="R30" s="63"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="82"/>
+      <c r="A31" s="78"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -5326,66 +5276,66 @@
       <c r="N31" s="17"/>
       <c r="O31" s="17"/>
       <c r="P31" s="17"/>
-      <c r="Q31" s="81"/>
-      <c r="R31" s="65"/>
+      <c r="Q31" s="77"/>
+      <c r="R31" s="63"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="63"/>
-      <c r="B32" s="64"/>
-      <c r="C32" s="64"/>
-      <c r="D32" s="64"/>
-      <c r="E32" s="64"/>
-      <c r="F32" s="64"/>
-      <c r="G32" s="64"/>
-      <c r="H32" s="64"/>
-      <c r="I32" s="64"/>
-      <c r="J32" s="64"/>
-      <c r="K32" s="64"/>
-      <c r="L32" s="64"/>
-      <c r="M32" s="64"/>
-      <c r="N32" s="64"/>
-      <c r="O32" s="64"/>
-      <c r="P32" s="64"/>
-      <c r="R32" s="65"/>
+      <c r="A32" s="61"/>
+      <c r="B32" s="62"/>
+      <c r="C32" s="62"/>
+      <c r="D32" s="62"/>
+      <c r="E32" s="62"/>
+      <c r="F32" s="62"/>
+      <c r="G32" s="62"/>
+      <c r="H32" s="62"/>
+      <c r="I32" s="62"/>
+      <c r="J32" s="62"/>
+      <c r="K32" s="62"/>
+      <c r="L32" s="62"/>
+      <c r="M32" s="62"/>
+      <c r="N32" s="62"/>
+      <c r="O32" s="62"/>
+      <c r="P32" s="62"/>
+      <c r="R32" s="63"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="63"/>
-      <c r="B33" s="64"/>
-      <c r="C33" s="64"/>
-      <c r="D33" s="64"/>
-      <c r="E33" s="64"/>
-      <c r="F33" s="64"/>
-      <c r="G33" s="64"/>
-      <c r="H33" s="64"/>
-      <c r="I33" s="64"/>
-      <c r="J33" s="64"/>
-      <c r="K33" s="64"/>
-      <c r="L33" s="64"/>
-      <c r="M33" s="64"/>
-      <c r="N33" s="64"/>
-      <c r="O33" s="64"/>
-      <c r="P33" s="64"/>
-      <c r="R33" s="65"/>
+      <c r="A33" s="61"/>
+      <c r="B33" s="62"/>
+      <c r="C33" s="62"/>
+      <c r="D33" s="62"/>
+      <c r="E33" s="62"/>
+      <c r="F33" s="62"/>
+      <c r="G33" s="62"/>
+      <c r="H33" s="62"/>
+      <c r="I33" s="62"/>
+      <c r="J33" s="62"/>
+      <c r="K33" s="62"/>
+      <c r="L33" s="62"/>
+      <c r="M33" s="62"/>
+      <c r="N33" s="62"/>
+      <c r="O33" s="62"/>
+      <c r="P33" s="62"/>
+      <c r="R33" s="63"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="69"/>
-      <c r="B34" s="70"/>
-      <c r="C34" s="70"/>
-      <c r="D34" s="70"/>
-      <c r="E34" s="70"/>
-      <c r="F34" s="70"/>
-      <c r="G34" s="70"/>
-      <c r="H34" s="70"/>
-      <c r="I34" s="70"/>
-      <c r="J34" s="70"/>
-      <c r="K34" s="70"/>
-      <c r="L34" s="70"/>
-      <c r="M34" s="70"/>
-      <c r="N34" s="70"/>
-      <c r="O34" s="70"/>
-      <c r="P34" s="70"/>
-      <c r="Q34" s="71"/>
-      <c r="R34" s="71"/>
+      <c r="A34" s="67"/>
+      <c r="B34" s="68"/>
+      <c r="C34" s="68"/>
+      <c r="D34" s="68"/>
+      <c r="E34" s="68"/>
+      <c r="F34" s="68"/>
+      <c r="G34" s="68"/>
+      <c r="H34" s="68"/>
+      <c r="I34" s="68"/>
+      <c r="J34" s="68"/>
+      <c r="K34" s="68"/>
+      <c r="L34" s="68"/>
+      <c r="M34" s="68"/>
+      <c r="N34" s="68"/>
+      <c r="O34" s="68"/>
+      <c r="P34" s="68"/>
+      <c r="Q34" s="69"/>
+      <c r="R34" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>

<commit_message>
feat: ficha funcional pagina final feita
</commit_message>
<xml_diff>
--- a/FICHA_FUNCIONAL_TEMPLATE.xlsx
+++ b/FICHA_FUNCIONAL_TEMPLATE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FRENTE" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="119">
   <si>
     <t xml:space="preserve">GOVERNO DO ESTADO DO AMAZONAS</t>
   </si>
@@ -364,7 +364,10 @@
     <t xml:space="preserve">SEJUSC        -        OUTRAS ANOTAÇÕES</t>
   </si>
   <si>
-    <t xml:space="preserve">NATHALIA MAISA ALENCAR DE ARAUJO</t>
+    <t xml:space="preserve">DOE PUBLICADO EM </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CAMPO_DATA</t>
   </si>
   <si>
     <r>
@@ -373,20 +376,28 @@
         <sz val="12"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">DOE PUBLICADO EM 14 DE FEVEREIRO DE 2025 - </t>
+      <t xml:space="preserve">- </t>
     </r>
     <r>
       <rPr>
         <sz val="12"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">NOMEAR, a contar de 15 de fevereiro de 2025, para exercer o cargo de provimento em comissão, </t>
+      <t xml:space="preserve">NOMEAR, a contar de</t>
     </r>
   </si>
   <si>
-    <t xml:space="preserve">de ASESSOR III AD-3 da Secretaria de Estado de Justiça, Direitos Humanos e Cidadania.</t>
+    <t xml:space="preserve">, para exercer o cargo de provimento em comissão</t>
+  </si>
+  <si>
+    <t xml:space="preserve">de</t>
+  </si>
+  <si>
+    <t xml:space="preserve">da Secretaria de Estado de Justiça, Direitos Humanos e Cidadania.</t>
   </si>
 </sst>
 </file>
@@ -405,6 +416,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -425,52 +437,61 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="24"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="14"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="9"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="28"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -613,7 +634,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="81">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -915,6 +936,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -953,9 +982,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>835920</xdr:colOff>
+      <xdr:colOff>834120</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>123840</xdr:rowOff>
+      <xdr:rowOff>122040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -968,8 +997,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="894240" y="847440"/>
-          <a:ext cx="1187640" cy="1569960"/>
+          <a:off x="893520" y="847440"/>
+          <a:ext cx="1185840" cy="1568160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1097,7 +1126,7 @@
   </sheetPr>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="AE50" activeCellId="0" sqref="AE50"/>
     </sheetView>
   </sheetViews>
@@ -4638,13 +4667,15 @@
   </sheetPr>
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="60" width="18.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="60" width="14.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="60" width="29.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="60" width="20.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="60" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="63" width="0.28"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="60" width="1.7"/>
@@ -4674,7 +4705,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>113</v>
+        <v>13</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -4696,16 +4727,24 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="75" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="75"/>
+      <c r="C3" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="B3" s="17"/>
-      <c r="C3" s="76"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="17"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="17"/>
-      <c r="I3" s="17"/>
+      <c r="D3" s="77" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="77"/>
+      <c r="F3" s="77"/>
+      <c r="G3" s="78" t="s">
+        <v>114</v>
+      </c>
+      <c r="H3" s="78"/>
+      <c r="I3" s="17" t="s">
+        <v>116</v>
+      </c>
       <c r="J3" s="17"/>
       <c r="K3" s="17"/>
       <c r="L3" s="17"/>
@@ -4713,17 +4752,21 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
-      <c r="Q3" s="77"/>
+      <c r="Q3" s="79"/>
       <c r="R3" s="63"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="78" t="s">
-        <v>115</v>
-      </c>
-      <c r="B4" s="17"/>
-      <c r="C4" s="76"/>
-      <c r="D4" s="76"/>
-      <c r="E4" s="76"/>
+      <c r="A4" s="80" t="s">
+        <v>117</v>
+      </c>
+      <c r="B4" s="17" t="s">
+        <v>74</v>
+      </c>
+      <c r="C4" s="17"/>
+      <c r="D4" s="17" t="s">
+        <v>118</v>
+      </c>
+      <c r="E4" s="17"/>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
@@ -4735,15 +4778,15 @@
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
-      <c r="Q4" s="77"/>
+      <c r="Q4" s="79"/>
       <c r="R4" s="63"/>
       <c r="S4" s="62"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="78"/>
-      <c r="B5" s="76"/>
-      <c r="C5" s="76"/>
-      <c r="D5" s="76"/>
+      <c r="A5" s="80"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="78"/>
+      <c r="D5" s="78"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -4756,14 +4799,14 @@
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
-      <c r="Q5" s="77"/>
+      <c r="Q5" s="79"/>
       <c r="R5" s="63"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="78"/>
-      <c r="B6" s="76"/>
-      <c r="C6" s="76"/>
-      <c r="D6" s="76"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="78"/>
+      <c r="D6" s="78"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -4776,11 +4819,11 @@
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
-      <c r="Q6" s="77"/>
+      <c r="Q6" s="79"/>
       <c r="R6" s="63"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="78"/>
+      <c r="A7" s="80"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
@@ -4796,11 +4839,11 @@
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
       <c r="P7" s="17"/>
-      <c r="Q7" s="77"/>
+      <c r="Q7" s="79"/>
       <c r="R7" s="63"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="78"/>
+      <c r="A8" s="80"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
@@ -4816,11 +4859,11 @@
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
-      <c r="Q8" s="77"/>
+      <c r="Q8" s="79"/>
       <c r="R8" s="63"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="78"/>
+      <c r="A9" s="80"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
@@ -4836,11 +4879,11 @@
       <c r="N9" s="17"/>
       <c r="O9" s="17"/>
       <c r="P9" s="17"/>
-      <c r="Q9" s="77"/>
+      <c r="Q9" s="79"/>
       <c r="R9" s="63"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="78"/>
+      <c r="A10" s="80"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -4856,11 +4899,11 @@
       <c r="N10" s="17"/>
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
-      <c r="Q10" s="77"/>
+      <c r="Q10" s="79"/>
       <c r="R10" s="63"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="78"/>
+      <c r="A11" s="80"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -4876,11 +4919,11 @@
       <c r="N11" s="17"/>
       <c r="O11" s="17"/>
       <c r="P11" s="17"/>
-      <c r="Q11" s="77"/>
+      <c r="Q11" s="79"/>
       <c r="R11" s="63"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="78"/>
+      <c r="A12" s="80"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -4896,11 +4939,11 @@
       <c r="N12" s="17"/>
       <c r="O12" s="17"/>
       <c r="P12" s="17"/>
-      <c r="Q12" s="77"/>
+      <c r="Q12" s="79"/>
       <c r="R12" s="63"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="78"/>
+      <c r="A13" s="80"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -4916,11 +4959,11 @@
       <c r="N13" s="17"/>
       <c r="O13" s="17"/>
       <c r="P13" s="17"/>
-      <c r="Q13" s="77"/>
+      <c r="Q13" s="79"/>
       <c r="R13" s="63"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="78"/>
+      <c r="A14" s="80"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -4936,11 +4979,11 @@
       <c r="N14" s="17"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
-      <c r="Q14" s="77"/>
+      <c r="Q14" s="79"/>
       <c r="R14" s="63"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="78"/>
+      <c r="A15" s="80"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -4956,11 +4999,11 @@
       <c r="N15" s="17"/>
       <c r="O15" s="17"/>
       <c r="P15" s="17"/>
-      <c r="Q15" s="77"/>
+      <c r="Q15" s="79"/>
       <c r="R15" s="63"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="78"/>
+      <c r="A16" s="80"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -4976,11 +5019,11 @@
       <c r="N16" s="17"/>
       <c r="O16" s="17"/>
       <c r="P16" s="17"/>
-      <c r="Q16" s="77"/>
+      <c r="Q16" s="79"/>
       <c r="R16" s="63"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="78"/>
+      <c r="A17" s="80"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -4996,11 +5039,11 @@
       <c r="N17" s="17"/>
       <c r="O17" s="17"/>
       <c r="P17" s="17"/>
-      <c r="Q17" s="77"/>
+      <c r="Q17" s="79"/>
       <c r="R17" s="63"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="78"/>
+      <c r="A18" s="80"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -5016,11 +5059,11 @@
       <c r="N18" s="17"/>
       <c r="O18" s="17"/>
       <c r="P18" s="17"/>
-      <c r="Q18" s="77"/>
+      <c r="Q18" s="79"/>
       <c r="R18" s="63"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="78"/>
+      <c r="A19" s="80"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -5036,11 +5079,11 @@
       <c r="N19" s="17"/>
       <c r="O19" s="17"/>
       <c r="P19" s="17"/>
-      <c r="Q19" s="77"/>
+      <c r="Q19" s="79"/>
       <c r="R19" s="63"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="78"/>
+      <c r="A20" s="80"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -5056,11 +5099,11 @@
       <c r="N20" s="17"/>
       <c r="O20" s="17"/>
       <c r="P20" s="17"/>
-      <c r="Q20" s="77"/>
+      <c r="Q20" s="79"/>
       <c r="R20" s="63"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="78"/>
+      <c r="A21" s="80"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -5076,11 +5119,11 @@
       <c r="N21" s="17"/>
       <c r="O21" s="17"/>
       <c r="P21" s="17"/>
-      <c r="Q21" s="77"/>
+      <c r="Q21" s="79"/>
       <c r="R21" s="63"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="78"/>
+      <c r="A22" s="80"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -5096,11 +5139,11 @@
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
-      <c r="Q22" s="77"/>
+      <c r="Q22" s="79"/>
       <c r="R22" s="63"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="78"/>
+      <c r="A23" s="80"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -5116,11 +5159,11 @@
       <c r="N23" s="17"/>
       <c r="O23" s="17"/>
       <c r="P23" s="17"/>
-      <c r="Q23" s="77"/>
+      <c r="Q23" s="79"/>
       <c r="R23" s="63"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="78"/>
+      <c r="A24" s="80"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -5136,11 +5179,11 @@
       <c r="N24" s="17"/>
       <c r="O24" s="17"/>
       <c r="P24" s="17"/>
-      <c r="Q24" s="77"/>
+      <c r="Q24" s="79"/>
       <c r="R24" s="63"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="78"/>
+      <c r="A25" s="80"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -5156,11 +5199,11 @@
       <c r="N25" s="17"/>
       <c r="O25" s="17"/>
       <c r="P25" s="17"/>
-      <c r="Q25" s="77"/>
+      <c r="Q25" s="79"/>
       <c r="R25" s="63"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="78"/>
+      <c r="A26" s="80"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -5176,11 +5219,11 @@
       <c r="N26" s="17"/>
       <c r="O26" s="17"/>
       <c r="P26" s="17"/>
-      <c r="Q26" s="77"/>
+      <c r="Q26" s="79"/>
       <c r="R26" s="63"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="78"/>
+      <c r="A27" s="80"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -5196,11 +5239,11 @@
       <c r="N27" s="17"/>
       <c r="O27" s="17"/>
       <c r="P27" s="17"/>
-      <c r="Q27" s="77"/>
+      <c r="Q27" s="79"/>
       <c r="R27" s="63"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="78"/>
+      <c r="A28" s="80"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -5216,11 +5259,11 @@
       <c r="N28" s="17"/>
       <c r="O28" s="17"/>
       <c r="P28" s="17"/>
-      <c r="Q28" s="77"/>
+      <c r="Q28" s="79"/>
       <c r="R28" s="63"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="78"/>
+      <c r="A29" s="80"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -5236,11 +5279,11 @@
       <c r="N29" s="17"/>
       <c r="O29" s="17"/>
       <c r="P29" s="17"/>
-      <c r="Q29" s="77"/>
+      <c r="Q29" s="79"/>
       <c r="R29" s="63"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="78"/>
+      <c r="A30" s="80"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -5256,11 +5299,11 @@
       <c r="N30" s="17"/>
       <c r="O30" s="17"/>
       <c r="P30" s="17"/>
-      <c r="Q30" s="77"/>
+      <c r="Q30" s="79"/>
       <c r="R30" s="63"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="78"/>
+      <c r="A31" s="80"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -5276,7 +5319,7 @@
       <c r="N31" s="17"/>
       <c r="O31" s="17"/>
       <c r="P31" s="17"/>
-      <c r="Q31" s="77"/>
+      <c r="Q31" s="79"/>
       <c r="R31" s="63"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5338,9 +5381,15 @@
       <c r="R34" s="69"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="8">
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A2:M2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="D3:F3"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="I3:O3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D4:I4"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
   <pageMargins left="0.590277777777778" right="0.590277777777778" top="0.7875" bottom="0.590277777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
feat: ficha funcional pagina final feita 3
</commit_message>
<xml_diff>
--- a/FICHA_FUNCIONAL_TEMPLATE.xlsx
+++ b/FICHA_FUNCIONAL_TEMPLATE.xlsx
@@ -634,7 +634,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="82">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -939,7 +939,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -947,15 +947,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -982,9 +986,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>834120</xdr:colOff>
+      <xdr:colOff>832680</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>122040</xdr:rowOff>
+      <xdr:rowOff>120600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -998,7 +1002,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="893520" y="847440"/>
-          <a:ext cx="1185840" cy="1568160"/>
+          <a:ext cx="1184400" cy="1566720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4668,14 +4672,16 @@
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="60" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="60" width="29.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="60" width="20.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="60" width="4.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="60" width="19.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="60" width="27.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="60" width="6.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="60" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="60" width="19.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="63" width="0.28"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="60" width="1.7"/>
@@ -4738,10 +4744,10 @@
       </c>
       <c r="E3" s="77"/>
       <c r="F3" s="77"/>
-      <c r="G3" s="78" t="s">
+      <c r="G3" s="76" t="s">
         <v>114</v>
       </c>
-      <c r="H3" s="78"/>
+      <c r="H3" s="76"/>
       <c r="I3" s="17" t="s">
         <v>116</v>
       </c>
@@ -4752,25 +4758,24 @@
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
       <c r="P3" s="17"/>
-      <c r="Q3" s="79"/>
+      <c r="Q3" s="78"/>
       <c r="R3" s="63"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="79" t="s">
         <v>117</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="17"/>
-      <c r="D4" s="17" t="s">
+      <c r="C4" s="17" t="s">
         <v>118</v>
       </c>
+      <c r="D4" s="17"/>
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
       <c r="G4" s="17"/>
       <c r="H4" s="17"/>
-      <c r="I4" s="17"/>
       <c r="J4" s="17"/>
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
@@ -4778,15 +4783,15 @@
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
       <c r="P4" s="17"/>
-      <c r="Q4" s="79"/>
+      <c r="Q4" s="78"/>
       <c r="R4" s="63"/>
       <c r="S4" s="62"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="80"/>
-      <c r="B5" s="78"/>
-      <c r="C5" s="78"/>
-      <c r="D5" s="78"/>
+      <c r="A5" s="79"/>
+      <c r="B5" s="81"/>
+      <c r="C5" s="81"/>
+      <c r="D5" s="81"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -4799,14 +4804,14 @@
       <c r="N5" s="17"/>
       <c r="O5" s="17"/>
       <c r="P5" s="17"/>
-      <c r="Q5" s="79"/>
+      <c r="Q5" s="78"/>
       <c r="R5" s="63"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="80"/>
-      <c r="B6" s="78"/>
-      <c r="C6" s="78"/>
-      <c r="D6" s="78"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="81"/>
+      <c r="C6" s="81"/>
+      <c r="D6" s="81"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -4819,11 +4824,11 @@
       <c r="N6" s="17"/>
       <c r="O6" s="17"/>
       <c r="P6" s="17"/>
-      <c r="Q6" s="79"/>
+      <c r="Q6" s="78"/>
       <c r="R6" s="63"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="80"/>
+      <c r="A7" s="79"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
@@ -4839,11 +4844,11 @@
       <c r="N7" s="17"/>
       <c r="O7" s="17"/>
       <c r="P7" s="17"/>
-      <c r="Q7" s="79"/>
+      <c r="Q7" s="78"/>
       <c r="R7" s="63"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="80"/>
+      <c r="A8" s="79"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
@@ -4859,11 +4864,11 @@
       <c r="N8" s="17"/>
       <c r="O8" s="17"/>
       <c r="P8" s="17"/>
-      <c r="Q8" s="79"/>
+      <c r="Q8" s="78"/>
       <c r="R8" s="63"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="80"/>
+      <c r="A9" s="79"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
@@ -4879,11 +4884,11 @@
       <c r="N9" s="17"/>
       <c r="O9" s="17"/>
       <c r="P9" s="17"/>
-      <c r="Q9" s="79"/>
+      <c r="Q9" s="78"/>
       <c r="R9" s="63"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="80"/>
+      <c r="A10" s="79"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -4899,11 +4904,11 @@
       <c r="N10" s="17"/>
       <c r="O10" s="17"/>
       <c r="P10" s="17"/>
-      <c r="Q10" s="79"/>
+      <c r="Q10" s="78"/>
       <c r="R10" s="63"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="80"/>
+      <c r="A11" s="79"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -4919,11 +4924,11 @@
       <c r="N11" s="17"/>
       <c r="O11" s="17"/>
       <c r="P11" s="17"/>
-      <c r="Q11" s="79"/>
+      <c r="Q11" s="78"/>
       <c r="R11" s="63"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="80"/>
+      <c r="A12" s="79"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -4939,11 +4944,11 @@
       <c r="N12" s="17"/>
       <c r="O12" s="17"/>
       <c r="P12" s="17"/>
-      <c r="Q12" s="79"/>
+      <c r="Q12" s="78"/>
       <c r="R12" s="63"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="80"/>
+      <c r="A13" s="79"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -4959,11 +4964,11 @@
       <c r="N13" s="17"/>
       <c r="O13" s="17"/>
       <c r="P13" s="17"/>
-      <c r="Q13" s="79"/>
+      <c r="Q13" s="78"/>
       <c r="R13" s="63"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="80"/>
+      <c r="A14" s="79"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -4979,11 +4984,11 @@
       <c r="N14" s="17"/>
       <c r="O14" s="17"/>
       <c r="P14" s="17"/>
-      <c r="Q14" s="79"/>
+      <c r="Q14" s="78"/>
       <c r="R14" s="63"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="80"/>
+      <c r="A15" s="79"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -4999,11 +5004,11 @@
       <c r="N15" s="17"/>
       <c r="O15" s="17"/>
       <c r="P15" s="17"/>
-      <c r="Q15" s="79"/>
+      <c r="Q15" s="78"/>
       <c r="R15" s="63"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="80"/>
+      <c r="A16" s="79"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -5019,11 +5024,11 @@
       <c r="N16" s="17"/>
       <c r="O16" s="17"/>
       <c r="P16" s="17"/>
-      <c r="Q16" s="79"/>
+      <c r="Q16" s="78"/>
       <c r="R16" s="63"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="80"/>
+      <c r="A17" s="79"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -5039,11 +5044,11 @@
       <c r="N17" s="17"/>
       <c r="O17" s="17"/>
       <c r="P17" s="17"/>
-      <c r="Q17" s="79"/>
+      <c r="Q17" s="78"/>
       <c r="R17" s="63"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="80"/>
+      <c r="A18" s="79"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -5059,11 +5064,11 @@
       <c r="N18" s="17"/>
       <c r="O18" s="17"/>
       <c r="P18" s="17"/>
-      <c r="Q18" s="79"/>
+      <c r="Q18" s="78"/>
       <c r="R18" s="63"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="80"/>
+      <c r="A19" s="79"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -5079,11 +5084,11 @@
       <c r="N19" s="17"/>
       <c r="O19" s="17"/>
       <c r="P19" s="17"/>
-      <c r="Q19" s="79"/>
+      <c r="Q19" s="78"/>
       <c r="R19" s="63"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="80"/>
+      <c r="A20" s="79"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -5099,11 +5104,11 @@
       <c r="N20" s="17"/>
       <c r="O20" s="17"/>
       <c r="P20" s="17"/>
-      <c r="Q20" s="79"/>
+      <c r="Q20" s="78"/>
       <c r="R20" s="63"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="80"/>
+      <c r="A21" s="79"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -5119,11 +5124,11 @@
       <c r="N21" s="17"/>
       <c r="O21" s="17"/>
       <c r="P21" s="17"/>
-      <c r="Q21" s="79"/>
+      <c r="Q21" s="78"/>
       <c r="R21" s="63"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="80"/>
+      <c r="A22" s="79"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -5139,11 +5144,11 @@
       <c r="N22" s="17"/>
       <c r="O22" s="17"/>
       <c r="P22" s="17"/>
-      <c r="Q22" s="79"/>
+      <c r="Q22" s="78"/>
       <c r="R22" s="63"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="80"/>
+      <c r="A23" s="79"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -5159,11 +5164,11 @@
       <c r="N23" s="17"/>
       <c r="O23" s="17"/>
       <c r="P23" s="17"/>
-      <c r="Q23" s="79"/>
+      <c r="Q23" s="78"/>
       <c r="R23" s="63"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="80"/>
+      <c r="A24" s="79"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -5179,11 +5184,11 @@
       <c r="N24" s="17"/>
       <c r="O24" s="17"/>
       <c r="P24" s="17"/>
-      <c r="Q24" s="79"/>
+      <c r="Q24" s="78"/>
       <c r="R24" s="63"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="80"/>
+      <c r="A25" s="79"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -5199,11 +5204,11 @@
       <c r="N25" s="17"/>
       <c r="O25" s="17"/>
       <c r="P25" s="17"/>
-      <c r="Q25" s="79"/>
+      <c r="Q25" s="78"/>
       <c r="R25" s="63"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="80"/>
+      <c r="A26" s="79"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -5219,11 +5224,11 @@
       <c r="N26" s="17"/>
       <c r="O26" s="17"/>
       <c r="P26" s="17"/>
-      <c r="Q26" s="79"/>
+      <c r="Q26" s="78"/>
       <c r="R26" s="63"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="80"/>
+      <c r="A27" s="79"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -5239,11 +5244,11 @@
       <c r="N27" s="17"/>
       <c r="O27" s="17"/>
       <c r="P27" s="17"/>
-      <c r="Q27" s="79"/>
+      <c r="Q27" s="78"/>
       <c r="R27" s="63"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="80"/>
+      <c r="A28" s="79"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -5259,11 +5264,11 @@
       <c r="N28" s="17"/>
       <c r="O28" s="17"/>
       <c r="P28" s="17"/>
-      <c r="Q28" s="79"/>
+      <c r="Q28" s="78"/>
       <c r="R28" s="63"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="80"/>
+      <c r="A29" s="79"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -5279,11 +5284,11 @@
       <c r="N29" s="17"/>
       <c r="O29" s="17"/>
       <c r="P29" s="17"/>
-      <c r="Q29" s="79"/>
+      <c r="Q29" s="78"/>
       <c r="R29" s="63"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="80"/>
+      <c r="A30" s="79"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -5299,11 +5304,11 @@
       <c r="N30" s="17"/>
       <c r="O30" s="17"/>
       <c r="P30" s="17"/>
-      <c r="Q30" s="79"/>
+      <c r="Q30" s="78"/>
       <c r="R30" s="63"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="80"/>
+      <c r="A31" s="79"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -5319,7 +5324,7 @@
       <c r="N31" s="17"/>
       <c r="O31" s="17"/>
       <c r="P31" s="17"/>
-      <c r="Q31" s="79"/>
+      <c r="Q31" s="78"/>
       <c r="R31" s="63"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5381,15 +5386,14 @@
       <c r="R34" s="69"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
+  <mergeCells count="7">
     <mergeCell ref="A1:R1"/>
     <mergeCell ref="A2:M2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="D3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:O3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="D4:I4"/>
+    <mergeCell ref="C4:H4"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="true" verticalCentered="true"/>
   <pageMargins left="0.590277777777778" right="0.590277777777778" top="0.7875" bottom="0.590277777777778" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
feat: ficha funcional pagina final feita 6
</commit_message>
<xml_diff>
--- a/FICHA_FUNCIONAL_TEMPLATE.xlsx
+++ b/FICHA_FUNCIONAL_TEMPLATE.xlsx
@@ -986,9 +986,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>832680</xdr:colOff>
+      <xdr:colOff>832320</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>120600</xdr:rowOff>
+      <xdr:rowOff>120240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1002,7 +1002,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="893520" y="847440"/>
-          <a:ext cx="1184400" cy="1566720"/>
+          <a:ext cx="1184040" cy="1566360"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4672,7 +4672,7 @@
   <dimension ref="A1:S34"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
feat : versao da ficha funcional 04
</commit_message>
<xml_diff>
--- a/FICHA_FUNCIONAL_TEMPLATE.xlsx
+++ b/FICHA_FUNCIONAL_TEMPLATE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="FRENTE" sheetId="1" state="visible" r:id="rId3"/>
@@ -986,9 +986,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>832320</xdr:colOff>
+      <xdr:colOff>831240</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>120240</xdr:rowOff>
+      <xdr:rowOff>119160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1002,7 +1002,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="893520" y="847440"/>
-          <a:ext cx="1184040" cy="1566360"/>
+          <a:ext cx="1182960" cy="1565280"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1130,8 +1130,8 @@
   </sheetPr>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AE50" activeCellId="0" sqref="AE50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="V45" activeCellId="0" sqref="V45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2835,7 +2835,7 @@
       </c>
       <c r="T45" s="13"/>
       <c r="U45" s="51"/>
-      <c r="V45" s="36" t="s">
+      <c r="V45" s="34" t="s">
         <v>82</v>
       </c>
       <c r="W45" s="13" t="s">
@@ -2882,7 +2882,7 @@
       <c r="S46" s="55"/>
       <c r="T46" s="55"/>
       <c r="U46" s="51"/>
-      <c r="V46" s="36"/>
+      <c r="V46" s="34"/>
       <c r="W46" s="56"/>
       <c r="X46" s="2"/>
       <c r="Z46" s="57"/>
@@ -4671,8 +4671,8 @@
   </sheetPr>
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4682,8 +4682,8 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="60" width="27.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="60" width="6.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="60" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="60" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="63" width="0.28"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="16" min="16" style="60" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="17" style="63" width="0.28"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="60" width="1.7"/>
   </cols>
   <sheetData>
@@ -4726,7 +4726,7 @@
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
       <c r="N2" s="73"/>
-      <c r="O2" s="73"/>
+      <c r="O2" s="74"/>
       <c r="P2" s="73"/>
       <c r="Q2" s="74"/>
       <c r="R2" s="66"/>
@@ -4748,15 +4748,15 @@
         <v>114</v>
       </c>
       <c r="H3" s="76"/>
-      <c r="I3" s="17" t="s">
+      <c r="I3" s="78" t="s">
         <v>116</v>
       </c>
-      <c r="J3" s="17"/>
-      <c r="K3" s="17"/>
-      <c r="L3" s="17"/>
-      <c r="M3" s="17"/>
-      <c r="N3" s="17"/>
-      <c r="O3" s="17"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="78"/>
+      <c r="L3" s="78"/>
+      <c r="M3" s="78"/>
+      <c r="N3" s="78"/>
+      <c r="O3" s="78"/>
       <c r="P3" s="17"/>
       <c r="Q3" s="78"/>
       <c r="R3" s="63"/>
@@ -4781,7 +4781,7 @@
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
-      <c r="O4" s="17"/>
+      <c r="O4" s="78"/>
       <c r="P4" s="17"/>
       <c r="Q4" s="78"/>
       <c r="R4" s="63"/>
@@ -4802,7 +4802,7 @@
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
       <c r="N5" s="17"/>
-      <c r="O5" s="17"/>
+      <c r="O5" s="78"/>
       <c r="P5" s="17"/>
       <c r="Q5" s="78"/>
       <c r="R5" s="63"/>
@@ -4822,7 +4822,7 @@
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
+      <c r="O6" s="78"/>
       <c r="P6" s="17"/>
       <c r="Q6" s="78"/>
       <c r="R6" s="63"/>
@@ -4842,7 +4842,7 @@
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
-      <c r="O7" s="17"/>
+      <c r="O7" s="78"/>
       <c r="P7" s="17"/>
       <c r="Q7" s="78"/>
       <c r="R7" s="63"/>
@@ -4862,7 +4862,7 @@
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
-      <c r="O8" s="17"/>
+      <c r="O8" s="78"/>
       <c r="P8" s="17"/>
       <c r="Q8" s="78"/>
       <c r="R8" s="63"/>
@@ -4882,7 +4882,7 @@
       <c r="L9" s="17"/>
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
-      <c r="O9" s="17"/>
+      <c r="O9" s="78"/>
       <c r="P9" s="17"/>
       <c r="Q9" s="78"/>
       <c r="R9" s="63"/>
@@ -4902,7 +4902,7 @@
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
-      <c r="O10" s="17"/>
+      <c r="O10" s="78"/>
       <c r="P10" s="17"/>
       <c r="Q10" s="78"/>
       <c r="R10" s="63"/>
@@ -4922,7 +4922,7 @@
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
-      <c r="O11" s="17"/>
+      <c r="O11" s="78"/>
       <c r="P11" s="17"/>
       <c r="Q11" s="78"/>
       <c r="R11" s="63"/>
@@ -4942,7 +4942,7 @@
       <c r="L12" s="17"/>
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
-      <c r="O12" s="17"/>
+      <c r="O12" s="78"/>
       <c r="P12" s="17"/>
       <c r="Q12" s="78"/>
       <c r="R12" s="63"/>
@@ -4962,7 +4962,7 @@
       <c r="L13" s="17"/>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
-      <c r="O13" s="17"/>
+      <c r="O13" s="78"/>
       <c r="P13" s="17"/>
       <c r="Q13" s="78"/>
       <c r="R13" s="63"/>
@@ -4982,7 +4982,7 @@
       <c r="L14" s="17"/>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
-      <c r="O14" s="17"/>
+      <c r="O14" s="78"/>
       <c r="P14" s="17"/>
       <c r="Q14" s="78"/>
       <c r="R14" s="63"/>
@@ -5002,7 +5002,7 @@
       <c r="L15" s="17"/>
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
-      <c r="O15" s="17"/>
+      <c r="O15" s="78"/>
       <c r="P15" s="17"/>
       <c r="Q15" s="78"/>
       <c r="R15" s="63"/>
@@ -5022,7 +5022,7 @@
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
-      <c r="O16" s="17"/>
+      <c r="O16" s="78"/>
       <c r="P16" s="17"/>
       <c r="Q16" s="78"/>
       <c r="R16" s="63"/>
@@ -5042,7 +5042,7 @@
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
-      <c r="O17" s="17"/>
+      <c r="O17" s="78"/>
       <c r="P17" s="17"/>
       <c r="Q17" s="78"/>
       <c r="R17" s="63"/>
@@ -5062,7 +5062,7 @@
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
-      <c r="O18" s="17"/>
+      <c r="O18" s="78"/>
       <c r="P18" s="17"/>
       <c r="Q18" s="78"/>
       <c r="R18" s="63"/>
@@ -5082,7 +5082,7 @@
       <c r="L19" s="17"/>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
-      <c r="O19" s="17"/>
+      <c r="O19" s="78"/>
       <c r="P19" s="17"/>
       <c r="Q19" s="78"/>
       <c r="R19" s="63"/>
@@ -5102,7 +5102,7 @@
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
-      <c r="O20" s="17"/>
+      <c r="O20" s="78"/>
       <c r="P20" s="17"/>
       <c r="Q20" s="78"/>
       <c r="R20" s="63"/>
@@ -5122,7 +5122,7 @@
       <c r="L21" s="17"/>
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
-      <c r="O21" s="17"/>
+      <c r="O21" s="78"/>
       <c r="P21" s="17"/>
       <c r="Q21" s="78"/>
       <c r="R21" s="63"/>
@@ -5142,7 +5142,7 @@
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
-      <c r="O22" s="17"/>
+      <c r="O22" s="78"/>
       <c r="P22" s="17"/>
       <c r="Q22" s="78"/>
       <c r="R22" s="63"/>
@@ -5162,7 +5162,7 @@
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
-      <c r="O23" s="17"/>
+      <c r="O23" s="78"/>
       <c r="P23" s="17"/>
       <c r="Q23" s="78"/>
       <c r="R23" s="63"/>
@@ -5182,7 +5182,7 @@
       <c r="L24" s="17"/>
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
-      <c r="O24" s="17"/>
+      <c r="O24" s="78"/>
       <c r="P24" s="17"/>
       <c r="Q24" s="78"/>
       <c r="R24" s="63"/>
@@ -5202,7 +5202,7 @@
       <c r="L25" s="17"/>
       <c r="M25" s="17"/>
       <c r="N25" s="17"/>
-      <c r="O25" s="17"/>
+      <c r="O25" s="78"/>
       <c r="P25" s="17"/>
       <c r="Q25" s="78"/>
       <c r="R25" s="63"/>
@@ -5222,7 +5222,7 @@
       <c r="L26" s="17"/>
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
-      <c r="O26" s="17"/>
+      <c r="O26" s="78"/>
       <c r="P26" s="17"/>
       <c r="Q26" s="78"/>
       <c r="R26" s="63"/>
@@ -5242,7 +5242,7 @@
       <c r="L27" s="17"/>
       <c r="M27" s="17"/>
       <c r="N27" s="17"/>
-      <c r="O27" s="17"/>
+      <c r="O27" s="78"/>
       <c r="P27" s="17"/>
       <c r="Q27" s="78"/>
       <c r="R27" s="63"/>
@@ -5262,7 +5262,7 @@
       <c r="L28" s="17"/>
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
-      <c r="O28" s="17"/>
+      <c r="O28" s="78"/>
       <c r="P28" s="17"/>
       <c r="Q28" s="78"/>
       <c r="R28" s="63"/>
@@ -5282,7 +5282,7 @@
       <c r="L29" s="17"/>
       <c r="M29" s="17"/>
       <c r="N29" s="17"/>
-      <c r="O29" s="17"/>
+      <c r="O29" s="78"/>
       <c r="P29" s="17"/>
       <c r="Q29" s="78"/>
       <c r="R29" s="63"/>
@@ -5302,7 +5302,7 @@
       <c r="L30" s="17"/>
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
-      <c r="O30" s="17"/>
+      <c r="O30" s="78"/>
       <c r="P30" s="17"/>
       <c r="Q30" s="78"/>
       <c r="R30" s="63"/>
@@ -5322,7 +5322,7 @@
       <c r="L31" s="17"/>
       <c r="M31" s="17"/>
       <c r="N31" s="17"/>
-      <c r="O31" s="17"/>
+      <c r="O31" s="78"/>
       <c r="P31" s="17"/>
       <c r="Q31" s="78"/>
       <c r="R31" s="63"/>
@@ -5342,7 +5342,7 @@
       <c r="L32" s="62"/>
       <c r="M32" s="62"/>
       <c r="N32" s="62"/>
-      <c r="O32" s="62"/>
+      <c r="O32" s="63"/>
       <c r="P32" s="62"/>
       <c r="R32" s="63"/>
     </row>
@@ -5361,7 +5361,7 @@
       <c r="L33" s="62"/>
       <c r="M33" s="62"/>
       <c r="N33" s="62"/>
-      <c r="O33" s="62"/>
+      <c r="O33" s="63"/>
       <c r="P33" s="62"/>
       <c r="R33" s="63"/>
     </row>
@@ -5380,7 +5380,7 @@
       <c r="L34" s="68"/>
       <c r="M34" s="68"/>
       <c r="N34" s="68"/>
-      <c r="O34" s="68"/>
+      <c r="O34" s="69"/>
       <c r="P34" s="68"/>
       <c r="Q34" s="69"/>
       <c r="R34" s="69"/>

</xml_diff>

<commit_message>
feat : versao da ficha funcional 05
</commit_message>
<xml_diff>
--- a/FICHA_FUNCIONAL_TEMPLATE.xlsx
+++ b/FICHA_FUNCIONAL_TEMPLATE.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="FRENTE" sheetId="1" state="visible" r:id="rId3"/>
@@ -394,7 +394,7 @@
     <t xml:space="preserve">, para exercer o cargo de provimento em comissão</t>
   </si>
   <si>
-    <t xml:space="preserve">de</t>
+    <t xml:space="preserve"> de</t>
   </si>
   <si>
     <t xml:space="preserve">da Secretaria de Estado de Justiça, Direitos Humanos e Cidadania.</t>
@@ -411,7 +411,7 @@
     <numFmt numFmtId="167" formatCode="#,##0"/>
     <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -489,6 +489,12 @@
     <font>
       <b val="true"/>
       <sz val="28"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -634,7 +640,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="84">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -935,7 +941,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -952,10 +958,18 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -986,9 +1000,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>831240</xdr:colOff>
+      <xdr:colOff>826920</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>119160</xdr:rowOff>
+      <xdr:rowOff>114840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1002,7 +1016,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="893520" y="847440"/>
-          <a:ext cx="1182960" cy="1565280"/>
+          <a:ext cx="1178640" cy="1560960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1130,7 +1144,7 @@
   </sheetPr>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="V45" activeCellId="0" sqref="V45"/>
     </sheetView>
   </sheetViews>
@@ -4671,14 +4685,14 @@
   </sheetPr>
   <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="60" width="4.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="60" width="19.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="60" width="3.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="60" width="17.27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="60" width="27.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="60" width="6.03"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="60" width="18.66"/>
@@ -4768,14 +4782,14 @@
       <c r="B4" s="80" t="s">
         <v>74</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="81" t="s">
         <v>118</v>
       </c>
-      <c r="D4" s="17"/>
-      <c r="E4" s="17"/>
-      <c r="F4" s="17"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="17"/>
+      <c r="D4" s="81"/>
+      <c r="E4" s="81"/>
+      <c r="F4" s="81"/>
+      <c r="G4" s="81"/>
+      <c r="H4" s="81"/>
       <c r="J4" s="17"/>
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
@@ -4788,10 +4802,10 @@
       <c r="S4" s="62"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="79"/>
-      <c r="B5" s="81"/>
-      <c r="C5" s="81"/>
-      <c r="D5" s="81"/>
+      <c r="A5" s="82"/>
+      <c r="B5" s="83"/>
+      <c r="C5" s="83"/>
+      <c r="D5" s="83"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -4808,10 +4822,10 @@
       <c r="R5" s="63"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="79"/>
-      <c r="B6" s="81"/>
-      <c r="C6" s="81"/>
-      <c r="D6" s="81"/>
+      <c r="A6" s="82"/>
+      <c r="B6" s="83"/>
+      <c r="C6" s="83"/>
+      <c r="D6" s="83"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -4828,7 +4842,7 @@
       <c r="R6" s="63"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="79"/>
+      <c r="A7" s="82"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
@@ -4848,7 +4862,7 @@
       <c r="R7" s="63"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="79"/>
+      <c r="A8" s="82"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
@@ -4868,7 +4882,7 @@
       <c r="R8" s="63"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="79"/>
+      <c r="A9" s="82"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
@@ -4888,7 +4902,7 @@
       <c r="R9" s="63"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="79"/>
+      <c r="A10" s="82"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -4908,7 +4922,7 @@
       <c r="R10" s="63"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="79"/>
+      <c r="A11" s="82"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -4928,7 +4942,7 @@
       <c r="R11" s="63"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="79"/>
+      <c r="A12" s="82"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -4948,7 +4962,7 @@
       <c r="R12" s="63"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="79"/>
+      <c r="A13" s="82"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -4968,7 +4982,7 @@
       <c r="R13" s="63"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="79"/>
+      <c r="A14" s="82"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -4988,7 +5002,7 @@
       <c r="R14" s="63"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="79"/>
+      <c r="A15" s="82"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -5008,7 +5022,7 @@
       <c r="R15" s="63"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="79"/>
+      <c r="A16" s="82"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -5028,7 +5042,7 @@
       <c r="R16" s="63"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="79"/>
+      <c r="A17" s="82"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -5048,7 +5062,7 @@
       <c r="R17" s="63"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="79"/>
+      <c r="A18" s="82"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -5068,7 +5082,7 @@
       <c r="R18" s="63"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="79"/>
+      <c r="A19" s="82"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -5088,7 +5102,7 @@
       <c r="R19" s="63"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="79"/>
+      <c r="A20" s="82"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -5108,7 +5122,7 @@
       <c r="R20" s="63"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="79"/>
+      <c r="A21" s="82"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -5128,7 +5142,7 @@
       <c r="R21" s="63"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="79"/>
+      <c r="A22" s="82"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -5148,7 +5162,7 @@
       <c r="R22" s="63"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="79"/>
+      <c r="A23" s="82"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -5168,7 +5182,7 @@
       <c r="R23" s="63"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="79"/>
+      <c r="A24" s="82"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -5188,7 +5202,7 @@
       <c r="R24" s="63"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="79"/>
+      <c r="A25" s="82"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -5208,7 +5222,7 @@
       <c r="R25" s="63"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="79"/>
+      <c r="A26" s="82"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -5228,7 +5242,7 @@
       <c r="R26" s="63"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="79"/>
+      <c r="A27" s="82"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -5248,7 +5262,7 @@
       <c r="R27" s="63"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="79"/>
+      <c r="A28" s="82"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -5268,7 +5282,7 @@
       <c r="R28" s="63"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="79"/>
+      <c r="A29" s="82"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -5288,7 +5302,7 @@
       <c r="R29" s="63"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="79"/>
+      <c r="A30" s="82"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -5308,7 +5322,7 @@
       <c r="R30" s="63"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="79"/>
+      <c r="A31" s="82"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>

</xml_diff>

<commit_message>
feat : versao da ficha funcional com o requirements atualizado
</commit_message>
<xml_diff>
--- a/FICHA_FUNCIONAL_TEMPLATE.xlsx
+++ b/FICHA_FUNCIONAL_TEMPLATE.xlsx
@@ -417,7 +417,7 @@
     <numFmt numFmtId="167" formatCode="#,##0"/>
     <numFmt numFmtId="168" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="13">
+  <fonts count="12">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -474,13 +474,6 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -639,7 +632,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="81">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -812,10 +805,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -852,10 +841,6 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -924,7 +909,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -960,7 +945,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -995,9 +980,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>826560</xdr:colOff>
+      <xdr:colOff>826200</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>114480</xdr:rowOff>
+      <xdr:rowOff>114120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1011,7 +996,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="893520" y="847440"/>
-          <a:ext cx="1178280" cy="1560600"/>
+          <a:ext cx="1177920" cy="1560240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1139,8 +1124,8 @@
   </sheetPr>
   <dimension ref="A1:AG57"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B28" activeCellId="0" sqref="B28"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B13" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P37" activeCellId="0" sqref="P37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.13671875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2372,7 +2357,7 @@
       <c r="AA34" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="AB34" s="43" t="s">
+      <c r="AB34" s="41" t="s">
         <v>66</v>
       </c>
       <c r="AC34" s="2"/>
@@ -2417,7 +2402,7 @@
       <c r="AA35" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="AB35" s="43" t="s">
+      <c r="AB35" s="41" t="s">
         <v>66</v>
       </c>
       <c r="AC35" s="2"/>
@@ -2462,7 +2447,7 @@
       <c r="AA36" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="AB36" s="43" t="s">
+      <c r="AB36" s="41" t="s">
         <v>66</v>
       </c>
       <c r="AC36" s="2"/>
@@ -2507,7 +2492,7 @@
       <c r="AA37" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="AB37" s="43" t="s">
+      <c r="AB37" s="41" t="s">
         <v>66</v>
       </c>
       <c r="AC37" s="2"/>
@@ -2552,7 +2537,7 @@
       <c r="AA38" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="AB38" s="43" t="s">
+      <c r="AB38" s="41" t="s">
         <v>66</v>
       </c>
       <c r="AC38" s="2"/>
@@ -2597,7 +2582,7 @@
       <c r="AA39" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="AB39" s="43" t="s">
+      <c r="AB39" s="41" t="s">
         <v>66</v>
       </c>
       <c r="AC39" s="2"/>
@@ -2637,12 +2622,12 @@
       <c r="V40" s="41"/>
       <c r="W40" s="41"/>
       <c r="X40" s="41"/>
-      <c r="Y40" s="44"/>
+      <c r="Y40" s="43"/>
       <c r="Z40" s="4"/>
       <c r="AA40" s="41" t="s">
         <v>65</v>
       </c>
-      <c r="AB40" s="43" t="s">
+      <c r="AB40" s="41" t="s">
         <v>66</v>
       </c>
       <c r="AC40" s="2"/>
@@ -2721,7 +2706,7 @@
       </c>
       <c r="W42" s="13"/>
       <c r="X42" s="2"/>
-      <c r="Y42" s="45"/>
+      <c r="Y42" s="44"/>
       <c r="Z42" s="2"/>
       <c r="AA42" s="13" t="s">
         <v>73</v>
@@ -2733,7 +2718,7 @@
       <c r="AF42" s="2"/>
       <c r="AG42" s="4"/>
     </row>
-    <row r="43" s="48" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" s="47" customFormat="true" ht="13.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="2"/>
       <c r="B43" s="19" t="s">
         <v>74</v>
@@ -2741,23 +2726,23 @@
       <c r="C43" s="19"/>
       <c r="D43" s="19"/>
       <c r="E43" s="2"/>
-      <c r="F43" s="46" t="s">
+      <c r="F43" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="G43" s="46"/>
+      <c r="G43" s="45"/>
       <c r="H43" s="3"/>
-      <c r="I43" s="47" t="s">
+      <c r="I43" s="46" t="s">
         <v>76</v>
       </c>
-      <c r="J43" s="47"/>
-      <c r="K43" s="47"/>
+      <c r="J43" s="46"/>
+      <c r="K43" s="46"/>
       <c r="L43" s="2"/>
-      <c r="M43" s="47" t="s">
+      <c r="M43" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="N43" s="47"/>
-      <c r="O43" s="47"/>
-      <c r="P43" s="47"/>
+      <c r="N43" s="46"/>
+      <c r="O43" s="46"/>
+      <c r="P43" s="46"/>
       <c r="Q43" s="2"/>
       <c r="R43" s="20" t="s">
         <v>78</v>
@@ -2771,8 +2756,8 @@
       <c r="W43" s="20"/>
       <c r="X43" s="2"/>
       <c r="Z43" s="3"/>
-      <c r="AA43" s="49"/>
-      <c r="AB43" s="49"/>
+      <c r="AA43" s="48"/>
+      <c r="AB43" s="48"/>
       <c r="AC43" s="2"/>
       <c r="AD43" s="3"/>
       <c r="AE43" s="3"/>
@@ -2839,7 +2824,7 @@
       <c r="N45" s="13"/>
       <c r="O45" s="13"/>
       <c r="P45" s="13"/>
-      <c r="Q45" s="50"/>
+      <c r="Q45" s="49"/>
       <c r="R45" s="35" t="s">
         <v>84</v>
       </c>
@@ -2847,7 +2832,7 @@
         <v>85</v>
       </c>
       <c r="T45" s="13"/>
-      <c r="U45" s="50"/>
+      <c r="U45" s="49"/>
       <c r="V45" s="33" t="s">
         <v>84</v>
       </c>
@@ -2861,49 +2846,49 @@
       </c>
       <c r="AB45" s="6"/>
       <c r="AC45" s="2"/>
-      <c r="AD45" s="51"/>
-      <c r="AE45" s="51"/>
+      <c r="AD45" s="50"/>
+      <c r="AE45" s="50"/>
       <c r="AF45" s="4"/>
     </row>
-    <row r="46" s="48" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="46" s="47" customFormat="true" ht="12.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="2"/>
-      <c r="B46" s="47" t="s">
+      <c r="B46" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="C46" s="47"/>
-      <c r="D46" s="47"/>
+      <c r="C46" s="46"/>
+      <c r="D46" s="46"/>
       <c r="E46" s="2"/>
-      <c r="F46" s="52" t="s">
+      <c r="F46" s="51" t="s">
         <v>89</v>
       </c>
-      <c r="G46" s="52"/>
+      <c r="G46" s="51"/>
       <c r="H46" s="2"/>
-      <c r="I46" s="53" t="s">
+      <c r="I46" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="J46" s="53"/>
-      <c r="K46" s="53"/>
+      <c r="J46" s="46"/>
+      <c r="K46" s="46"/>
       <c r="L46" s="2"/>
-      <c r="M46" s="47" t="s">
+      <c r="M46" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="N46" s="47"/>
-      <c r="O46" s="47"/>
-      <c r="P46" s="47"/>
-      <c r="Q46" s="50"/>
+      <c r="N46" s="46"/>
+      <c r="O46" s="46"/>
+      <c r="P46" s="46"/>
+      <c r="Q46" s="49"/>
       <c r="R46" s="35"/>
-      <c r="S46" s="54"/>
-      <c r="T46" s="54"/>
-      <c r="U46" s="50"/>
+      <c r="S46" s="52"/>
+      <c r="T46" s="52"/>
+      <c r="U46" s="49"/>
       <c r="V46" s="33"/>
-      <c r="W46" s="55"/>
+      <c r="W46" s="53"/>
       <c r="X46" s="2"/>
-      <c r="Z46" s="56"/>
+      <c r="Z46" s="54"/>
       <c r="AA46" s="6"/>
       <c r="AB46" s="6"/>
       <c r="AC46" s="2"/>
-      <c r="AD46" s="57"/>
-      <c r="AE46" s="57"/>
+      <c r="AD46" s="55"/>
+      <c r="AE46" s="55"/>
       <c r="AF46" s="17"/>
     </row>
     <row r="47" customFormat="false" ht="6.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2934,8 +2919,8 @@
       <c r="AA47" s="6"/>
       <c r="AB47" s="6"/>
       <c r="AC47" s="2"/>
-      <c r="AD47" s="51"/>
-      <c r="AE47" s="51"/>
+      <c r="AD47" s="50"/>
+      <c r="AE47" s="50"/>
       <c r="AF47" s="4"/>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2966,8 +2951,8 @@
       <c r="AA48" s="6"/>
       <c r="AB48" s="6"/>
       <c r="AC48" s="2"/>
-      <c r="AD48" s="51"/>
-      <c r="AE48" s="51"/>
+      <c r="AD48" s="50"/>
+      <c r="AE48" s="50"/>
       <c r="AF48" s="4"/>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -2998,8 +2983,8 @@
       <c r="AA49" s="6"/>
       <c r="AB49" s="6"/>
       <c r="AC49" s="2"/>
-      <c r="AD49" s="51"/>
-      <c r="AE49" s="51"/>
+      <c r="AD49" s="50"/>
+      <c r="AE49" s="50"/>
       <c r="AF49" s="4"/>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3030,8 +3015,8 @@
       <c r="AA50" s="6"/>
       <c r="AB50" s="6"/>
       <c r="AC50" s="2"/>
-      <c r="AD50" s="51"/>
-      <c r="AE50" s="51"/>
+      <c r="AD50" s="50"/>
+      <c r="AE50" s="50"/>
       <c r="AF50" s="4"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3062,8 +3047,8 @@
       <c r="AA51" s="6"/>
       <c r="AB51" s="6"/>
       <c r="AC51" s="2"/>
-      <c r="AD51" s="51"/>
-      <c r="AE51" s="51"/>
+      <c r="AD51" s="50"/>
+      <c r="AE51" s="50"/>
       <c r="AF51" s="4"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3094,20 +3079,20 @@
       <c r="AA52" s="6"/>
       <c r="AB52" s="6"/>
       <c r="AC52" s="2"/>
-      <c r="AD52" s="51"/>
-      <c r="AE52" s="51"/>
+      <c r="AD52" s="50"/>
+      <c r="AE52" s="50"/>
       <c r="AF52" s="4"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="2"/>
-      <c r="B53" s="58" t="s">
+      <c r="B53" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="C53" s="58"/>
-      <c r="D53" s="58"/>
-      <c r="E53" s="58"/>
-      <c r="F53" s="58"/>
-      <c r="G53" s="58"/>
+      <c r="C53" s="56"/>
+      <c r="D53" s="56"/>
+      <c r="E53" s="56"/>
+      <c r="F53" s="56"/>
+      <c r="G53" s="56"/>
       <c r="H53" s="2" t="s">
         <v>93</v>
       </c>
@@ -3132,8 +3117,8 @@
       <c r="AA53" s="6"/>
       <c r="AB53" s="6"/>
       <c r="AC53" s="2"/>
-      <c r="AD53" s="51"/>
-      <c r="AE53" s="51"/>
+      <c r="AD53" s="50"/>
+      <c r="AE53" s="50"/>
       <c r="AF53" s="4"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3166,8 +3151,8 @@
       <c r="AA54" s="6"/>
       <c r="AB54" s="6"/>
       <c r="AC54" s="2"/>
-      <c r="AD54" s="51"/>
-      <c r="AE54" s="51"/>
+      <c r="AD54" s="50"/>
+      <c r="AE54" s="50"/>
       <c r="AF54" s="4"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3200,18 +3185,18 @@
       <c r="AA55" s="2"/>
       <c r="AB55" s="2"/>
       <c r="AC55" s="2"/>
-      <c r="AD55" s="51"/>
-      <c r="AE55" s="51"/>
+      <c r="AD55" s="50"/>
+      <c r="AE55" s="50"/>
       <c r="AF55" s="4"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="AC56" s="2"/>
-      <c r="AD56" s="51"/>
+      <c r="AD56" s="50"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="AD57" s="51"/>
-      <c r="AE57" s="51"/>
-      <c r="AF57" s="51"/>
+      <c r="AD57" s="50"/>
+      <c r="AE57" s="50"/>
+      <c r="AF57" s="50"/>
     </row>
   </sheetData>
   <mergeCells count="174">
@@ -3414,17 +3399,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="59" width="3.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="59" width="6.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="3" style="59" width="7.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="59" width="2.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="59" width="6.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="59" width="3.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="59" width="6.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="59" width="3.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="59" width="12.56"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="59" width="9.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="59" width="1.56"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="1" min="1" style="57" width="3.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="57" width="6.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="3" style="57" width="7.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="57" width="2.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="57" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="57" width="3.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="57" width="6.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="57" width="3.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="57" width="12.56"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="57" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="57" width="1.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3496,512 +3481,512 @@
       <c r="Z2" s="13"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="60"/>
-      <c r="C3" s="61"/>
-      <c r="D3" s="61"/>
-      <c r="E3" s="62"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="61"/>
-      <c r="H3" s="61"/>
-      <c r="I3" s="62"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="61"/>
-      <c r="L3" s="61"/>
-      <c r="M3" s="62"/>
-      <c r="O3" s="60"/>
-      <c r="P3" s="62"/>
-      <c r="Q3" s="60"/>
-      <c r="R3" s="62"/>
-      <c r="S3" s="63"/>
-      <c r="T3" s="64"/>
-      <c r="U3" s="64"/>
-      <c r="V3" s="64"/>
-      <c r="W3" s="64"/>
-      <c r="X3" s="64"/>
-      <c r="Y3" s="64"/>
-      <c r="Z3" s="65"/>
+      <c r="B3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="60"/>
+      <c r="F3" s="58"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="60"/>
+      <c r="J3" s="58"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="60"/>
+      <c r="O3" s="58"/>
+      <c r="P3" s="60"/>
+      <c r="Q3" s="58"/>
+      <c r="R3" s="60"/>
+      <c r="S3" s="61"/>
+      <c r="T3" s="62"/>
+      <c r="U3" s="62"/>
+      <c r="V3" s="62"/>
+      <c r="W3" s="62"/>
+      <c r="X3" s="62"/>
+      <c r="Y3" s="62"/>
+      <c r="Z3" s="63"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="60"/>
-      <c r="C4" s="61"/>
-      <c r="D4" s="61"/>
-      <c r="E4" s="62"/>
-      <c r="F4" s="60"/>
-      <c r="G4" s="61"/>
-      <c r="H4" s="61"/>
-      <c r="I4" s="62"/>
-      <c r="J4" s="60"/>
-      <c r="K4" s="61"/>
-      <c r="L4" s="61"/>
-      <c r="M4" s="62"/>
-      <c r="O4" s="60"/>
-      <c r="P4" s="62"/>
-      <c r="Q4" s="60"/>
-      <c r="R4" s="62"/>
-      <c r="S4" s="60"/>
-      <c r="T4" s="61"/>
-      <c r="U4" s="61"/>
-      <c r="V4" s="61"/>
-      <c r="W4" s="61"/>
-      <c r="X4" s="61"/>
-      <c r="Y4" s="61"/>
-      <c r="Z4" s="62"/>
+      <c r="B4" s="58"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="60"/>
+      <c r="F4" s="58"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="60"/>
+      <c r="J4" s="58"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="60"/>
+      <c r="O4" s="58"/>
+      <c r="P4" s="60"/>
+      <c r="Q4" s="58"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="58"/>
+      <c r="T4" s="59"/>
+      <c r="U4" s="59"/>
+      <c r="V4" s="59"/>
+      <c r="W4" s="59"/>
+      <c r="X4" s="59"/>
+      <c r="Y4" s="59"/>
+      <c r="Z4" s="60"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="60"/>
-      <c r="C5" s="61"/>
-      <c r="D5" s="61"/>
-      <c r="E5" s="62"/>
-      <c r="F5" s="60"/>
-      <c r="G5" s="61"/>
-      <c r="H5" s="61"/>
-      <c r="I5" s="62"/>
-      <c r="J5" s="60"/>
-      <c r="K5" s="61"/>
-      <c r="L5" s="61"/>
-      <c r="M5" s="62"/>
-      <c r="O5" s="60"/>
-      <c r="P5" s="62"/>
-      <c r="Q5" s="60"/>
-      <c r="R5" s="62"/>
-      <c r="S5" s="60"/>
-      <c r="T5" s="61"/>
-      <c r="U5" s="61"/>
-      <c r="V5" s="61"/>
-      <c r="W5" s="61"/>
-      <c r="X5" s="61"/>
-      <c r="Y5" s="61"/>
-      <c r="Z5" s="62"/>
+      <c r="B5" s="58"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="60"/>
+      <c r="F5" s="58"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="60"/>
+      <c r="J5" s="58"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="60"/>
+      <c r="O5" s="58"/>
+      <c r="P5" s="60"/>
+      <c r="Q5" s="58"/>
+      <c r="R5" s="60"/>
+      <c r="S5" s="58"/>
+      <c r="T5" s="59"/>
+      <c r="U5" s="59"/>
+      <c r="V5" s="59"/>
+      <c r="W5" s="59"/>
+      <c r="X5" s="59"/>
+      <c r="Y5" s="59"/>
+      <c r="Z5" s="60"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="60"/>
-      <c r="C6" s="61"/>
-      <c r="D6" s="61"/>
-      <c r="E6" s="62"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="61"/>
-      <c r="H6" s="61"/>
-      <c r="I6" s="62"/>
-      <c r="J6" s="60"/>
-      <c r="K6" s="61"/>
-      <c r="L6" s="61"/>
-      <c r="M6" s="62"/>
-      <c r="O6" s="60"/>
-      <c r="P6" s="62"/>
-      <c r="Q6" s="60"/>
-      <c r="R6" s="62"/>
-      <c r="S6" s="60"/>
-      <c r="T6" s="61"/>
-      <c r="U6" s="61"/>
-      <c r="V6" s="61"/>
-      <c r="W6" s="61"/>
-      <c r="X6" s="61"/>
-      <c r="Y6" s="61"/>
-      <c r="Z6" s="62"/>
+      <c r="B6" s="58"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="60"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="60"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="60"/>
+      <c r="O6" s="58"/>
+      <c r="P6" s="60"/>
+      <c r="Q6" s="58"/>
+      <c r="R6" s="60"/>
+      <c r="S6" s="58"/>
+      <c r="T6" s="59"/>
+      <c r="U6" s="59"/>
+      <c r="V6" s="59"/>
+      <c r="W6" s="59"/>
+      <c r="X6" s="59"/>
+      <c r="Y6" s="59"/>
+      <c r="Z6" s="60"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="60"/>
-      <c r="C7" s="61"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="62"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="61"/>
-      <c r="H7" s="61"/>
-      <c r="I7" s="62"/>
-      <c r="J7" s="60"/>
-      <c r="K7" s="61"/>
-      <c r="L7" s="61"/>
-      <c r="M7" s="62"/>
-      <c r="O7" s="60"/>
-      <c r="P7" s="62"/>
-      <c r="Q7" s="60"/>
-      <c r="R7" s="62"/>
-      <c r="S7" s="60"/>
-      <c r="T7" s="61"/>
-      <c r="U7" s="61"/>
-      <c r="V7" s="61"/>
-      <c r="W7" s="61"/>
-      <c r="X7" s="61"/>
-      <c r="Y7" s="61"/>
-      <c r="Z7" s="62"/>
+      <c r="B7" s="58"/>
+      <c r="C7" s="59"/>
+      <c r="D7" s="59"/>
+      <c r="E7" s="60"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="60"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="60"/>
+      <c r="O7" s="58"/>
+      <c r="P7" s="60"/>
+      <c r="Q7" s="58"/>
+      <c r="R7" s="60"/>
+      <c r="S7" s="58"/>
+      <c r="T7" s="59"/>
+      <c r="U7" s="59"/>
+      <c r="V7" s="59"/>
+      <c r="W7" s="59"/>
+      <c r="X7" s="59"/>
+      <c r="Y7" s="59"/>
+      <c r="Z7" s="60"/>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="60"/>
-      <c r="C8" s="61"/>
-      <c r="D8" s="61"/>
-      <c r="E8" s="62"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="61"/>
-      <c r="I8" s="62"/>
-      <c r="J8" s="60"/>
-      <c r="K8" s="61"/>
-      <c r="L8" s="61"/>
-      <c r="M8" s="62"/>
-      <c r="O8" s="60"/>
-      <c r="P8" s="62"/>
-      <c r="Q8" s="60"/>
-      <c r="R8" s="62"/>
-      <c r="S8" s="60"/>
-      <c r="T8" s="61"/>
-      <c r="U8" s="61"/>
-      <c r="V8" s="61"/>
-      <c r="W8" s="61"/>
-      <c r="X8" s="61"/>
-      <c r="Y8" s="61"/>
-      <c r="Z8" s="62"/>
+      <c r="B8" s="58"/>
+      <c r="C8" s="59"/>
+      <c r="D8" s="59"/>
+      <c r="E8" s="60"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="59"/>
+      <c r="H8" s="59"/>
+      <c r="I8" s="60"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="59"/>
+      <c r="L8" s="59"/>
+      <c r="M8" s="60"/>
+      <c r="O8" s="58"/>
+      <c r="P8" s="60"/>
+      <c r="Q8" s="58"/>
+      <c r="R8" s="60"/>
+      <c r="S8" s="58"/>
+      <c r="T8" s="59"/>
+      <c r="U8" s="59"/>
+      <c r="V8" s="59"/>
+      <c r="W8" s="59"/>
+      <c r="X8" s="59"/>
+      <c r="Y8" s="59"/>
+      <c r="Z8" s="60"/>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="60"/>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="62"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="61"/>
-      <c r="H9" s="61"/>
-      <c r="I9" s="62"/>
-      <c r="J9" s="60"/>
-      <c r="K9" s="61"/>
-      <c r="L9" s="61"/>
-      <c r="M9" s="62"/>
-      <c r="O9" s="60"/>
-      <c r="P9" s="62"/>
-      <c r="Q9" s="60"/>
-      <c r="R9" s="62"/>
-      <c r="S9" s="60"/>
-      <c r="T9" s="61"/>
-      <c r="U9" s="61"/>
-      <c r="V9" s="61"/>
-      <c r="W9" s="61"/>
-      <c r="X9" s="61"/>
-      <c r="Y9" s="61"/>
-      <c r="Z9" s="62"/>
+      <c r="B9" s="58"/>
+      <c r="C9" s="59"/>
+      <c r="D9" s="59"/>
+      <c r="E9" s="60"/>
+      <c r="F9" s="58"/>
+      <c r="G9" s="59"/>
+      <c r="H9" s="59"/>
+      <c r="I9" s="60"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="59"/>
+      <c r="L9" s="59"/>
+      <c r="M9" s="60"/>
+      <c r="O9" s="58"/>
+      <c r="P9" s="60"/>
+      <c r="Q9" s="58"/>
+      <c r="R9" s="60"/>
+      <c r="S9" s="58"/>
+      <c r="T9" s="59"/>
+      <c r="U9" s="59"/>
+      <c r="V9" s="59"/>
+      <c r="W9" s="59"/>
+      <c r="X9" s="59"/>
+      <c r="Y9" s="59"/>
+      <c r="Z9" s="60"/>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="60"/>
-      <c r="C10" s="61"/>
-      <c r="D10" s="61"/>
-      <c r="E10" s="62"/>
-      <c r="F10" s="60"/>
-      <c r="G10" s="61"/>
-      <c r="H10" s="61"/>
-      <c r="I10" s="62"/>
-      <c r="J10" s="60"/>
-      <c r="K10" s="61"/>
-      <c r="L10" s="61"/>
-      <c r="M10" s="62"/>
-      <c r="O10" s="60"/>
-      <c r="P10" s="62"/>
-      <c r="Q10" s="60"/>
-      <c r="R10" s="62"/>
-      <c r="S10" s="60"/>
-      <c r="T10" s="61"/>
-      <c r="U10" s="61"/>
-      <c r="V10" s="61"/>
-      <c r="W10" s="61"/>
-      <c r="X10" s="61"/>
-      <c r="Y10" s="61"/>
-      <c r="Z10" s="62"/>
+      <c r="B10" s="58"/>
+      <c r="C10" s="59"/>
+      <c r="D10" s="59"/>
+      <c r="E10" s="60"/>
+      <c r="F10" s="58"/>
+      <c r="G10" s="59"/>
+      <c r="H10" s="59"/>
+      <c r="I10" s="60"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="59"/>
+      <c r="L10" s="59"/>
+      <c r="M10" s="60"/>
+      <c r="O10" s="58"/>
+      <c r="P10" s="60"/>
+      <c r="Q10" s="58"/>
+      <c r="R10" s="60"/>
+      <c r="S10" s="58"/>
+      <c r="T10" s="59"/>
+      <c r="U10" s="59"/>
+      <c r="V10" s="59"/>
+      <c r="W10" s="59"/>
+      <c r="X10" s="59"/>
+      <c r="Y10" s="59"/>
+      <c r="Z10" s="60"/>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="60"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="60"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="61"/>
-      <c r="I11" s="62"/>
-      <c r="J11" s="60"/>
-      <c r="K11" s="61"/>
-      <c r="L11" s="61"/>
-      <c r="M11" s="62"/>
-      <c r="O11" s="60"/>
-      <c r="P11" s="62"/>
-      <c r="Q11" s="60"/>
-      <c r="R11" s="62"/>
-      <c r="S11" s="60"/>
-      <c r="T11" s="61"/>
-      <c r="U11" s="61"/>
-      <c r="V11" s="61"/>
-      <c r="W11" s="61"/>
-      <c r="X11" s="61"/>
-      <c r="Y11" s="61"/>
-      <c r="Z11" s="62"/>
+      <c r="B11" s="58"/>
+      <c r="C11" s="59"/>
+      <c r="D11" s="59"/>
+      <c r="E11" s="60"/>
+      <c r="F11" s="58"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="60"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="59"/>
+      <c r="L11" s="59"/>
+      <c r="M11" s="60"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="60"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="60"/>
+      <c r="S11" s="58"/>
+      <c r="T11" s="59"/>
+      <c r="U11" s="59"/>
+      <c r="V11" s="59"/>
+      <c r="W11" s="59"/>
+      <c r="X11" s="59"/>
+      <c r="Y11" s="59"/>
+      <c r="Z11" s="60"/>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="60"/>
-      <c r="C12" s="61"/>
-      <c r="D12" s="61"/>
-      <c r="E12" s="62"/>
-      <c r="F12" s="60"/>
-      <c r="G12" s="61"/>
-      <c r="H12" s="61"/>
-      <c r="I12" s="62"/>
-      <c r="J12" s="60"/>
-      <c r="K12" s="61"/>
-      <c r="L12" s="61"/>
-      <c r="M12" s="62"/>
-      <c r="O12" s="60"/>
-      <c r="P12" s="62"/>
-      <c r="Q12" s="60"/>
-      <c r="R12" s="62"/>
-      <c r="S12" s="60"/>
-      <c r="T12" s="61"/>
-      <c r="U12" s="61"/>
-      <c r="V12" s="61"/>
-      <c r="W12" s="61"/>
-      <c r="X12" s="61"/>
-      <c r="Y12" s="61"/>
-      <c r="Z12" s="62"/>
+      <c r="B12" s="58"/>
+      <c r="C12" s="59"/>
+      <c r="D12" s="59"/>
+      <c r="E12" s="60"/>
+      <c r="F12" s="58"/>
+      <c r="G12" s="59"/>
+      <c r="H12" s="59"/>
+      <c r="I12" s="60"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="59"/>
+      <c r="L12" s="59"/>
+      <c r="M12" s="60"/>
+      <c r="O12" s="58"/>
+      <c r="P12" s="60"/>
+      <c r="Q12" s="58"/>
+      <c r="R12" s="60"/>
+      <c r="S12" s="58"/>
+      <c r="T12" s="59"/>
+      <c r="U12" s="59"/>
+      <c r="V12" s="59"/>
+      <c r="W12" s="59"/>
+      <c r="X12" s="59"/>
+      <c r="Y12" s="59"/>
+      <c r="Z12" s="60"/>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="60"/>
-      <c r="C13" s="61"/>
-      <c r="D13" s="61"/>
-      <c r="E13" s="62"/>
-      <c r="F13" s="60"/>
-      <c r="G13" s="61"/>
-      <c r="H13" s="61"/>
-      <c r="I13" s="62"/>
-      <c r="J13" s="60"/>
-      <c r="K13" s="61"/>
-      <c r="L13" s="61"/>
-      <c r="M13" s="62"/>
-      <c r="O13" s="60"/>
-      <c r="P13" s="62"/>
-      <c r="Q13" s="60"/>
-      <c r="R13" s="62"/>
-      <c r="S13" s="60"/>
-      <c r="T13" s="61"/>
-      <c r="U13" s="61"/>
-      <c r="V13" s="61"/>
-      <c r="W13" s="61"/>
-      <c r="X13" s="61"/>
-      <c r="Y13" s="61"/>
-      <c r="Z13" s="62"/>
+      <c r="B13" s="58"/>
+      <c r="C13" s="59"/>
+      <c r="D13" s="59"/>
+      <c r="E13" s="60"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="59"/>
+      <c r="H13" s="59"/>
+      <c r="I13" s="60"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="59"/>
+      <c r="L13" s="59"/>
+      <c r="M13" s="60"/>
+      <c r="O13" s="58"/>
+      <c r="P13" s="60"/>
+      <c r="Q13" s="58"/>
+      <c r="R13" s="60"/>
+      <c r="S13" s="58"/>
+      <c r="T13" s="59"/>
+      <c r="U13" s="59"/>
+      <c r="V13" s="59"/>
+      <c r="W13" s="59"/>
+      <c r="X13" s="59"/>
+      <c r="Y13" s="59"/>
+      <c r="Z13" s="60"/>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="60"/>
-      <c r="C14" s="61"/>
-      <c r="D14" s="61"/>
-      <c r="E14" s="62"/>
-      <c r="F14" s="60"/>
-      <c r="G14" s="61"/>
-      <c r="H14" s="61"/>
-      <c r="I14" s="62"/>
-      <c r="J14" s="60"/>
-      <c r="K14" s="61"/>
-      <c r="L14" s="61"/>
-      <c r="M14" s="62"/>
-      <c r="O14" s="60"/>
-      <c r="P14" s="62"/>
-      <c r="Q14" s="60"/>
-      <c r="R14" s="62"/>
-      <c r="S14" s="60"/>
-      <c r="T14" s="61"/>
-      <c r="U14" s="61"/>
-      <c r="V14" s="61"/>
-      <c r="W14" s="61"/>
-      <c r="X14" s="61"/>
-      <c r="Y14" s="61"/>
-      <c r="Z14" s="62"/>
+      <c r="B14" s="58"/>
+      <c r="C14" s="59"/>
+      <c r="D14" s="59"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="58"/>
+      <c r="G14" s="59"/>
+      <c r="H14" s="59"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="59"/>
+      <c r="L14" s="59"/>
+      <c r="M14" s="60"/>
+      <c r="O14" s="58"/>
+      <c r="P14" s="60"/>
+      <c r="Q14" s="58"/>
+      <c r="R14" s="60"/>
+      <c r="S14" s="58"/>
+      <c r="T14" s="59"/>
+      <c r="U14" s="59"/>
+      <c r="V14" s="59"/>
+      <c r="W14" s="59"/>
+      <c r="X14" s="59"/>
+      <c r="Y14" s="59"/>
+      <c r="Z14" s="60"/>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="60"/>
-      <c r="C15" s="61"/>
-      <c r="D15" s="61"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="61"/>
-      <c r="H15" s="61"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="61"/>
-      <c r="L15" s="61"/>
-      <c r="M15" s="62"/>
-      <c r="O15" s="60"/>
-      <c r="P15" s="62"/>
-      <c r="Q15" s="60"/>
-      <c r="R15" s="62"/>
-      <c r="S15" s="60"/>
-      <c r="T15" s="61"/>
-      <c r="U15" s="61"/>
-      <c r="V15" s="61"/>
-      <c r="W15" s="61"/>
-      <c r="X15" s="61"/>
-      <c r="Y15" s="61"/>
-      <c r="Z15" s="62"/>
+      <c r="B15" s="58"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="59"/>
+      <c r="E15" s="60"/>
+      <c r="F15" s="58"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="59"/>
+      <c r="L15" s="59"/>
+      <c r="M15" s="60"/>
+      <c r="O15" s="58"/>
+      <c r="P15" s="60"/>
+      <c r="Q15" s="58"/>
+      <c r="R15" s="60"/>
+      <c r="S15" s="58"/>
+      <c r="T15" s="59"/>
+      <c r="U15" s="59"/>
+      <c r="V15" s="59"/>
+      <c r="W15" s="59"/>
+      <c r="X15" s="59"/>
+      <c r="Y15" s="59"/>
+      <c r="Z15" s="60"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="60"/>
-      <c r="C16" s="61"/>
-      <c r="D16" s="61"/>
-      <c r="E16" s="62"/>
-      <c r="F16" s="60"/>
-      <c r="G16" s="61"/>
-      <c r="H16" s="61"/>
-      <c r="I16" s="62"/>
-      <c r="J16" s="60"/>
-      <c r="K16" s="61"/>
-      <c r="L16" s="61"/>
-      <c r="M16" s="62"/>
-      <c r="O16" s="60"/>
-      <c r="P16" s="62"/>
-      <c r="Q16" s="60"/>
-      <c r="R16" s="62"/>
-      <c r="S16" s="60"/>
-      <c r="T16" s="61"/>
-      <c r="U16" s="61"/>
-      <c r="V16" s="61"/>
-      <c r="W16" s="61"/>
-      <c r="X16" s="61"/>
-      <c r="Y16" s="61"/>
-      <c r="Z16" s="62"/>
+      <c r="B16" s="58"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="59"/>
+      <c r="E16" s="60"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="59"/>
+      <c r="H16" s="59"/>
+      <c r="I16" s="60"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="59"/>
+      <c r="L16" s="59"/>
+      <c r="M16" s="60"/>
+      <c r="O16" s="58"/>
+      <c r="P16" s="60"/>
+      <c r="Q16" s="58"/>
+      <c r="R16" s="60"/>
+      <c r="S16" s="58"/>
+      <c r="T16" s="59"/>
+      <c r="U16" s="59"/>
+      <c r="V16" s="59"/>
+      <c r="W16" s="59"/>
+      <c r="X16" s="59"/>
+      <c r="Y16" s="59"/>
+      <c r="Z16" s="60"/>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="60"/>
-      <c r="C17" s="61"/>
-      <c r="D17" s="61"/>
-      <c r="E17" s="62"/>
-      <c r="F17" s="60"/>
-      <c r="G17" s="61"/>
-      <c r="H17" s="61"/>
-      <c r="I17" s="62"/>
-      <c r="J17" s="60"/>
-      <c r="K17" s="61"/>
-      <c r="L17" s="61"/>
-      <c r="M17" s="62"/>
-      <c r="O17" s="60"/>
-      <c r="P17" s="62"/>
-      <c r="Q17" s="60"/>
-      <c r="R17" s="62"/>
-      <c r="S17" s="60"/>
-      <c r="T17" s="61"/>
-      <c r="U17" s="61"/>
-      <c r="V17" s="61"/>
-      <c r="W17" s="61"/>
-      <c r="X17" s="61"/>
-      <c r="Y17" s="61"/>
-      <c r="Z17" s="62"/>
+      <c r="B17" s="58"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="59"/>
+      <c r="E17" s="60"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="59"/>
+      <c r="H17" s="59"/>
+      <c r="I17" s="60"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="59"/>
+      <c r="L17" s="59"/>
+      <c r="M17" s="60"/>
+      <c r="O17" s="58"/>
+      <c r="P17" s="60"/>
+      <c r="Q17" s="58"/>
+      <c r="R17" s="60"/>
+      <c r="S17" s="58"/>
+      <c r="T17" s="59"/>
+      <c r="U17" s="59"/>
+      <c r="V17" s="59"/>
+      <c r="W17" s="59"/>
+      <c r="X17" s="59"/>
+      <c r="Y17" s="59"/>
+      <c r="Z17" s="60"/>
     </row>
     <row r="18" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="60"/>
-      <c r="C18" s="61"/>
-      <c r="D18" s="61"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="60"/>
-      <c r="G18" s="61"/>
-      <c r="H18" s="61"/>
-      <c r="I18" s="62"/>
-      <c r="J18" s="60"/>
-      <c r="K18" s="61"/>
-      <c r="L18" s="61"/>
-      <c r="M18" s="62"/>
-      <c r="O18" s="60"/>
-      <c r="P18" s="62"/>
-      <c r="Q18" s="60"/>
-      <c r="R18" s="62"/>
-      <c r="S18" s="60"/>
-      <c r="T18" s="61"/>
-      <c r="U18" s="61"/>
-      <c r="V18" s="61"/>
-      <c r="W18" s="61"/>
-      <c r="X18" s="61"/>
-      <c r="Y18" s="61"/>
-      <c r="Z18" s="62"/>
+      <c r="B18" s="58"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="59"/>
+      <c r="E18" s="60"/>
+      <c r="F18" s="58"/>
+      <c r="G18" s="59"/>
+      <c r="H18" s="59"/>
+      <c r="I18" s="60"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="59"/>
+      <c r="L18" s="59"/>
+      <c r="M18" s="60"/>
+      <c r="O18" s="58"/>
+      <c r="P18" s="60"/>
+      <c r="Q18" s="58"/>
+      <c r="R18" s="60"/>
+      <c r="S18" s="58"/>
+      <c r="T18" s="59"/>
+      <c r="U18" s="59"/>
+      <c r="V18" s="59"/>
+      <c r="W18" s="59"/>
+      <c r="X18" s="59"/>
+      <c r="Y18" s="59"/>
+      <c r="Z18" s="60"/>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="60"/>
-      <c r="C19" s="61"/>
-      <c r="D19" s="61"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="61"/>
-      <c r="H19" s="61"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="61"/>
-      <c r="L19" s="61"/>
-      <c r="M19" s="62"/>
-      <c r="O19" s="60"/>
-      <c r="P19" s="62"/>
-      <c r="Q19" s="60"/>
-      <c r="R19" s="62"/>
-      <c r="S19" s="60"/>
-      <c r="T19" s="61"/>
-      <c r="U19" s="61"/>
-      <c r="V19" s="61"/>
-      <c r="W19" s="61"/>
-      <c r="X19" s="61"/>
-      <c r="Y19" s="61"/>
-      <c r="Z19" s="62"/>
+      <c r="B19" s="58"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="59"/>
+      <c r="E19" s="60"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="59"/>
+      <c r="L19" s="59"/>
+      <c r="M19" s="60"/>
+      <c r="O19" s="58"/>
+      <c r="P19" s="60"/>
+      <c r="Q19" s="58"/>
+      <c r="R19" s="60"/>
+      <c r="S19" s="58"/>
+      <c r="T19" s="59"/>
+      <c r="U19" s="59"/>
+      <c r="V19" s="59"/>
+      <c r="W19" s="59"/>
+      <c r="X19" s="59"/>
+      <c r="Y19" s="59"/>
+      <c r="Z19" s="60"/>
     </row>
     <row r="20" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="60"/>
-      <c r="C20" s="61"/>
-      <c r="D20" s="61"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="60"/>
-      <c r="G20" s="61"/>
-      <c r="H20" s="61"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="60"/>
-      <c r="K20" s="61"/>
-      <c r="L20" s="61"/>
-      <c r="M20" s="62"/>
-      <c r="O20" s="60"/>
-      <c r="P20" s="62"/>
-      <c r="Q20" s="60"/>
-      <c r="R20" s="62"/>
-      <c r="S20" s="60"/>
-      <c r="T20" s="61"/>
-      <c r="U20" s="61"/>
-      <c r="V20" s="61"/>
-      <c r="W20" s="61"/>
-      <c r="X20" s="61"/>
-      <c r="Y20" s="61"/>
-      <c r="Z20" s="62"/>
+      <c r="B20" s="58"/>
+      <c r="C20" s="59"/>
+      <c r="D20" s="59"/>
+      <c r="E20" s="60"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="59"/>
+      <c r="H20" s="59"/>
+      <c r="I20" s="60"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="59"/>
+      <c r="L20" s="59"/>
+      <c r="M20" s="60"/>
+      <c r="O20" s="58"/>
+      <c r="P20" s="60"/>
+      <c r="Q20" s="58"/>
+      <c r="R20" s="60"/>
+      <c r="S20" s="58"/>
+      <c r="T20" s="59"/>
+      <c r="U20" s="59"/>
+      <c r="V20" s="59"/>
+      <c r="W20" s="59"/>
+      <c r="X20" s="59"/>
+      <c r="Y20" s="59"/>
+      <c r="Z20" s="60"/>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="66"/>
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="68"/>
-      <c r="F21" s="66"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="68"/>
-      <c r="J21" s="66"/>
-      <c r="K21" s="67"/>
-      <c r="L21" s="67"/>
-      <c r="M21" s="68"/>
-      <c r="O21" s="60"/>
-      <c r="P21" s="62"/>
-      <c r="Q21" s="60"/>
-      <c r="R21" s="62"/>
-      <c r="S21" s="60"/>
-      <c r="T21" s="61"/>
-      <c r="U21" s="61"/>
-      <c r="V21" s="61"/>
-      <c r="W21" s="61"/>
-      <c r="X21" s="61"/>
-      <c r="Y21" s="61"/>
-      <c r="Z21" s="62"/>
+      <c r="B21" s="64"/>
+      <c r="C21" s="65"/>
+      <c r="D21" s="65"/>
+      <c r="E21" s="66"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="65"/>
+      <c r="H21" s="65"/>
+      <c r="I21" s="66"/>
+      <c r="J21" s="64"/>
+      <c r="K21" s="65"/>
+      <c r="L21" s="65"/>
+      <c r="M21" s="66"/>
+      <c r="O21" s="58"/>
+      <c r="P21" s="60"/>
+      <c r="Q21" s="58"/>
+      <c r="R21" s="60"/>
+      <c r="S21" s="58"/>
+      <c r="T21" s="59"/>
+      <c r="U21" s="59"/>
+      <c r="V21" s="59"/>
+      <c r="W21" s="59"/>
+      <c r="X21" s="59"/>
+      <c r="Y21" s="59"/>
+      <c r="Z21" s="60"/>
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="O22" s="60"/>
-      <c r="P22" s="62"/>
-      <c r="Q22" s="60"/>
-      <c r="R22" s="62"/>
-      <c r="S22" s="60"/>
-      <c r="T22" s="61"/>
-      <c r="U22" s="61"/>
-      <c r="V22" s="61"/>
-      <c r="W22" s="61"/>
-      <c r="X22" s="61"/>
-      <c r="Y22" s="61"/>
-      <c r="Z22" s="62"/>
+      <c r="O22" s="58"/>
+      <c r="P22" s="60"/>
+      <c r="Q22" s="58"/>
+      <c r="R22" s="60"/>
+      <c r="S22" s="58"/>
+      <c r="T22" s="59"/>
+      <c r="U22" s="59"/>
+      <c r="V22" s="59"/>
+      <c r="W22" s="59"/>
+      <c r="X22" s="59"/>
+      <c r="Y22" s="59"/>
+      <c r="Z22" s="60"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="12" t="s">
@@ -4018,18 +4003,18 @@
       <c r="K23" s="12"/>
       <c r="L23" s="12"/>
       <c r="M23" s="12"/>
-      <c r="O23" s="60"/>
-      <c r="P23" s="62"/>
-      <c r="Q23" s="60"/>
-      <c r="R23" s="62"/>
-      <c r="S23" s="60"/>
-      <c r="T23" s="61"/>
-      <c r="U23" s="61"/>
-      <c r="V23" s="61"/>
-      <c r="W23" s="61"/>
-      <c r="X23" s="61"/>
-      <c r="Y23" s="61"/>
-      <c r="Z23" s="62"/>
+      <c r="O23" s="58"/>
+      <c r="P23" s="60"/>
+      <c r="Q23" s="58"/>
+      <c r="R23" s="60"/>
+      <c r="S23" s="58"/>
+      <c r="T23" s="59"/>
+      <c r="U23" s="59"/>
+      <c r="V23" s="59"/>
+      <c r="W23" s="59"/>
+      <c r="X23" s="59"/>
+      <c r="Y23" s="59"/>
+      <c r="Z23" s="60"/>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="13" t="s">
@@ -4050,304 +4035,304 @@
       <c r="K24" s="13"/>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
-      <c r="O24" s="60"/>
-      <c r="P24" s="62"/>
-      <c r="Q24" s="60"/>
-      <c r="R24" s="62"/>
-      <c r="S24" s="60"/>
-      <c r="T24" s="61"/>
-      <c r="U24" s="61"/>
-      <c r="V24" s="61"/>
-      <c r="W24" s="61"/>
-      <c r="X24" s="61"/>
-      <c r="Y24" s="61"/>
-      <c r="Z24" s="62"/>
+      <c r="O24" s="58"/>
+      <c r="P24" s="60"/>
+      <c r="Q24" s="58"/>
+      <c r="R24" s="60"/>
+      <c r="S24" s="58"/>
+      <c r="T24" s="59"/>
+      <c r="U24" s="59"/>
+      <c r="V24" s="59"/>
+      <c r="W24" s="59"/>
+      <c r="X24" s="59"/>
+      <c r="Y24" s="59"/>
+      <c r="Z24" s="60"/>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="60"/>
-      <c r="C25" s="61"/>
-      <c r="D25" s="61"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="60"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="60"/>
-      <c r="K25" s="64"/>
-      <c r="L25" s="64"/>
-      <c r="M25" s="65"/>
-      <c r="O25" s="60"/>
-      <c r="P25" s="62"/>
-      <c r="Q25" s="60"/>
-      <c r="R25" s="62"/>
-      <c r="S25" s="60"/>
-      <c r="T25" s="61"/>
-      <c r="U25" s="61"/>
-      <c r="V25" s="61"/>
-      <c r="W25" s="61"/>
-      <c r="X25" s="61"/>
-      <c r="Y25" s="61"/>
-      <c r="Z25" s="62"/>
+      <c r="B25" s="58"/>
+      <c r="C25" s="59"/>
+      <c r="D25" s="59"/>
+      <c r="E25" s="60"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="59"/>
+      <c r="H25" s="59"/>
+      <c r="I25" s="60"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="62"/>
+      <c r="M25" s="63"/>
+      <c r="O25" s="58"/>
+      <c r="P25" s="60"/>
+      <c r="Q25" s="58"/>
+      <c r="R25" s="60"/>
+      <c r="S25" s="58"/>
+      <c r="T25" s="59"/>
+      <c r="U25" s="59"/>
+      <c r="V25" s="59"/>
+      <c r="W25" s="59"/>
+      <c r="X25" s="59"/>
+      <c r="Y25" s="59"/>
+      <c r="Z25" s="60"/>
     </row>
     <row r="26" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="60"/>
-      <c r="C26" s="61"/>
-      <c r="D26" s="61"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="60"/>
-      <c r="G26" s="61"/>
-      <c r="H26" s="61"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="60"/>
-      <c r="K26" s="61"/>
-      <c r="L26" s="61"/>
-      <c r="M26" s="62"/>
-      <c r="O26" s="60"/>
-      <c r="P26" s="62"/>
-      <c r="Q26" s="60"/>
-      <c r="R26" s="62"/>
-      <c r="S26" s="60"/>
-      <c r="T26" s="61"/>
-      <c r="U26" s="61"/>
-      <c r="V26" s="61"/>
-      <c r="W26" s="61"/>
-      <c r="X26" s="61"/>
-      <c r="Y26" s="61"/>
-      <c r="Z26" s="62"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="59"/>
+      <c r="D26" s="59"/>
+      <c r="E26" s="60"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="59"/>
+      <c r="H26" s="59"/>
+      <c r="I26" s="60"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="59"/>
+      <c r="L26" s="59"/>
+      <c r="M26" s="60"/>
+      <c r="O26" s="58"/>
+      <c r="P26" s="60"/>
+      <c r="Q26" s="58"/>
+      <c r="R26" s="60"/>
+      <c r="S26" s="58"/>
+      <c r="T26" s="59"/>
+      <c r="U26" s="59"/>
+      <c r="V26" s="59"/>
+      <c r="W26" s="59"/>
+      <c r="X26" s="59"/>
+      <c r="Y26" s="59"/>
+      <c r="Z26" s="60"/>
     </row>
     <row r="27" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="60"/>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
-      <c r="E27" s="62"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="61"/>
-      <c r="I27" s="62"/>
-      <c r="J27" s="60"/>
-      <c r="K27" s="61"/>
-      <c r="L27" s="61"/>
-      <c r="M27" s="62"/>
-      <c r="O27" s="60"/>
-      <c r="P27" s="62"/>
-      <c r="Q27" s="60"/>
-      <c r="R27" s="62"/>
-      <c r="S27" s="60"/>
-      <c r="T27" s="61"/>
-      <c r="U27" s="61"/>
-      <c r="V27" s="61"/>
-      <c r="W27" s="61"/>
-      <c r="X27" s="61"/>
-      <c r="Y27" s="61"/>
-      <c r="Z27" s="62"/>
+      <c r="B27" s="58"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="59"/>
+      <c r="E27" s="60"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="58"/>
+      <c r="K27" s="59"/>
+      <c r="L27" s="59"/>
+      <c r="M27" s="60"/>
+      <c r="O27" s="58"/>
+      <c r="P27" s="60"/>
+      <c r="Q27" s="58"/>
+      <c r="R27" s="60"/>
+      <c r="S27" s="58"/>
+      <c r="T27" s="59"/>
+      <c r="U27" s="59"/>
+      <c r="V27" s="59"/>
+      <c r="W27" s="59"/>
+      <c r="X27" s="59"/>
+      <c r="Y27" s="59"/>
+      <c r="Z27" s="60"/>
     </row>
     <row r="28" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="60"/>
-      <c r="C28" s="61"/>
-      <c r="D28" s="61"/>
-      <c r="E28" s="62"/>
-      <c r="F28" s="60"/>
-      <c r="G28" s="61"/>
-      <c r="H28" s="61"/>
-      <c r="I28" s="62"/>
-      <c r="J28" s="60"/>
-      <c r="K28" s="61"/>
-      <c r="L28" s="61"/>
-      <c r="M28" s="62"/>
-      <c r="O28" s="60"/>
-      <c r="P28" s="62"/>
-      <c r="Q28" s="60"/>
-      <c r="R28" s="62"/>
-      <c r="S28" s="60"/>
-      <c r="T28" s="61"/>
-      <c r="U28" s="61"/>
-      <c r="V28" s="61"/>
-      <c r="W28" s="61"/>
-      <c r="X28" s="61"/>
-      <c r="Y28" s="61"/>
-      <c r="Z28" s="62"/>
+      <c r="B28" s="58"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="59"/>
+      <c r="E28" s="60"/>
+      <c r="F28" s="58"/>
+      <c r="G28" s="59"/>
+      <c r="H28" s="59"/>
+      <c r="I28" s="60"/>
+      <c r="J28" s="58"/>
+      <c r="K28" s="59"/>
+      <c r="L28" s="59"/>
+      <c r="M28" s="60"/>
+      <c r="O28" s="58"/>
+      <c r="P28" s="60"/>
+      <c r="Q28" s="58"/>
+      <c r="R28" s="60"/>
+      <c r="S28" s="58"/>
+      <c r="T28" s="59"/>
+      <c r="U28" s="59"/>
+      <c r="V28" s="59"/>
+      <c r="W28" s="59"/>
+      <c r="X28" s="59"/>
+      <c r="Y28" s="59"/>
+      <c r="Z28" s="60"/>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="60"/>
-      <c r="C29" s="61"/>
-      <c r="D29" s="61"/>
-      <c r="E29" s="62"/>
-      <c r="F29" s="60"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="61"/>
-      <c r="I29" s="62"/>
-      <c r="J29" s="60"/>
-      <c r="K29" s="61"/>
-      <c r="L29" s="61"/>
-      <c r="M29" s="62"/>
-      <c r="O29" s="60"/>
-      <c r="P29" s="62"/>
-      <c r="Q29" s="60"/>
-      <c r="R29" s="62"/>
-      <c r="S29" s="60"/>
-      <c r="T29" s="61"/>
-      <c r="U29" s="61"/>
-      <c r="V29" s="61"/>
-      <c r="W29" s="61"/>
-      <c r="X29" s="61"/>
-      <c r="Y29" s="61"/>
-      <c r="Z29" s="62"/>
+      <c r="B29" s="58"/>
+      <c r="C29" s="59"/>
+      <c r="D29" s="59"/>
+      <c r="E29" s="60"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="59"/>
+      <c r="H29" s="59"/>
+      <c r="I29" s="60"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="59"/>
+      <c r="L29" s="59"/>
+      <c r="M29" s="60"/>
+      <c r="O29" s="58"/>
+      <c r="P29" s="60"/>
+      <c r="Q29" s="58"/>
+      <c r="R29" s="60"/>
+      <c r="S29" s="58"/>
+      <c r="T29" s="59"/>
+      <c r="U29" s="59"/>
+      <c r="V29" s="59"/>
+      <c r="W29" s="59"/>
+      <c r="X29" s="59"/>
+      <c r="Y29" s="59"/>
+      <c r="Z29" s="60"/>
     </row>
     <row r="30" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="60"/>
-      <c r="C30" s="61"/>
-      <c r="D30" s="61"/>
-      <c r="E30" s="62"/>
-      <c r="F30" s="60"/>
-      <c r="G30" s="61"/>
-      <c r="H30" s="61"/>
-      <c r="I30" s="62"/>
-      <c r="J30" s="60"/>
-      <c r="K30" s="61"/>
-      <c r="L30" s="61"/>
-      <c r="M30" s="62"/>
-      <c r="O30" s="60"/>
-      <c r="P30" s="62"/>
-      <c r="Q30" s="60"/>
-      <c r="R30" s="62"/>
-      <c r="S30" s="60"/>
-      <c r="T30" s="61"/>
-      <c r="U30" s="61"/>
-      <c r="V30" s="61"/>
-      <c r="W30" s="61"/>
-      <c r="X30" s="61"/>
-      <c r="Y30" s="61"/>
-      <c r="Z30" s="62"/>
+      <c r="B30" s="58"/>
+      <c r="C30" s="59"/>
+      <c r="D30" s="59"/>
+      <c r="E30" s="60"/>
+      <c r="F30" s="58"/>
+      <c r="G30" s="59"/>
+      <c r="H30" s="59"/>
+      <c r="I30" s="60"/>
+      <c r="J30" s="58"/>
+      <c r="K30" s="59"/>
+      <c r="L30" s="59"/>
+      <c r="M30" s="60"/>
+      <c r="O30" s="58"/>
+      <c r="P30" s="60"/>
+      <c r="Q30" s="58"/>
+      <c r="R30" s="60"/>
+      <c r="S30" s="58"/>
+      <c r="T30" s="59"/>
+      <c r="U30" s="59"/>
+      <c r="V30" s="59"/>
+      <c r="W30" s="59"/>
+      <c r="X30" s="59"/>
+      <c r="Y30" s="59"/>
+      <c r="Z30" s="60"/>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="60"/>
-      <c r="C31" s="61"/>
-      <c r="D31" s="61"/>
-      <c r="E31" s="62"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="61"/>
-      <c r="H31" s="61"/>
-      <c r="I31" s="62"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="61"/>
-      <c r="L31" s="61"/>
-      <c r="M31" s="62"/>
-      <c r="O31" s="60"/>
-      <c r="P31" s="62"/>
-      <c r="Q31" s="60"/>
-      <c r="R31" s="62"/>
-      <c r="S31" s="60"/>
-      <c r="T31" s="61"/>
-      <c r="U31" s="61"/>
-      <c r="V31" s="61"/>
-      <c r="W31" s="61"/>
-      <c r="X31" s="61"/>
-      <c r="Y31" s="61"/>
-      <c r="Z31" s="62"/>
+      <c r="B31" s="58"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="59"/>
+      <c r="E31" s="60"/>
+      <c r="F31" s="58"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="59"/>
+      <c r="L31" s="59"/>
+      <c r="M31" s="60"/>
+      <c r="O31" s="58"/>
+      <c r="P31" s="60"/>
+      <c r="Q31" s="58"/>
+      <c r="R31" s="60"/>
+      <c r="S31" s="58"/>
+      <c r="T31" s="59"/>
+      <c r="U31" s="59"/>
+      <c r="V31" s="59"/>
+      <c r="W31" s="59"/>
+      <c r="X31" s="59"/>
+      <c r="Y31" s="59"/>
+      <c r="Z31" s="60"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="60"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="62"/>
-      <c r="F32" s="60"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="62"/>
-      <c r="J32" s="60"/>
-      <c r="K32" s="61"/>
-      <c r="L32" s="61"/>
-      <c r="M32" s="62"/>
-      <c r="O32" s="60"/>
-      <c r="P32" s="62"/>
-      <c r="Q32" s="60"/>
-      <c r="R32" s="62"/>
-      <c r="S32" s="60"/>
-      <c r="T32" s="61"/>
-      <c r="U32" s="61"/>
-      <c r="V32" s="61"/>
-      <c r="W32" s="61"/>
-      <c r="X32" s="61"/>
-      <c r="Y32" s="61"/>
-      <c r="Z32" s="62"/>
+      <c r="B32" s="58"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="60"/>
+      <c r="F32" s="58"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="60"/>
+      <c r="J32" s="58"/>
+      <c r="K32" s="59"/>
+      <c r="L32" s="59"/>
+      <c r="M32" s="60"/>
+      <c r="O32" s="58"/>
+      <c r="P32" s="60"/>
+      <c r="Q32" s="58"/>
+      <c r="R32" s="60"/>
+      <c r="S32" s="58"/>
+      <c r="T32" s="59"/>
+      <c r="U32" s="59"/>
+      <c r="V32" s="59"/>
+      <c r="W32" s="59"/>
+      <c r="X32" s="59"/>
+      <c r="Y32" s="59"/>
+      <c r="Z32" s="60"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="60"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="62"/>
-      <c r="F33" s="60"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="62"/>
-      <c r="J33" s="60"/>
-      <c r="K33" s="61"/>
-      <c r="L33" s="61"/>
-      <c r="M33" s="62"/>
-      <c r="O33" s="60"/>
-      <c r="P33" s="62"/>
-      <c r="Q33" s="60"/>
-      <c r="R33" s="62"/>
-      <c r="S33" s="60"/>
-      <c r="T33" s="61"/>
-      <c r="U33" s="61"/>
-      <c r="V33" s="61"/>
-      <c r="W33" s="61"/>
-      <c r="X33" s="61"/>
-      <c r="Y33" s="61"/>
-      <c r="Z33" s="62"/>
+      <c r="B33" s="58"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="60"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="60"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="59"/>
+      <c r="L33" s="59"/>
+      <c r="M33" s="60"/>
+      <c r="O33" s="58"/>
+      <c r="P33" s="60"/>
+      <c r="Q33" s="58"/>
+      <c r="R33" s="60"/>
+      <c r="S33" s="58"/>
+      <c r="T33" s="59"/>
+      <c r="U33" s="59"/>
+      <c r="V33" s="59"/>
+      <c r="W33" s="59"/>
+      <c r="X33" s="59"/>
+      <c r="Y33" s="59"/>
+      <c r="Z33" s="60"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="60"/>
-      <c r="C34" s="61"/>
-      <c r="D34" s="61"/>
-      <c r="E34" s="62"/>
-      <c r="F34" s="60"/>
-      <c r="G34" s="61"/>
-      <c r="H34" s="61"/>
-      <c r="I34" s="62"/>
-      <c r="J34" s="60"/>
-      <c r="K34" s="61"/>
-      <c r="L34" s="61"/>
-      <c r="M34" s="62"/>
-      <c r="O34" s="60"/>
-      <c r="P34" s="62"/>
-      <c r="Q34" s="60"/>
-      <c r="R34" s="62"/>
-      <c r="S34" s="60"/>
-      <c r="T34" s="61"/>
-      <c r="U34" s="61"/>
-      <c r="V34" s="61"/>
-      <c r="W34" s="61"/>
-      <c r="X34" s="61"/>
-      <c r="Y34" s="61"/>
-      <c r="Z34" s="62"/>
+      <c r="B34" s="58"/>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="60"/>
+      <c r="F34" s="58"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
+      <c r="I34" s="60"/>
+      <c r="J34" s="58"/>
+      <c r="K34" s="59"/>
+      <c r="L34" s="59"/>
+      <c r="M34" s="60"/>
+      <c r="O34" s="58"/>
+      <c r="P34" s="60"/>
+      <c r="Q34" s="58"/>
+      <c r="R34" s="60"/>
+      <c r="S34" s="58"/>
+      <c r="T34" s="59"/>
+      <c r="U34" s="59"/>
+      <c r="V34" s="59"/>
+      <c r="W34" s="59"/>
+      <c r="X34" s="59"/>
+      <c r="Y34" s="59"/>
+      <c r="Z34" s="60"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="66"/>
-      <c r="C35" s="67"/>
-      <c r="D35" s="67"/>
-      <c r="E35" s="68"/>
-      <c r="F35" s="66"/>
-      <c r="G35" s="67"/>
-      <c r="H35" s="67"/>
-      <c r="I35" s="68"/>
-      <c r="J35" s="66"/>
-      <c r="K35" s="67"/>
-      <c r="L35" s="67"/>
-      <c r="M35" s="68"/>
-      <c r="O35" s="66"/>
-      <c r="P35" s="68"/>
-      <c r="Q35" s="66"/>
-      <c r="R35" s="68"/>
-      <c r="S35" s="66"/>
-      <c r="T35" s="67"/>
-      <c r="U35" s="67"/>
-      <c r="V35" s="67"/>
-      <c r="W35" s="67"/>
-      <c r="X35" s="67"/>
-      <c r="Y35" s="67"/>
-      <c r="Z35" s="68"/>
+      <c r="B35" s="64"/>
+      <c r="C35" s="65"/>
+      <c r="D35" s="65"/>
+      <c r="E35" s="66"/>
+      <c r="F35" s="64"/>
+      <c r="G35" s="65"/>
+      <c r="H35" s="65"/>
+      <c r="I35" s="66"/>
+      <c r="J35" s="64"/>
+      <c r="K35" s="65"/>
+      <c r="L35" s="65"/>
+      <c r="M35" s="66"/>
+      <c r="O35" s="64"/>
+      <c r="P35" s="66"/>
+      <c r="Q35" s="64"/>
+      <c r="R35" s="66"/>
+      <c r="S35" s="64"/>
+      <c r="T35" s="65"/>
+      <c r="U35" s="65"/>
+      <c r="V35" s="65"/>
+      <c r="W35" s="65"/>
+      <c r="X35" s="65"/>
+      <c r="Y35" s="65"/>
+      <c r="Z35" s="66"/>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="10" t="s">
@@ -4390,7 +4375,7 @@
         <v>110</v>
       </c>
       <c r="F38" s="13"/>
-      <c r="G38" s="69"/>
+      <c r="G38" s="67"/>
       <c r="H38" s="13" t="s">
         <v>111</v>
       </c>
@@ -4420,229 +4405,229 @@
       <c r="Z38" s="13"/>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="63"/>
-      <c r="C39" s="64"/>
-      <c r="D39" s="65"/>
-      <c r="E39" s="60"/>
-      <c r="F39" s="62"/>
-      <c r="G39" s="61"/>
-      <c r="H39" s="60"/>
-      <c r="I39" s="62"/>
-      <c r="J39" s="61"/>
-      <c r="K39" s="61"/>
-      <c r="L39" s="61"/>
-      <c r="M39" s="62"/>
-      <c r="O39" s="70"/>
-      <c r="P39" s="61"/>
-      <c r="Q39" s="62"/>
-      <c r="S39" s="60"/>
-      <c r="T39" s="61"/>
-      <c r="U39" s="61"/>
-      <c r="V39" s="62"/>
-      <c r="W39" s="63"/>
-      <c r="X39" s="64"/>
-      <c r="Y39" s="64"/>
-      <c r="Z39" s="65"/>
+      <c r="B39" s="61"/>
+      <c r="C39" s="62"/>
+      <c r="D39" s="63"/>
+      <c r="E39" s="58"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="59"/>
+      <c r="H39" s="58"/>
+      <c r="I39" s="60"/>
+      <c r="J39" s="59"/>
+      <c r="K39" s="59"/>
+      <c r="L39" s="59"/>
+      <c r="M39" s="60"/>
+      <c r="O39" s="68"/>
+      <c r="P39" s="59"/>
+      <c r="Q39" s="60"/>
+      <c r="S39" s="58"/>
+      <c r="T39" s="59"/>
+      <c r="U39" s="59"/>
+      <c r="V39" s="60"/>
+      <c r="W39" s="61"/>
+      <c r="X39" s="62"/>
+      <c r="Y39" s="62"/>
+      <c r="Z39" s="63"/>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="60"/>
-      <c r="C40" s="61"/>
-      <c r="D40" s="62"/>
-      <c r="E40" s="60"/>
-      <c r="F40" s="62"/>
-      <c r="G40" s="61"/>
-      <c r="H40" s="60"/>
-      <c r="I40" s="62"/>
-      <c r="J40" s="61"/>
-      <c r="K40" s="61"/>
-      <c r="L40" s="61"/>
-      <c r="M40" s="62"/>
-      <c r="O40" s="60"/>
-      <c r="P40" s="61"/>
-      <c r="Q40" s="62"/>
-      <c r="S40" s="60"/>
-      <c r="T40" s="61"/>
-      <c r="U40" s="61"/>
-      <c r="V40" s="62"/>
-      <c r="W40" s="60"/>
-      <c r="X40" s="61"/>
-      <c r="Y40" s="61"/>
-      <c r="Z40" s="62"/>
+      <c r="B40" s="58"/>
+      <c r="C40" s="59"/>
+      <c r="D40" s="60"/>
+      <c r="E40" s="58"/>
+      <c r="F40" s="60"/>
+      <c r="G40" s="59"/>
+      <c r="H40" s="58"/>
+      <c r="I40" s="60"/>
+      <c r="J40" s="59"/>
+      <c r="K40" s="59"/>
+      <c r="L40" s="59"/>
+      <c r="M40" s="60"/>
+      <c r="O40" s="58"/>
+      <c r="P40" s="59"/>
+      <c r="Q40" s="60"/>
+      <c r="S40" s="58"/>
+      <c r="T40" s="59"/>
+      <c r="U40" s="59"/>
+      <c r="V40" s="60"/>
+      <c r="W40" s="58"/>
+      <c r="X40" s="59"/>
+      <c r="Y40" s="59"/>
+      <c r="Z40" s="60"/>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="60"/>
-      <c r="C41" s="61"/>
-      <c r="D41" s="62"/>
-      <c r="E41" s="60"/>
-      <c r="F41" s="62"/>
-      <c r="G41" s="61"/>
-      <c r="H41" s="60"/>
-      <c r="I41" s="62"/>
-      <c r="J41" s="61"/>
-      <c r="K41" s="61"/>
-      <c r="L41" s="61"/>
-      <c r="M41" s="62"/>
-      <c r="O41" s="60"/>
-      <c r="P41" s="61"/>
-      <c r="Q41" s="62"/>
-      <c r="S41" s="60"/>
-      <c r="T41" s="61"/>
-      <c r="U41" s="61"/>
-      <c r="V41" s="62"/>
-      <c r="W41" s="60"/>
-      <c r="X41" s="61"/>
-      <c r="Y41" s="61"/>
-      <c r="Z41" s="62"/>
+      <c r="B41" s="58"/>
+      <c r="C41" s="59"/>
+      <c r="D41" s="60"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="60"/>
+      <c r="G41" s="59"/>
+      <c r="H41" s="58"/>
+      <c r="I41" s="60"/>
+      <c r="J41" s="59"/>
+      <c r="K41" s="59"/>
+      <c r="L41" s="59"/>
+      <c r="M41" s="60"/>
+      <c r="O41" s="58"/>
+      <c r="P41" s="59"/>
+      <c r="Q41" s="60"/>
+      <c r="S41" s="58"/>
+      <c r="T41" s="59"/>
+      <c r="U41" s="59"/>
+      <c r="V41" s="60"/>
+      <c r="W41" s="58"/>
+      <c r="X41" s="59"/>
+      <c r="Y41" s="59"/>
+      <c r="Z41" s="60"/>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="60"/>
-      <c r="C42" s="61"/>
-      <c r="D42" s="62"/>
-      <c r="E42" s="60"/>
-      <c r="F42" s="62"/>
-      <c r="G42" s="61"/>
-      <c r="H42" s="60"/>
-      <c r="I42" s="62"/>
-      <c r="J42" s="61"/>
-      <c r="K42" s="61"/>
-      <c r="L42" s="61"/>
-      <c r="M42" s="62"/>
-      <c r="O42" s="60"/>
-      <c r="P42" s="61"/>
-      <c r="Q42" s="62"/>
-      <c r="S42" s="60"/>
-      <c r="T42" s="61"/>
-      <c r="U42" s="61"/>
-      <c r="V42" s="62"/>
-      <c r="W42" s="60"/>
-      <c r="X42" s="61"/>
-      <c r="Y42" s="61"/>
-      <c r="Z42" s="62"/>
+      <c r="B42" s="58"/>
+      <c r="C42" s="59"/>
+      <c r="D42" s="60"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="60"/>
+      <c r="G42" s="59"/>
+      <c r="H42" s="58"/>
+      <c r="I42" s="60"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="59"/>
+      <c r="M42" s="60"/>
+      <c r="O42" s="58"/>
+      <c r="P42" s="59"/>
+      <c r="Q42" s="60"/>
+      <c r="S42" s="58"/>
+      <c r="T42" s="59"/>
+      <c r="U42" s="59"/>
+      <c r="V42" s="60"/>
+      <c r="W42" s="58"/>
+      <c r="X42" s="59"/>
+      <c r="Y42" s="59"/>
+      <c r="Z42" s="60"/>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="60"/>
-      <c r="C43" s="61"/>
-      <c r="D43" s="62"/>
-      <c r="E43" s="60"/>
-      <c r="F43" s="62"/>
-      <c r="G43" s="61"/>
-      <c r="H43" s="60"/>
-      <c r="I43" s="62"/>
-      <c r="J43" s="61"/>
-      <c r="K43" s="61"/>
-      <c r="L43" s="61"/>
-      <c r="M43" s="62"/>
-      <c r="O43" s="60"/>
-      <c r="P43" s="61"/>
-      <c r="Q43" s="62"/>
-      <c r="S43" s="60"/>
-      <c r="T43" s="61"/>
-      <c r="U43" s="61"/>
-      <c r="V43" s="62"/>
-      <c r="W43" s="60"/>
-      <c r="X43" s="61"/>
-      <c r="Y43" s="61"/>
-      <c r="Z43" s="62"/>
+      <c r="B43" s="58"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="60"/>
+      <c r="E43" s="58"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="59"/>
+      <c r="H43" s="58"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="59"/>
+      <c r="K43" s="59"/>
+      <c r="L43" s="59"/>
+      <c r="M43" s="60"/>
+      <c r="O43" s="58"/>
+      <c r="P43" s="59"/>
+      <c r="Q43" s="60"/>
+      <c r="S43" s="58"/>
+      <c r="T43" s="59"/>
+      <c r="U43" s="59"/>
+      <c r="V43" s="60"/>
+      <c r="W43" s="58"/>
+      <c r="X43" s="59"/>
+      <c r="Y43" s="59"/>
+      <c r="Z43" s="60"/>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="60"/>
-      <c r="C44" s="61"/>
-      <c r="D44" s="62"/>
-      <c r="E44" s="60"/>
-      <c r="F44" s="62"/>
-      <c r="G44" s="61"/>
-      <c r="H44" s="60"/>
-      <c r="I44" s="62"/>
-      <c r="J44" s="61"/>
-      <c r="K44" s="61"/>
-      <c r="L44" s="61"/>
-      <c r="M44" s="62"/>
-      <c r="O44" s="60"/>
-      <c r="P44" s="61"/>
-      <c r="Q44" s="62"/>
-      <c r="S44" s="60"/>
-      <c r="T44" s="61"/>
-      <c r="U44" s="61"/>
-      <c r="V44" s="62"/>
-      <c r="W44" s="60"/>
-      <c r="X44" s="61"/>
-      <c r="Y44" s="61"/>
-      <c r="Z44" s="62"/>
+      <c r="B44" s="58"/>
+      <c r="C44" s="59"/>
+      <c r="D44" s="60"/>
+      <c r="E44" s="58"/>
+      <c r="F44" s="60"/>
+      <c r="G44" s="59"/>
+      <c r="H44" s="58"/>
+      <c r="I44" s="60"/>
+      <c r="J44" s="59"/>
+      <c r="K44" s="59"/>
+      <c r="L44" s="59"/>
+      <c r="M44" s="60"/>
+      <c r="O44" s="58"/>
+      <c r="P44" s="59"/>
+      <c r="Q44" s="60"/>
+      <c r="S44" s="58"/>
+      <c r="T44" s="59"/>
+      <c r="U44" s="59"/>
+      <c r="V44" s="60"/>
+      <c r="W44" s="58"/>
+      <c r="X44" s="59"/>
+      <c r="Y44" s="59"/>
+      <c r="Z44" s="60"/>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="60"/>
-      <c r="C45" s="61"/>
-      <c r="D45" s="62"/>
-      <c r="E45" s="60"/>
-      <c r="F45" s="62"/>
-      <c r="G45" s="61"/>
-      <c r="H45" s="60"/>
-      <c r="I45" s="62"/>
-      <c r="J45" s="61"/>
-      <c r="K45" s="61"/>
-      <c r="L45" s="61"/>
-      <c r="M45" s="62"/>
-      <c r="O45" s="60"/>
-      <c r="P45" s="61"/>
-      <c r="Q45" s="62"/>
-      <c r="S45" s="60"/>
-      <c r="T45" s="61"/>
-      <c r="U45" s="61"/>
-      <c r="V45" s="62"/>
-      <c r="W45" s="60"/>
-      <c r="X45" s="61"/>
-      <c r="Y45" s="61"/>
-      <c r="Z45" s="62"/>
+      <c r="B45" s="58"/>
+      <c r="C45" s="59"/>
+      <c r="D45" s="60"/>
+      <c r="E45" s="58"/>
+      <c r="F45" s="60"/>
+      <c r="G45" s="59"/>
+      <c r="H45" s="58"/>
+      <c r="I45" s="60"/>
+      <c r="J45" s="59"/>
+      <c r="K45" s="59"/>
+      <c r="L45" s="59"/>
+      <c r="M45" s="60"/>
+      <c r="O45" s="58"/>
+      <c r="P45" s="59"/>
+      <c r="Q45" s="60"/>
+      <c r="S45" s="58"/>
+      <c r="T45" s="59"/>
+      <c r="U45" s="59"/>
+      <c r="V45" s="60"/>
+      <c r="W45" s="58"/>
+      <c r="X45" s="59"/>
+      <c r="Y45" s="59"/>
+      <c r="Z45" s="60"/>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="60"/>
-      <c r="C46" s="61"/>
-      <c r="D46" s="62"/>
-      <c r="E46" s="60"/>
-      <c r="F46" s="62"/>
-      <c r="G46" s="61"/>
-      <c r="H46" s="60"/>
-      <c r="I46" s="62"/>
-      <c r="J46" s="61"/>
-      <c r="K46" s="61"/>
-      <c r="L46" s="61"/>
-      <c r="M46" s="62"/>
-      <c r="O46" s="60"/>
-      <c r="P46" s="61"/>
-      <c r="Q46" s="62"/>
-      <c r="S46" s="60"/>
-      <c r="T46" s="61"/>
-      <c r="U46" s="61"/>
-      <c r="V46" s="62"/>
-      <c r="W46" s="60"/>
-      <c r="X46" s="61"/>
-      <c r="Y46" s="61"/>
-      <c r="Z46" s="62"/>
+      <c r="B46" s="58"/>
+      <c r="C46" s="59"/>
+      <c r="D46" s="60"/>
+      <c r="E46" s="58"/>
+      <c r="F46" s="60"/>
+      <c r="G46" s="59"/>
+      <c r="H46" s="58"/>
+      <c r="I46" s="60"/>
+      <c r="J46" s="59"/>
+      <c r="K46" s="59"/>
+      <c r="L46" s="59"/>
+      <c r="M46" s="60"/>
+      <c r="O46" s="58"/>
+      <c r="P46" s="59"/>
+      <c r="Q46" s="60"/>
+      <c r="S46" s="58"/>
+      <c r="T46" s="59"/>
+      <c r="U46" s="59"/>
+      <c r="V46" s="60"/>
+      <c r="W46" s="58"/>
+      <c r="X46" s="59"/>
+      <c r="Y46" s="59"/>
+      <c r="Z46" s="60"/>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="66"/>
-      <c r="C47" s="67"/>
-      <c r="D47" s="68"/>
-      <c r="E47" s="66"/>
-      <c r="F47" s="68"/>
-      <c r="G47" s="67"/>
-      <c r="H47" s="66"/>
-      <c r="I47" s="68"/>
-      <c r="J47" s="67"/>
-      <c r="K47" s="67"/>
-      <c r="L47" s="67"/>
-      <c r="M47" s="68"/>
-      <c r="O47" s="66"/>
-      <c r="P47" s="67"/>
-      <c r="Q47" s="68"/>
-      <c r="S47" s="66"/>
-      <c r="T47" s="67"/>
-      <c r="U47" s="67"/>
-      <c r="V47" s="68"/>
-      <c r="W47" s="66"/>
-      <c r="X47" s="67"/>
-      <c r="Y47" s="67"/>
-      <c r="Z47" s="68"/>
+      <c r="B47" s="64"/>
+      <c r="C47" s="65"/>
+      <c r="D47" s="66"/>
+      <c r="E47" s="64"/>
+      <c r="F47" s="66"/>
+      <c r="G47" s="65"/>
+      <c r="H47" s="64"/>
+      <c r="I47" s="66"/>
+      <c r="J47" s="65"/>
+      <c r="K47" s="65"/>
+      <c r="L47" s="65"/>
+      <c r="M47" s="66"/>
+      <c r="O47" s="64"/>
+      <c r="P47" s="65"/>
+      <c r="Q47" s="66"/>
+      <c r="S47" s="64"/>
+      <c r="T47" s="65"/>
+      <c r="U47" s="65"/>
+      <c r="V47" s="66"/>
+      <c r="W47" s="64"/>
+      <c r="X47" s="65"/>
+      <c r="Y47" s="65"/>
+      <c r="Z47" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="22">
@@ -4692,37 +4677,37 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.0546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="59" width="3.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="59" width="17.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="59" width="27.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="59" width="6.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="59" width="18.66"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="16" min="16" style="59" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="17" style="62" width="0.28"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="59" width="1.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="57" width="3.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="57" width="17.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="57" width="27.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="57" width="6.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="57" width="18.66"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="16" min="16" style="57" width="19.99"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="17" min="17" style="60" width="0.28"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="57" width="1.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="43.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="71" t="s">
+      <c r="A1" s="69" t="s">
         <v>114</v>
       </c>
-      <c r="B1" s="71"/>
-      <c r="C1" s="71"/>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="71"/>
-      <c r="H1" s="71"/>
-      <c r="I1" s="71"/>
-      <c r="J1" s="71"/>
-      <c r="K1" s="71"/>
-      <c r="L1" s="71"/>
-      <c r="M1" s="71"/>
-      <c r="N1" s="71"/>
-      <c r="O1" s="71"/>
-      <c r="P1" s="71"/>
-      <c r="Q1" s="71"/>
-      <c r="R1" s="71"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
@@ -4740,73 +4725,73 @@
       <c r="K2" s="11"/>
       <c r="L2" s="11"/>
       <c r="M2" s="11"/>
-      <c r="N2" s="72"/>
-      <c r="O2" s="73"/>
-      <c r="P2" s="72"/>
-      <c r="Q2" s="73"/>
-      <c r="R2" s="65"/>
+      <c r="N2" s="70"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="71"/>
+      <c r="R2" s="63"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="72" t="s">
         <v>115</v>
       </c>
-      <c r="B3" s="74"/>
-      <c r="C3" s="75" t="s">
+      <c r="B3" s="72"/>
+      <c r="C3" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="74" t="s">
         <v>117</v>
       </c>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="75" t="s">
+      <c r="E3" s="74"/>
+      <c r="F3" s="74"/>
+      <c r="G3" s="73" t="s">
         <v>116</v>
       </c>
-      <c r="H3" s="75"/>
-      <c r="I3" s="77" t="s">
+      <c r="H3" s="73"/>
+      <c r="I3" s="75" t="s">
         <v>118</v>
       </c>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="77"/>
-      <c r="N3" s="77"/>
-      <c r="O3" s="77"/>
+      <c r="J3" s="75"/>
+      <c r="K3" s="75"/>
+      <c r="L3" s="75"/>
+      <c r="M3" s="75"/>
+      <c r="N3" s="75"/>
+      <c r="O3" s="75"/>
       <c r="P3" s="17"/>
-      <c r="Q3" s="77"/>
-      <c r="R3" s="62"/>
+      <c r="Q3" s="75"/>
+      <c r="R3" s="60"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="78" t="s">
+      <c r="A4" s="76" t="s">
         <v>119</v>
       </c>
-      <c r="B4" s="79" t="s">
+      <c r="B4" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="80" t="s">
+      <c r="C4" s="78" t="s">
         <v>120</v>
       </c>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="78"/>
+      <c r="F4" s="78"/>
+      <c r="G4" s="78"/>
+      <c r="H4" s="78"/>
       <c r="J4" s="17"/>
       <c r="K4" s="17"/>
       <c r="L4" s="17"/>
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
-      <c r="O4" s="77"/>
+      <c r="O4" s="75"/>
       <c r="P4" s="17"/>
-      <c r="Q4" s="77"/>
-      <c r="R4" s="62"/>
-      <c r="S4" s="61"/>
+      <c r="Q4" s="75"/>
+      <c r="R4" s="60"/>
+      <c r="S4" s="59"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="81"/>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
+      <c r="A5" s="79"/>
+      <c r="B5" s="80"/>
+      <c r="C5" s="80"/>
+      <c r="D5" s="80"/>
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
       <c r="G5" s="17"/>
@@ -4817,16 +4802,16 @@
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
       <c r="N5" s="17"/>
-      <c r="O5" s="77"/>
+      <c r="O5" s="75"/>
       <c r="P5" s="17"/>
-      <c r="Q5" s="77"/>
-      <c r="R5" s="62"/>
+      <c r="Q5" s="75"/>
+      <c r="R5" s="60"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="81"/>
-      <c r="B6" s="82"/>
-      <c r="C6" s="82"/>
-      <c r="D6" s="82"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="80"/>
+      <c r="C6" s="80"/>
+      <c r="D6" s="80"/>
       <c r="E6" s="17"/>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -4837,19 +4822,19 @@
       <c r="L6" s="17"/>
       <c r="M6" s="17"/>
       <c r="N6" s="17"/>
-      <c r="O6" s="77"/>
+      <c r="O6" s="75"/>
       <c r="P6" s="17"/>
-      <c r="Q6" s="77"/>
-      <c r="R6" s="62"/>
+      <c r="Q6" s="75"/>
+      <c r="R6" s="60"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="81"/>
+      <c r="A7" s="79"/>
       <c r="B7" s="17"/>
       <c r="C7" s="17"/>
       <c r="D7" s="17"/>
       <c r="E7" s="17"/>
       <c r="F7" s="17"/>
-      <c r="G7" s="48"/>
+      <c r="G7" s="47"/>
       <c r="H7" s="17"/>
       <c r="I7" s="17"/>
       <c r="J7" s="17"/>
@@ -4857,13 +4842,13 @@
       <c r="L7" s="17"/>
       <c r="M7" s="17"/>
       <c r="N7" s="17"/>
-      <c r="O7" s="77"/>
+      <c r="O7" s="75"/>
       <c r="P7" s="17"/>
-      <c r="Q7" s="77"/>
-      <c r="R7" s="62"/>
+      <c r="Q7" s="75"/>
+      <c r="R7" s="60"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="81"/>
+      <c r="A8" s="79"/>
       <c r="B8" s="17"/>
       <c r="C8" s="17"/>
       <c r="D8" s="17"/>
@@ -4877,13 +4862,13 @@
       <c r="L8" s="17"/>
       <c r="M8" s="17"/>
       <c r="N8" s="17"/>
-      <c r="O8" s="77"/>
+      <c r="O8" s="75"/>
       <c r="P8" s="17"/>
-      <c r="Q8" s="77"/>
-      <c r="R8" s="62"/>
+      <c r="Q8" s="75"/>
+      <c r="R8" s="60"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="81"/>
+      <c r="A9" s="79"/>
       <c r="B9" s="17"/>
       <c r="C9" s="17"/>
       <c r="D9" s="17"/>
@@ -4897,13 +4882,13 @@
       <c r="L9" s="17"/>
       <c r="M9" s="17"/>
       <c r="N9" s="17"/>
-      <c r="O9" s="77"/>
+      <c r="O9" s="75"/>
       <c r="P9" s="17"/>
-      <c r="Q9" s="77"/>
-      <c r="R9" s="62"/>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="60"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="81"/>
+      <c r="A10" s="79"/>
       <c r="B10" s="17"/>
       <c r="C10" s="17"/>
       <c r="D10" s="17"/>
@@ -4917,13 +4902,13 @@
       <c r="L10" s="17"/>
       <c r="M10" s="17"/>
       <c r="N10" s="17"/>
-      <c r="O10" s="77"/>
+      <c r="O10" s="75"/>
       <c r="P10" s="17"/>
-      <c r="Q10" s="77"/>
-      <c r="R10" s="62"/>
+      <c r="Q10" s="75"/>
+      <c r="R10" s="60"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="81"/>
+      <c r="A11" s="79"/>
       <c r="B11" s="17"/>
       <c r="C11" s="17"/>
       <c r="D11" s="17"/>
@@ -4937,13 +4922,13 @@
       <c r="L11" s="17"/>
       <c r="M11" s="17"/>
       <c r="N11" s="17"/>
-      <c r="O11" s="77"/>
+      <c r="O11" s="75"/>
       <c r="P11" s="17"/>
-      <c r="Q11" s="77"/>
-      <c r="R11" s="62"/>
+      <c r="Q11" s="75"/>
+      <c r="R11" s="60"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="81"/>
+      <c r="A12" s="79"/>
       <c r="B12" s="17"/>
       <c r="C12" s="17"/>
       <c r="D12" s="17"/>
@@ -4957,13 +4942,13 @@
       <c r="L12" s="17"/>
       <c r="M12" s="17"/>
       <c r="N12" s="17"/>
-      <c r="O12" s="77"/>
+      <c r="O12" s="75"/>
       <c r="P12" s="17"/>
-      <c r="Q12" s="77"/>
-      <c r="R12" s="62"/>
+      <c r="Q12" s="75"/>
+      <c r="R12" s="60"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="81"/>
+      <c r="A13" s="79"/>
       <c r="B13" s="17"/>
       <c r="C13" s="17"/>
       <c r="D13" s="17"/>
@@ -4977,13 +4962,13 @@
       <c r="L13" s="17"/>
       <c r="M13" s="17"/>
       <c r="N13" s="17"/>
-      <c r="O13" s="77"/>
+      <c r="O13" s="75"/>
       <c r="P13" s="17"/>
-      <c r="Q13" s="77"/>
-      <c r="R13" s="62"/>
+      <c r="Q13" s="75"/>
+      <c r="R13" s="60"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="81"/>
+      <c r="A14" s="79"/>
       <c r="B14" s="17"/>
       <c r="C14" s="17"/>
       <c r="D14" s="17"/>
@@ -4997,13 +4982,13 @@
       <c r="L14" s="17"/>
       <c r="M14" s="17"/>
       <c r="N14" s="17"/>
-      <c r="O14" s="77"/>
+      <c r="O14" s="75"/>
       <c r="P14" s="17"/>
-      <c r="Q14" s="77"/>
-      <c r="R14" s="62"/>
+      <c r="Q14" s="75"/>
+      <c r="R14" s="60"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="81"/>
+      <c r="A15" s="79"/>
       <c r="B15" s="17"/>
       <c r="C15" s="17"/>
       <c r="D15" s="17"/>
@@ -5017,13 +5002,13 @@
       <c r="L15" s="17"/>
       <c r="M15" s="17"/>
       <c r="N15" s="17"/>
-      <c r="O15" s="77"/>
+      <c r="O15" s="75"/>
       <c r="P15" s="17"/>
-      <c r="Q15" s="77"/>
-      <c r="R15" s="62"/>
+      <c r="Q15" s="75"/>
+      <c r="R15" s="60"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="81"/>
+      <c r="A16" s="79"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
       <c r="D16" s="17"/>
@@ -5037,13 +5022,13 @@
       <c r="L16" s="17"/>
       <c r="M16" s="17"/>
       <c r="N16" s="17"/>
-      <c r="O16" s="77"/>
+      <c r="O16" s="75"/>
       <c r="P16" s="17"/>
-      <c r="Q16" s="77"/>
-      <c r="R16" s="62"/>
+      <c r="Q16" s="75"/>
+      <c r="R16" s="60"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="81"/>
+      <c r="A17" s="79"/>
       <c r="B17" s="17"/>
       <c r="C17" s="17"/>
       <c r="D17" s="17"/>
@@ -5057,13 +5042,13 @@
       <c r="L17" s="17"/>
       <c r="M17" s="17"/>
       <c r="N17" s="17"/>
-      <c r="O17" s="77"/>
+      <c r="O17" s="75"/>
       <c r="P17" s="17"/>
-      <c r="Q17" s="77"/>
-      <c r="R17" s="62"/>
+      <c r="Q17" s="75"/>
+      <c r="R17" s="60"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="81"/>
+      <c r="A18" s="79"/>
       <c r="B18" s="17"/>
       <c r="C18" s="17"/>
       <c r="D18" s="17"/>
@@ -5077,13 +5062,13 @@
       <c r="L18" s="17"/>
       <c r="M18" s="17"/>
       <c r="N18" s="17"/>
-      <c r="O18" s="77"/>
+      <c r="O18" s="75"/>
       <c r="P18" s="17"/>
-      <c r="Q18" s="77"/>
-      <c r="R18" s="62"/>
+      <c r="Q18" s="75"/>
+      <c r="R18" s="60"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="81"/>
+      <c r="A19" s="79"/>
       <c r="B19" s="17"/>
       <c r="C19" s="17"/>
       <c r="D19" s="17"/>
@@ -5097,13 +5082,13 @@
       <c r="L19" s="17"/>
       <c r="M19" s="17"/>
       <c r="N19" s="17"/>
-      <c r="O19" s="77"/>
+      <c r="O19" s="75"/>
       <c r="P19" s="17"/>
-      <c r="Q19" s="77"/>
-      <c r="R19" s="62"/>
+      <c r="Q19" s="75"/>
+      <c r="R19" s="60"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="81"/>
+      <c r="A20" s="79"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
       <c r="D20" s="17"/>
@@ -5117,13 +5102,13 @@
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
       <c r="N20" s="17"/>
-      <c r="O20" s="77"/>
+      <c r="O20" s="75"/>
       <c r="P20" s="17"/>
-      <c r="Q20" s="77"/>
-      <c r="R20" s="62"/>
+      <c r="Q20" s="75"/>
+      <c r="R20" s="60"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="81"/>
+      <c r="A21" s="79"/>
       <c r="B21" s="17"/>
       <c r="C21" s="17"/>
       <c r="D21" s="17"/>
@@ -5137,13 +5122,13 @@
       <c r="L21" s="17"/>
       <c r="M21" s="17"/>
       <c r="N21" s="17"/>
-      <c r="O21" s="77"/>
+      <c r="O21" s="75"/>
       <c r="P21" s="17"/>
-      <c r="Q21" s="77"/>
-      <c r="R21" s="62"/>
+      <c r="Q21" s="75"/>
+      <c r="R21" s="60"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="81"/>
+      <c r="A22" s="79"/>
       <c r="B22" s="17"/>
       <c r="C22" s="17"/>
       <c r="D22" s="17"/>
@@ -5157,13 +5142,13 @@
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
       <c r="N22" s="17"/>
-      <c r="O22" s="77"/>
+      <c r="O22" s="75"/>
       <c r="P22" s="17"/>
-      <c r="Q22" s="77"/>
-      <c r="R22" s="62"/>
+      <c r="Q22" s="75"/>
+      <c r="R22" s="60"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="81"/>
+      <c r="A23" s="79"/>
       <c r="B23" s="17"/>
       <c r="C23" s="17"/>
       <c r="D23" s="17"/>
@@ -5177,13 +5162,13 @@
       <c r="L23" s="17"/>
       <c r="M23" s="17"/>
       <c r="N23" s="17"/>
-      <c r="O23" s="77"/>
+      <c r="O23" s="75"/>
       <c r="P23" s="17"/>
-      <c r="Q23" s="77"/>
-      <c r="R23" s="62"/>
+      <c r="Q23" s="75"/>
+      <c r="R23" s="60"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="81"/>
+      <c r="A24" s="79"/>
       <c r="B24" s="17"/>
       <c r="C24" s="17"/>
       <c r="D24" s="17"/>
@@ -5197,13 +5182,13 @@
       <c r="L24" s="17"/>
       <c r="M24" s="17"/>
       <c r="N24" s="17"/>
-      <c r="O24" s="77"/>
+      <c r="O24" s="75"/>
       <c r="P24" s="17"/>
-      <c r="Q24" s="77"/>
-      <c r="R24" s="62"/>
+      <c r="Q24" s="75"/>
+      <c r="R24" s="60"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="81"/>
+      <c r="A25" s="79"/>
       <c r="B25" s="17"/>
       <c r="C25" s="17"/>
       <c r="D25" s="17"/>
@@ -5217,13 +5202,13 @@
       <c r="L25" s="17"/>
       <c r="M25" s="17"/>
       <c r="N25" s="17"/>
-      <c r="O25" s="77"/>
+      <c r="O25" s="75"/>
       <c r="P25" s="17"/>
-      <c r="Q25" s="77"/>
-      <c r="R25" s="62"/>
+      <c r="Q25" s="75"/>
+      <c r="R25" s="60"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="81"/>
+      <c r="A26" s="79"/>
       <c r="B26" s="17"/>
       <c r="C26" s="17"/>
       <c r="D26" s="17"/>
@@ -5237,13 +5222,13 @@
       <c r="L26" s="17"/>
       <c r="M26" s="17"/>
       <c r="N26" s="17"/>
-      <c r="O26" s="77"/>
+      <c r="O26" s="75"/>
       <c r="P26" s="17"/>
-      <c r="Q26" s="77"/>
-      <c r="R26" s="62"/>
+      <c r="Q26" s="75"/>
+      <c r="R26" s="60"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="81"/>
+      <c r="A27" s="79"/>
       <c r="B27" s="17"/>
       <c r="C27" s="17"/>
       <c r="D27" s="17"/>
@@ -5257,13 +5242,13 @@
       <c r="L27" s="17"/>
       <c r="M27" s="17"/>
       <c r="N27" s="17"/>
-      <c r="O27" s="77"/>
+      <c r="O27" s="75"/>
       <c r="P27" s="17"/>
-      <c r="Q27" s="77"/>
-      <c r="R27" s="62"/>
+      <c r="Q27" s="75"/>
+      <c r="R27" s="60"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="81"/>
+      <c r="A28" s="79"/>
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
       <c r="D28" s="17"/>
@@ -5277,13 +5262,13 @@
       <c r="L28" s="17"/>
       <c r="M28" s="17"/>
       <c r="N28" s="17"/>
-      <c r="O28" s="77"/>
+      <c r="O28" s="75"/>
       <c r="P28" s="17"/>
-      <c r="Q28" s="77"/>
-      <c r="R28" s="62"/>
+      <c r="Q28" s="75"/>
+      <c r="R28" s="60"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="81"/>
+      <c r="A29" s="79"/>
       <c r="B29" s="17"/>
       <c r="C29" s="17"/>
       <c r="D29" s="17"/>
@@ -5297,13 +5282,13 @@
       <c r="L29" s="17"/>
       <c r="M29" s="17"/>
       <c r="N29" s="17"/>
-      <c r="O29" s="77"/>
+      <c r="O29" s="75"/>
       <c r="P29" s="17"/>
-      <c r="Q29" s="77"/>
-      <c r="R29" s="62"/>
+      <c r="Q29" s="75"/>
+      <c r="R29" s="60"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="81"/>
+      <c r="A30" s="79"/>
       <c r="B30" s="17"/>
       <c r="C30" s="17"/>
       <c r="D30" s="17"/>
@@ -5317,13 +5302,13 @@
       <c r="L30" s="17"/>
       <c r="M30" s="17"/>
       <c r="N30" s="17"/>
-      <c r="O30" s="77"/>
+      <c r="O30" s="75"/>
       <c r="P30" s="17"/>
-      <c r="Q30" s="77"/>
-      <c r="R30" s="62"/>
+      <c r="Q30" s="75"/>
+      <c r="R30" s="60"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="81"/>
+      <c r="A31" s="79"/>
       <c r="B31" s="17"/>
       <c r="C31" s="17"/>
       <c r="D31" s="17"/>
@@ -5337,68 +5322,68 @@
       <c r="L31" s="17"/>
       <c r="M31" s="17"/>
       <c r="N31" s="17"/>
-      <c r="O31" s="77"/>
+      <c r="O31" s="75"/>
       <c r="P31" s="17"/>
-      <c r="Q31" s="77"/>
-      <c r="R31" s="62"/>
+      <c r="Q31" s="75"/>
+      <c r="R31" s="60"/>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="60"/>
-      <c r="B32" s="61"/>
-      <c r="C32" s="61"/>
-      <c r="D32" s="61"/>
-      <c r="E32" s="61"/>
-      <c r="F32" s="61"/>
-      <c r="G32" s="61"/>
-      <c r="H32" s="61"/>
-      <c r="I32" s="61"/>
-      <c r="J32" s="61"/>
-      <c r="K32" s="61"/>
-      <c r="L32" s="61"/>
-      <c r="M32" s="61"/>
-      <c r="N32" s="61"/>
-      <c r="O32" s="62"/>
-      <c r="P32" s="61"/>
-      <c r="R32" s="62"/>
+      <c r="A32" s="58"/>
+      <c r="B32" s="59"/>
+      <c r="C32" s="59"/>
+      <c r="D32" s="59"/>
+      <c r="E32" s="59"/>
+      <c r="F32" s="59"/>
+      <c r="G32" s="59"/>
+      <c r="H32" s="59"/>
+      <c r="I32" s="59"/>
+      <c r="J32" s="59"/>
+      <c r="K32" s="59"/>
+      <c r="L32" s="59"/>
+      <c r="M32" s="59"/>
+      <c r="N32" s="59"/>
+      <c r="O32" s="60"/>
+      <c r="P32" s="59"/>
+      <c r="R32" s="60"/>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="60"/>
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
-      <c r="D33" s="61"/>
-      <c r="E33" s="61"/>
-      <c r="F33" s="61"/>
-      <c r="G33" s="61"/>
-      <c r="H33" s="61"/>
-      <c r="I33" s="61"/>
-      <c r="J33" s="61"/>
-      <c r="K33" s="61"/>
-      <c r="L33" s="61"/>
-      <c r="M33" s="61"/>
-      <c r="N33" s="61"/>
-      <c r="O33" s="62"/>
-      <c r="P33" s="61"/>
-      <c r="R33" s="62"/>
+      <c r="A33" s="58"/>
+      <c r="B33" s="59"/>
+      <c r="C33" s="59"/>
+      <c r="D33" s="59"/>
+      <c r="E33" s="59"/>
+      <c r="F33" s="59"/>
+      <c r="G33" s="59"/>
+      <c r="H33" s="59"/>
+      <c r="I33" s="59"/>
+      <c r="J33" s="59"/>
+      <c r="K33" s="59"/>
+      <c r="L33" s="59"/>
+      <c r="M33" s="59"/>
+      <c r="N33" s="59"/>
+      <c r="O33" s="60"/>
+      <c r="P33" s="59"/>
+      <c r="R33" s="60"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="66"/>
-      <c r="B34" s="67"/>
-      <c r="C34" s="67"/>
-      <c r="D34" s="67"/>
-      <c r="E34" s="67"/>
-      <c r="F34" s="67"/>
-      <c r="G34" s="67"/>
-      <c r="H34" s="67"/>
-      <c r="I34" s="67"/>
-      <c r="J34" s="67"/>
-      <c r="K34" s="67"/>
-      <c r="L34" s="67"/>
-      <c r="M34" s="67"/>
-      <c r="N34" s="67"/>
-      <c r="O34" s="68"/>
-      <c r="P34" s="67"/>
-      <c r="Q34" s="68"/>
-      <c r="R34" s="68"/>
+      <c r="A34" s="64"/>
+      <c r="B34" s="65"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="65"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
+      <c r="H34" s="65"/>
+      <c r="I34" s="65"/>
+      <c r="J34" s="65"/>
+      <c r="K34" s="65"/>
+      <c r="L34" s="65"/>
+      <c r="M34" s="65"/>
+      <c r="N34" s="65"/>
+      <c r="O34" s="66"/>
+      <c r="P34" s="65"/>
+      <c r="Q34" s="66"/>
+      <c r="R34" s="66"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>